<commit_message>
Note that we are allocating Mortality Per Recruit, fixed spreadsheet Mitigation
</commit_message>
<xml_diff>
--- a/src/dashboard/data/harvestPolicy/SPRbasedPSC.xlsx
+++ b/src/dashboard/data/harvestPolicy/SPRbasedPSC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2480" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Proof of Concept" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Proof of Concept'!$C$55</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Proof of Concept'!$C$15</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>SPR Based PSC Caps</t>
   </si>
@@ -405,9 +405,6 @@
     <t>ypr_3</t>
   </si>
   <si>
-    <t>PSC limit</t>
-  </si>
-  <si>
     <t>len</t>
   </si>
   <si>
@@ -436,6 +433,24 @@
   </si>
   <si>
     <t>Available yield at age</t>
+  </si>
+  <si>
+    <t>ypr1</t>
+  </si>
+  <si>
+    <t>ypr2</t>
+  </si>
+  <si>
+    <t>ypr3</t>
+  </si>
+  <si>
+    <t>mpr1</t>
+  </si>
+  <si>
+    <t>mpr2</t>
+  </si>
+  <si>
+    <t>mpr3</t>
   </si>
 </sst>
 </file>
@@ -644,7 +659,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -697,6 +712,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
@@ -1037,9 +1054,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="10" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K35" sqref="K35"/>
+      <selection pane="topRight" activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1166,10 +1183,10 @@
       </c>
       <c r="C4" s="22">
         <f>$C44</f>
-        <v>0.37525792595872431</v>
+        <v>0.4232805123398507</v>
       </c>
       <c r="J4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" ref="K4:AI4" si="0">linf*(1-EXP(-vonbk*age))</f>
@@ -1281,7 +1298,7 @@
       </c>
       <c r="C5" s="22">
         <f>$C45</f>
-        <v>0.24948414051706141</v>
+        <v>0.15342619826674431</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -1397,7 +1414,7 @@
       </c>
       <c r="C6" s="22">
         <f>$C46</f>
-        <v>0.37525793352421427</v>
+        <v>0.42329328939340488</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
@@ -1512,7 +1529,7 @@
       </c>
       <c r="C7" s="23">
         <f>spr</f>
-        <v>0.39999855522103445</v>
+        <v>0.40000071794109937</v>
       </c>
       <c r="J7" t="s">
         <v>7</v>
@@ -1523,99 +1540,99 @@
       </c>
       <c r="L7" s="1">
         <f>K7*EXP(-K8)</f>
-        <v>0.85900827925841472</v>
+        <v>0.85966080121150346</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" ref="M7:AH7" si="3">L7*EXP(-L8)</f>
-        <v>0.72936528936255107</v>
+        <v>0.73373796646230416</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="3"/>
-        <v>0.59437660857517127</v>
+        <v>0.61051999589550976</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="3"/>
-        <v>0.4791557486424079</v>
+        <v>0.50348795423534487</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="3"/>
-        <v>0.38436277876920294</v>
+        <v>0.40828209710437069</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="3"/>
-        <v>0.30505155612601553</v>
+        <v>0.32440462206133175</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" si="3"/>
-        <v>0.24338143204333321</v>
+        <v>0.25801224289839353</v>
       </c>
       <c r="S7" s="1">
         <f t="shared" si="3"/>
-        <v>0.19523019947119899</v>
+        <v>0.20584950412059194</v>
       </c>
       <c r="T7" s="1">
         <f t="shared" si="3"/>
-        <v>0.15715041457524606</v>
+        <v>0.16458138440261749</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" si="3"/>
-        <v>0.12676713971690712</v>
+        <v>0.13175857293223367</v>
       </c>
       <c r="V7" s="1">
         <f t="shared" si="3"/>
-        <v>0.10239017874408822</v>
+        <v>0.10556552184956695</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" si="3"/>
-        <v>8.2765654137124944E-2</v>
+        <v>8.4620376192300603E-2</v>
       </c>
       <c r="X7" s="1">
         <f t="shared" si="3"/>
-        <v>6.6934286147931288E-2</v>
+        <v>6.7850844998950235E-2</v>
       </c>
       <c r="Y7" s="1">
         <f t="shared" si="3"/>
-        <v>5.4146789719211719E-2</v>
+        <v>5.4414316299530335E-2</v>
       </c>
       <c r="Z7" s="1">
         <f t="shared" si="3"/>
-        <v>4.3809997570385346E-2</v>
+        <v>4.3643388773698728E-2</v>
       </c>
       <c r="AA7" s="1">
         <f t="shared" si="3"/>
-        <v>3.5450337216877535E-2</v>
+        <v>3.500683005781937E-2</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" si="3"/>
-        <v>2.868772143813518E-2</v>
+        <v>2.8080511736160489E-2</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" si="3"/>
-        <v>2.3216102618967307E-2</v>
+        <v>2.2525187452363739E-2</v>
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="3"/>
-        <v>1.8788560049267523E-2</v>
+        <v>1.8069198197903036E-2</v>
       </c>
       <c r="AE7" s="1">
         <f t="shared" si="3"/>
-        <v>1.5205635217165262E-2</v>
+        <v>1.4494857147528328E-2</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="3"/>
-        <v>1.2306089767026372E-2</v>
+        <v>1.1627653523262319E-2</v>
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="3"/>
-        <v>9.9595231708173929E-3</v>
+        <v>9.3276533315331308E-3</v>
       </c>
       <c r="AH7" s="1">
         <f t="shared" si="3"/>
-        <v>8.0604459486215609E-3</v>
+        <v>7.48263100878998E-3</v>
       </c>
       <c r="AI7" s="1">
         <f>AH7*EXP(-AH8)/(1-EXP(-AI8))</f>
-        <v>3.4212785794285813E-2</v>
+        <v>3.0347148419000908E-2</v>
       </c>
     </row>
     <row r="8" spans="1:35">
@@ -1625,110 +1642,110 @@
       </c>
       <c r="C8" s="26">
         <f>SUMXMY2(B4:B7,C4:C7)</f>
-        <v>1.0545192280660786E-2</v>
+        <v>4.8548066821489308E-2</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" ref="K8:AI8" si="4">M+f1_*flt1_ +f2_*flt2_ +f3_*flt3_</f>
-        <v>0.15197671879239133</v>
+        <v>0.15121738473343066</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="4"/>
-        <v>0.16360387087929923</v>
+        <v>0.15838592329225679</v>
       </c>
       <c r="M8" s="1">
         <f t="shared" si="4"/>
-        <v>0.20466154968398695</v>
+        <v>0.18384092463247001</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21548744132458728</v>
+        <v>0.19275125851243177</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" si="4"/>
-        <v>0.22043885531855648</v>
+        <v>0.20960143785275456</v>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="4"/>
-        <v>0.2311060441822208</v>
+        <v>0.22996677978780555</v>
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="4"/>
-        <v>0.22585090692859816</v>
+        <v>0.22898453328068435</v>
       </c>
       <c r="R8" s="1">
         <f t="shared" si="4"/>
-        <v>0.22045051945419322</v>
+        <v>0.22586169761296321</v>
       </c>
       <c r="S8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21697597109200883</v>
+        <v>0.22374015340458009</v>
       </c>
       <c r="T8" s="1">
         <f t="shared" si="4"/>
-        <v>0.2148515434060404</v>
+        <v>0.22243393087385593</v>
       </c>
       <c r="U8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21356106061683644</v>
+        <v>0.22163943467537744</v>
       </c>
       <c r="V8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21277762707482792</v>
+        <v>0.22115672937497102</v>
       </c>
       <c r="W8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21230183590258897</v>
+        <v>0.22086325081817856</v>
       </c>
       <c r="X8" s="1">
         <f t="shared" si="4"/>
-        <v>0.2120126476001975</v>
+        <v>0.22068455362013389</v>
       </c>
       <c r="Y8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21183664035799113</v>
+        <v>0.22057547563402019</v>
       </c>
       <c r="Z8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21172928097010918</v>
+        <v>0.22050862391589743</v>
       </c>
       <c r="AA8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21166355863034145</v>
+        <v>0.22046738374653468</v>
       </c>
       <c r="AB8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21162309045235206</v>
+        <v>0.22044167778448334</v>
       </c>
       <c r="AC8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21159793971293653</v>
+        <v>0.22042539381278933</v>
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21158207948478536</v>
+        <v>0.22041482458443815</v>
       </c>
       <c r="AE8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21157185425169875</v>
+        <v>0.22040772154044935</v>
       </c>
       <c r="AF8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21156504683102398</v>
+        <v>0.22040272086086043</v>
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21156031243350348</v>
+        <v>0.22039899534704935</v>
       </c>
       <c r="AH8" s="1">
         <f t="shared" si="4"/>
-        <v>0.2115568354032214</v>
+        <v>0.22039604327768969</v>
       </c>
       <c r="AI8" s="1">
         <f t="shared" si="4"/>
-        <v>0.21155412101985654</v>
+        <v>0.22039356034341401</v>
       </c>
     </row>
     <row r="9" spans="1:35">
@@ -1831,103 +1848,103 @@
       </c>
       <c r="K10" s="1">
         <f t="shared" ref="K10:AI10" si="5">EXP(-za)</f>
-        <v>0.85900827925841472</v>
+        <v>0.85966080121150346</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="5"/>
-        <v>0.84907829991139905</v>
+        <v>0.8535203250261747</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" si="5"/>
-        <v>0.81492308071671893</v>
+        <v>0.83206815484704133</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80614839435056385</v>
+        <v>0.82468708252025313</v>
       </c>
       <c r="O10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80216668558859638</v>
+        <v>0.81090737855771577</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="5"/>
-        <v>0.79365529904545939</v>
+        <v>0.79455999751662632</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="5"/>
-        <v>0.79783704477414086</v>
+        <v>0.79534083472341488</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80215732906214032</v>
+        <v>0.79782843561286532</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80494931112555368</v>
+        <v>0.79952286067301614</v>
       </c>
       <c r="T10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80666118546069143</v>
+        <v>0.80056789782440418</v>
       </c>
       <c r="U10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80770283981119351</v>
+        <v>0.8012041987116969</v>
       </c>
       <c r="V10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80833586924374468</v>
+        <v>0.8015910375821983</v>
       </c>
       <c r="W10" s="1">
         <f t="shared" si="5"/>
-        <v>0.8087205598234688</v>
+        <v>0.80182632188680603</v>
       </c>
       <c r="X10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80895446616913258</v>
+        <v>0.80196961880684337</v>
       </c>
       <c r="Y10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80909686054464658</v>
+        <v>0.80205710080888082</v>
       </c>
       <c r="Z10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80918372935133942</v>
+        <v>0.80211072149639995</v>
       </c>
       <c r="AA10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80923691254697727</v>
+        <v>0.80214380136050711</v>
       </c>
       <c r="AB10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80926966155303159</v>
+        <v>0.80216442150365375</v>
       </c>
       <c r="AC10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80929001553936408</v>
+        <v>0.80217748403274214</v>
       </c>
       <c r="AD10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80930285116543865</v>
+        <v>0.8021859624745542</v>
       </c>
       <c r="AE10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80931112651803816</v>
+        <v>0.80219166045696932</v>
       </c>
       <c r="AF10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80931663585808533</v>
+        <v>0.80219567197046238</v>
       </c>
       <c r="AG10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80932046749382969</v>
+        <v>0.80219866056708444</v>
       </c>
       <c r="AH10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80932328153049526</v>
+        <v>0.80220102871666621</v>
       </c>
       <c r="AI10" s="1">
         <f t="shared" si="5"/>
-        <v>0.80932547834712898</v>
+        <v>0.80220302053156911</v>
       </c>
     </row>
     <row r="11" spans="1:35">
@@ -1939,110 +1956,110 @@
       </c>
       <c r="C11" s="18">
         <f>$C34</f>
-        <v>0.25841295705322731</v>
+        <v>0.33333013650151561</v>
       </c>
       <c r="J11" t="s">
         <v>56</v>
       </c>
       <c r="K11" s="1">
         <f>1-sa</f>
-        <v>0.14099172074158528</v>
+        <v>0.14033919878849654</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" ref="L11:AI11" si="6">1-sa</f>
-        <v>0.15092170008860095</v>
+        <v>0.1464796749738253</v>
       </c>
       <c r="M11" s="1">
         <f t="shared" si="6"/>
-        <v>0.18507691928328107</v>
+        <v>0.16793184515295867</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19385160564943615</v>
+        <v>0.17531291747974687</v>
       </c>
       <c r="O11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19783331441140362</v>
+        <v>0.18909262144228423</v>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="6"/>
-        <v>0.20634470095454061</v>
+        <v>0.20544000248337368</v>
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="6"/>
-        <v>0.20216295522585914</v>
+        <v>0.20465916527658512</v>
       </c>
       <c r="R11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19784267093785968</v>
+        <v>0.20217156438713468</v>
       </c>
       <c r="S11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19505068887444632</v>
+        <v>0.20047713932698386</v>
       </c>
       <c r="T11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19333881453930857</v>
+        <v>0.19943210217559582</v>
       </c>
       <c r="U11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19229716018880649</v>
+        <v>0.1987958012883031</v>
       </c>
       <c r="V11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19166413075625532</v>
+        <v>0.1984089624178017</v>
       </c>
       <c r="W11" s="1">
         <f t="shared" si="6"/>
-        <v>0.1912794401765312</v>
+        <v>0.19817367811319397</v>
       </c>
       <c r="X11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19104553383086742</v>
+        <v>0.19803038119315663</v>
       </c>
       <c r="Y11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19090313945535342</v>
+        <v>0.19794289919111918</v>
       </c>
       <c r="Z11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19081627064866058</v>
+        <v>0.19788927850360005</v>
       </c>
       <c r="AA11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19076308745302273</v>
+        <v>0.19785619863949289</v>
       </c>
       <c r="AB11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19073033844696841</v>
+        <v>0.19783557849634625</v>
       </c>
       <c r="AC11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19070998446063592</v>
+        <v>0.19782251596725786</v>
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19069714883456135</v>
+        <v>0.1978140375254458</v>
       </c>
       <c r="AE11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19068887348196184</v>
+        <v>0.19780833954303068</v>
       </c>
       <c r="AF11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19068336414191467</v>
+        <v>0.19780432802953762</v>
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19067953250617031</v>
+        <v>0.19780133943291556</v>
       </c>
       <c r="AH11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19067671846950474</v>
+        <v>0.19779897128333379</v>
       </c>
       <c r="AI11" s="1">
         <f t="shared" si="6"/>
-        <v>0.19067452165287102</v>
+        <v>0.19779697946843089</v>
       </c>
     </row>
     <row r="12" spans="1:35">
@@ -2054,10 +2071,10 @@
       </c>
       <c r="C12" s="18">
         <f>$C35</f>
-        <v>0.48317407867273576</v>
+        <v>0.33332966266868663</v>
       </c>
       <c r="J12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K12">
         <f t="shared" ref="K12:AI12" si="7">1/(1+EXP(($E18-len)/2.5))</f>
@@ -2170,7 +2187,7 @@
       </c>
       <c r="C13" s="18">
         <f>$C36</f>
-        <v>0.25841296427403693</v>
+        <v>0.33334020082979787</v>
       </c>
     </row>
     <row r="14" spans="1:35">
@@ -2182,7 +2199,7 @@
       </c>
       <c r="C14" s="29">
         <f>spr</f>
-        <v>0.39999855522103445</v>
+        <v>0.40000071794109937</v>
       </c>
     </row>
     <row r="15" spans="1:35">
@@ -2192,7 +2209,7 @@
       </c>
       <c r="C15" s="26">
         <f>SUMXMY2(B11:B14,C11:C14)</f>
-        <v>3.3679871921936735E-2</v>
+        <v>6.8819710860641874E-13</v>
       </c>
     </row>
     <row r="17" spans="1:35">
@@ -2202,10 +2219,10 @@
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
         <v>83</v>
-      </c>
-      <c r="F17" t="s">
-        <v>84</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>9</v>
@@ -2662,7 +2679,7 @@
     </row>
     <row r="22" spans="1:35">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1">
         <v>98.238757374230488</v>
@@ -2672,108 +2689,108 @@
       </c>
       <c r="K22" s="1">
         <f t="shared" ref="K22:AI22" si="11">wa*flt1_*(1-EXP(-za))/za</f>
-        <v>3.2655808350543217E-6</v>
+        <v>3.2667895782250959E-6</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="11"/>
-        <v>2.3009539672437534E-4</v>
+        <v>2.3068035094066158E-4</v>
       </c>
       <c r="M22" s="1">
         <f t="shared" si="11"/>
-        <v>6.787051360975121E-3</v>
+        <v>6.8557661652764983E-3</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="11"/>
-        <v>0.13522994726863335</v>
+        <v>0.13672317508944951</v>
       </c>
       <c r="O22" s="1">
         <f t="shared" si="11"/>
-        <v>1.3105879209331885</v>
+        <v>1.317453228807103</v>
       </c>
       <c r="P22" s="1">
         <f t="shared" si="11"/>
-        <v>3.1801295895148693</v>
+        <v>3.1818720295293748</v>
       </c>
       <c r="Q22" s="1">
         <f t="shared" si="11"/>
-        <v>4.2038930844753279</v>
+        <v>4.1975605846596737</v>
       </c>
       <c r="R22" s="1">
         <f t="shared" si="11"/>
-        <v>4.9457485563634975</v>
+        <v>4.9328814288278497</v>
       </c>
       <c r="S22" s="1">
         <f t="shared" si="11"/>
-        <v>5.5737058202817948</v>
+        <v>5.555576348374184</v>
       </c>
       <c r="T22" s="1">
         <f t="shared" si="11"/>
-        <v>6.1082303046212862</v>
+        <v>6.0859567268192647</v>
       </c>
       <c r="U22" s="1">
         <f t="shared" si="11"/>
-        <v>6.5575712507721953</v>
+        <v>6.5320934644769757</v>
       </c>
       <c r="V22" s="1">
         <f t="shared" si="11"/>
-        <v>6.9310607701675107</v>
+        <v>6.9031283991504475</v>
       </c>
       <c r="W22" s="1">
         <f t="shared" si="11"/>
-        <v>7.2387860179234256</v>
+        <v>7.2089781044514902</v>
       </c>
       <c r="X22" s="1">
         <f t="shared" si="11"/>
-        <v>7.4906144439321123</v>
+        <v>7.4593710479823745</v>
       </c>
       <c r="Y22" s="1">
         <f t="shared" si="11"/>
-        <v>7.6956180045381997</v>
+        <v>7.6632715312191024</v>
       </c>
       <c r="Z22" s="1">
         <f t="shared" si="11"/>
-        <v>7.8618172879284858</v>
+        <v>7.8286188906919065</v>
       </c>
       <c r="AA22" s="1">
         <f t="shared" si="11"/>
-        <v>7.9961200483677413</v>
+        <v>7.962260254768359</v>
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="11"/>
-        <v>8.104367324155465</v>
+        <v>8.0699915363324557</v>
       </c>
       <c r="AC22" s="1">
         <f t="shared" si="11"/>
-        <v>8.19143282470956</v>
+        <v>8.1566527519325192</v>
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="11"/>
-        <v>8.2613431173784324</v>
+        <v>8.2262451524053013</v>
       </c>
       <c r="AE22" s="1">
         <f t="shared" si="11"/>
-        <v>8.3174001148777066</v>
+        <v>8.2820514774272187</v>
       </c>
       <c r="AF22" s="1">
         <f t="shared" si="11"/>
-        <v>8.3622960478271651</v>
+        <v>8.3267493166599582</v>
       </c>
       <c r="AG22" s="1">
         <f t="shared" si="11"/>
-        <v>8.3982163541531687</v>
+        <v>8.3625128390686108</v>
       </c>
       <c r="AH22" s="1">
         <f t="shared" si="11"/>
-        <v>8.426928978432386</v>
+        <v>8.3911012536579772</v>
       </c>
       <c r="AI22" s="1">
         <f t="shared" si="11"/>
-        <v>8.4498602722864771</v>
+        <v>8.4139340986396451</v>
       </c>
     </row>
     <row r="23" spans="1:35">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1">
         <f>1.5*M</f>
@@ -2784,103 +2801,103 @@
       </c>
       <c r="K23" s="1">
         <f t="shared" ref="K23:AI23" si="12">wa*flt2_*(1-EXP(-za))/za</f>
-        <v>2.1588031906815412E-3</v>
+        <v>2.159602264030384E-3</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="12"/>
-        <v>8.5850280804110821E-2</v>
+        <v>8.6068531514210317E-2</v>
       </c>
       <c r="M23" s="1">
         <f t="shared" si="12"/>
-        <v>0.8361533687560635</v>
+        <v>0.84461891764381447</v>
       </c>
       <c r="N23" s="1">
         <f t="shared" si="12"/>
-        <v>1.6478537077416682</v>
+        <v>1.6660495367775761</v>
       </c>
       <c r="O23" s="1">
         <f t="shared" si="12"/>
-        <v>1.5796210200624421</v>
+        <v>1.5878956153441637</v>
       </c>
       <c r="P23" s="1">
         <f t="shared" si="12"/>
-        <v>1.2656186379972079</v>
+        <v>1.2663120891588275</v>
       </c>
       <c r="Q23" s="1">
         <f t="shared" si="12"/>
-        <v>0.94460187624045111</v>
+        <v>0.94317898296344316</v>
       </c>
       <c r="R23" s="1">
         <f t="shared" si="12"/>
-        <v>0.66993795805300171</v>
+        <v>0.66819501114638069</v>
       </c>
       <c r="S23" s="1">
         <f t="shared" si="12"/>
-        <v>0.45771092505901934</v>
+        <v>0.45622213867071221</v>
       </c>
       <c r="T23" s="1">
         <f t="shared" si="12"/>
-        <v>0.30423437261107672</v>
+        <v>0.30312498615535072</v>
       </c>
       <c r="U23" s="1">
         <f t="shared" si="12"/>
-        <v>0.1981061851135778</v>
+        <v>0.1973364935837312</v>
       </c>
       <c r="V23" s="1">
         <f t="shared" si="12"/>
-        <v>0.12700423965766686</v>
+        <v>0.12649240897828123</v>
       </c>
       <c r="W23" s="1">
         <f t="shared" si="12"/>
-        <v>8.045404007360292E-2</v>
+        <v>8.0122745978288626E-2</v>
       </c>
       <c r="X23" s="1">
         <f t="shared" si="12"/>
-        <v>5.0496720970001067E-2</v>
+        <v>5.0286098856256151E-2</v>
       </c>
       <c r="Y23" s="1">
         <f t="shared" si="12"/>
-        <v>3.1466819764729079E-2</v>
+        <v>3.1334557398619373E-2</v>
       </c>
       <c r="Z23" s="1">
         <f t="shared" si="12"/>
-        <v>1.9498262521711916E-2</v>
+        <v>1.9415926461115236E-2</v>
       </c>
       <c r="AA23" s="1">
         <f t="shared" si="12"/>
-        <v>1.2028622323982512E-2</v>
+        <v>1.1977686786908113E-2</v>
       </c>
       <c r="AB23" s="1">
         <f t="shared" si="12"/>
-        <v>7.3946788373168548E-3</v>
+        <v>7.3633132907462715E-3</v>
       </c>
       <c r="AC23" s="1">
         <f t="shared" si="12"/>
-        <v>4.5333963465475184E-3</v>
+        <v>4.5141479612852385E-3</v>
       </c>
       <c r="AD23" s="1">
         <f t="shared" si="12"/>
-        <v>2.773180212049248E-3</v>
+        <v>2.7613984738302003E-3</v>
       </c>
       <c r="AE23" s="1">
         <f t="shared" si="12"/>
-        <v>1.6934744280831789E-3</v>
+        <v>1.6862772255002581E-3</v>
       </c>
       <c r="AF23" s="1">
         <f t="shared" si="12"/>
-        <v>1.0327143317838466E-3</v>
+        <v>1.0283244347370922E-3</v>
       </c>
       <c r="AG23" s="1">
         <f t="shared" si="12"/>
-        <v>6.2907922131657243E-4</v>
+        <v>6.264048034972993E-4</v>
       </c>
       <c r="AH23" s="1">
         <f t="shared" si="12"/>
-        <v>3.8286990628042661E-4</v>
+        <v>3.8124210596767605E-4</v>
       </c>
       <c r="AI23" s="1">
         <f t="shared" si="12"/>
-        <v>2.3286007989363263E-4</v>
+        <v>2.3187003137258055E-4</v>
       </c>
     </row>
     <row r="24" spans="1:35">
@@ -2890,103 +2907,103 @@
       </c>
       <c r="K24" s="1">
         <f t="shared" ref="K24:AI24" si="13">wa*flt3_*(1-EXP(-za))/za</f>
-        <v>3.2667706364552806E-6</v>
+        <v>3.2679798200268268E-6</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="13"/>
-        <v>2.3009554729323399E-4</v>
+        <v>2.3068050189230013E-4</v>
       </c>
       <c r="M24" s="1">
         <f t="shared" si="13"/>
-        <v>6.7870513894874645E-3</v>
+        <v>6.8557661940775137E-3</v>
       </c>
       <c r="N24" s="1">
         <f t="shared" si="13"/>
-        <v>0.13522994727871884</v>
+        <v>0.13672317509964638</v>
       </c>
       <c r="O24" s="1">
         <f t="shared" si="13"/>
-        <v>1.3105879209370981</v>
+        <v>1.317453228811033</v>
       </c>
       <c r="P24" s="1">
         <f t="shared" si="13"/>
-        <v>3.180129589515595</v>
+        <v>3.1818720295301008</v>
       </c>
       <c r="Q24" s="1">
         <f t="shared" si="13"/>
-        <v>4.2038930844754514</v>
+        <v>4.1975605846597963</v>
       </c>
       <c r="R24" s="1">
         <f t="shared" si="13"/>
-        <v>4.9457485563635268</v>
+        <v>4.9328814288278782</v>
       </c>
       <c r="S24" s="1">
         <f t="shared" si="13"/>
-        <v>5.5737058202818037</v>
+        <v>5.5555763483741929</v>
       </c>
       <c r="T24" s="1">
         <f t="shared" si="13"/>
-        <v>6.1082303046212889</v>
+        <v>6.0859567268192691</v>
       </c>
       <c r="U24" s="1">
         <f t="shared" si="13"/>
-        <v>6.5575712507721962</v>
+        <v>6.5320934644769766</v>
       </c>
       <c r="V24" s="1">
         <f t="shared" si="13"/>
-        <v>6.9310607701675115</v>
+        <v>6.9031283991504502</v>
       </c>
       <c r="W24" s="1">
         <f t="shared" si="13"/>
-        <v>7.2387860179234256</v>
+        <v>7.2089781044514902</v>
       </c>
       <c r="X24" s="1">
         <f t="shared" si="13"/>
-        <v>7.4906144439321123</v>
+        <v>7.4593710479823745</v>
       </c>
       <c r="Y24" s="1">
         <f t="shared" si="13"/>
-        <v>7.6956180045381997</v>
+        <v>7.6632715312191024</v>
       </c>
       <c r="Z24" s="1">
         <f t="shared" si="13"/>
-        <v>7.8618172879284858</v>
+        <v>7.8286188906919065</v>
       </c>
       <c r="AA24" s="1">
         <f t="shared" si="13"/>
-        <v>7.9961200483677413</v>
+        <v>7.962260254768359</v>
       </c>
       <c r="AB24" s="1">
         <f t="shared" si="13"/>
-        <v>8.104367324155465</v>
+        <v>8.0699915363324557</v>
       </c>
       <c r="AC24" s="1">
         <f t="shared" si="13"/>
-        <v>8.19143282470956</v>
+        <v>8.1566527519325192</v>
       </c>
       <c r="AD24" s="1">
         <f t="shared" si="13"/>
-        <v>8.2613431173784324</v>
+        <v>8.2262451524053013</v>
       </c>
       <c r="AE24" s="1">
         <f t="shared" si="13"/>
-        <v>8.3174001148777066</v>
+        <v>8.2820514774272187</v>
       </c>
       <c r="AF24" s="1">
         <f t="shared" si="13"/>
-        <v>8.3622960478271651</v>
+        <v>8.3267493166599582</v>
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="13"/>
-        <v>8.3982163541531687</v>
+        <v>8.3625128390686108</v>
       </c>
       <c r="AH24" s="1">
         <f t="shared" si="13"/>
-        <v>8.426928978432386</v>
+        <v>8.3911012536579772</v>
       </c>
       <c r="AI24" s="1">
         <f t="shared" si="13"/>
-        <v>8.4498602722864771</v>
+        <v>8.4139340986396451</v>
       </c>
     </row>
     <row r="25" spans="1:35">
@@ -3005,103 +3022,103 @@
       </c>
       <c r="K26">
         <f>qa1_/wa</f>
-        <v>4.2110614543555917E-5</v>
+        <v>4.212620163826208E-5</v>
       </c>
       <c r="L26">
         <f t="shared" ref="L26:AI26" si="14">qa1_/wa</f>
-        <v>5.1003032088331945E-4</v>
+        <v>5.1132693259690323E-4</v>
       </c>
       <c r="M26">
         <f t="shared" si="14"/>
-        <v>6.0534535049642842E-3</v>
+        <v>6.1147410731316396E-3</v>
       </c>
       <c r="N26">
         <f t="shared" si="14"/>
-        <v>6.825194896496356E-2</v>
+        <v>6.9005596445258388E-2</v>
       </c>
       <c r="O26">
         <f t="shared" si="14"/>
-        <v>0.44878220402434965</v>
+        <v>0.45113307873466074</v>
       </c>
       <c r="P26">
         <f t="shared" si="14"/>
-        <v>0.82520932297060579</v>
+        <v>0.82566146735787471</v>
       </c>
       <c r="Q26">
         <f t="shared" si="14"/>
-        <v>0.88919278071825503</v>
+        <v>0.88785335247713881</v>
       </c>
       <c r="R26">
         <f t="shared" si="14"/>
-        <v>0.89699593671803524</v>
+        <v>0.89466226346611499</v>
       </c>
       <c r="S26">
         <f t="shared" si="14"/>
-        <v>0.89893242240135751</v>
+        <v>0.89600848442826553</v>
       </c>
       <c r="T26">
         <f t="shared" si="14"/>
-        <v>0.89986842054044003</v>
+        <v>0.89658706272043032</v>
       </c>
       <c r="U26">
         <f t="shared" si="14"/>
-        <v>0.90040908341103965</v>
+        <v>0.89691077140982123</v>
       </c>
       <c r="V26">
         <f t="shared" si="14"/>
-        <v>0.90072706597160135</v>
+        <v>0.89709711040980333</v>
       </c>
       <c r="W26">
         <f t="shared" si="14"/>
-        <v>0.90091128162617939</v>
+        <v>0.89720150412175925</v>
       </c>
       <c r="X26">
         <f t="shared" si="14"/>
-        <v>0.90101443024329764</v>
+        <v>0.89725629386994277</v>
       </c>
       <c r="Y26">
         <f t="shared" si="14"/>
-        <v>0.90106840059187354</v>
+        <v>0.89728100041670389</v>
       </c>
       <c r="Z26">
         <f t="shared" si="14"/>
-        <v>0.90109253727645255</v>
+        <v>0.89728745927682085</v>
       </c>
       <c r="AA26">
         <f t="shared" si="14"/>
-        <v>0.90109857696314799</v>
+        <v>0.89728284987999873</v>
       </c>
       <c r="AB26">
         <f t="shared" si="14"/>
-        <v>0.90109363975518164</v>
+        <v>0.89727152724103609</v>
       </c>
       <c r="AC26">
         <f t="shared" si="14"/>
-        <v>0.90108204472528941</v>
+        <v>0.89725613297526041</v>
       </c>
       <c r="AD26">
         <f t="shared" si="14"/>
-        <v>0.90106641168848289</v>
+        <v>0.8972382693505403</v>
       </c>
       <c r="AE26">
         <f t="shared" si="14"/>
-        <v>0.90104832968869231</v>
+        <v>0.89721890819981143</v>
       </c>
       <c r="AF26">
         <f t="shared" si="14"/>
-        <v>0.90102876253753994</v>
+        <v>0.8971986389670924</v>
       </c>
       <c r="AG26">
         <f t="shared" si="14"/>
-        <v>0.90100829481365896</v>
+        <v>0.89717781916399519</v>
       </c>
       <c r="AH26">
         <f t="shared" si="14"/>
-        <v>0.90098728107758164</v>
+        <v>0.89715666562866692</v>
       </c>
       <c r="AI26">
         <f t="shared" si="14"/>
-        <v>0.90096593637751587</v>
+        <v>0.89713530987753232</v>
       </c>
     </row>
     <row r="27" spans="1:35">
@@ -3109,7 +3126,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="28">
-        <v>3.0787693388999178E-2</v>
+        <v>3.5208887951138419E-2</v>
       </c>
       <c r="C27">
         <v>3.0826511509620572E-2</v>
@@ -3119,103 +3136,103 @@
       </c>
       <c r="K27">
         <f t="shared" ref="K27:AI27" si="15">qa2_/wa</f>
-        <v>2.7838394953306003E-2</v>
+        <v>2.7848699236520776E-2</v>
       </c>
       <c r="L27">
         <f t="shared" si="15"/>
-        <v>0.19029605498320337</v>
+        <v>0.19077983032721166</v>
       </c>
       <c r="M27">
         <f t="shared" si="15"/>
-        <v>0.74577534065645623</v>
+        <v>0.75332586648283517</v>
       </c>
       <c r="N27">
         <f t="shared" si="15"/>
-        <v>0.83168876002806524</v>
+        <v>0.84087238258961927</v>
       </c>
       <c r="O27">
         <f t="shared" si="15"/>
-        <v>0.5409067118534453</v>
+        <v>0.54374016625099264</v>
       </c>
       <c r="P27">
         <f t="shared" si="15"/>
-        <v>0.3284143837547136</v>
+        <v>0.32859432685057988</v>
       </c>
       <c r="Q27">
         <f t="shared" si="15"/>
-        <v>0.1997988892980509</v>
+        <v>0.19949792388236978</v>
       </c>
       <c r="R27">
         <f t="shared" si="15"/>
-        <v>0.12150468617203058</v>
+        <v>0.1211885729941492</v>
       </c>
       <c r="S27">
         <f t="shared" si="15"/>
-        <v>7.3820040721501223E-2</v>
+        <v>7.3579927877796922E-2</v>
       </c>
       <c r="T27">
         <f t="shared" si="15"/>
-        <v>4.4820003618481E-2</v>
+        <v>4.465656809167582E-2</v>
       </c>
       <c r="U27">
         <f t="shared" si="15"/>
-        <v>2.7201627208422535E-2</v>
+        <v>2.7095942158516777E-2</v>
       </c>
       <c r="V27">
         <f t="shared" si="15"/>
-        <v>1.6504855453754682E-2</v>
+        <v>1.643834041927373E-2</v>
       </c>
       <c r="W27">
         <f t="shared" si="15"/>
-        <v>1.0012998336357281E-2</v>
+        <v>9.9717667559146798E-3</v>
       </c>
       <c r="X27">
         <f t="shared" si="15"/>
-        <v>6.0740376660017347E-3</v>
+        <v>6.0487028199443143E-3</v>
       </c>
       <c r="Y27">
         <f t="shared" si="15"/>
-        <v>3.6844028563263703E-3</v>
+        <v>3.6689164537244364E-3</v>
       </c>
       <c r="Z27">
         <f t="shared" si="15"/>
-        <v>2.2348190252588804E-3</v>
+        <v>2.2253819692913839E-3</v>
       </c>
       <c r="AA27">
         <f t="shared" si="15"/>
-        <v>1.355529230852452E-3</v>
+        <v>1.3497892044775398E-3</v>
       </c>
       <c r="AB27">
         <f t="shared" si="15"/>
-        <v>8.2218608829318139E-4</v>
+        <v>8.1869867300316153E-4</v>
       </c>
       <c r="AC27">
         <f t="shared" si="15"/>
-        <v>4.986871206676878E-4</v>
+        <v>4.965697408733402E-4</v>
       </c>
       <c r="AD27">
         <f t="shared" si="15"/>
-        <v>3.0247134238744355E-4</v>
+        <v>3.011863057499798E-4</v>
       </c>
       <c r="AE27">
         <f t="shared" si="15"/>
-        <v>1.8345904774563049E-4</v>
+        <v>1.8267935369746614E-4</v>
       </c>
       <c r="AF27">
         <f t="shared" si="15"/>
-        <v>1.1127390265784259E-4</v>
+        <v>1.1080089578495962E-4</v>
       </c>
       <c r="AG27">
         <f t="shared" si="15"/>
-        <v>6.7491187723551203E-5</v>
+        <v>6.7204261007526453E-5</v>
       </c>
       <c r="AH27">
         <f t="shared" si="15"/>
-        <v>4.0935543274295071E-5</v>
+        <v>4.0761502721482056E-5</v>
       </c>
       <c r="AI27">
         <f t="shared" si="15"/>
-        <v>2.4828694577873729E-5</v>
+        <v>2.4723130702959205E-5</v>
       </c>
     </row>
     <row r="28" spans="1:35">
@@ -3223,7 +3240,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="28">
-        <v>6.5781326112657759E-2</v>
+        <v>4.0463010824188246E-2</v>
       </c>
       <c r="C28">
         <v>6.5872059610417921E-2</v>
@@ -3233,103 +3250,103 @@
       </c>
       <c r="K28">
         <f t="shared" ref="K28:AI28" si="16">qa3_/wa</f>
-        <v>4.212595737863179E-5</v>
+        <v>4.214155015243398E-5</v>
       </c>
       <c r="L28">
         <f t="shared" si="16"/>
-        <v>5.1003065463481724E-4</v>
+        <v>5.1132726719687238E-4</v>
       </c>
       <c r="M28">
         <f t="shared" si="16"/>
-        <v>6.0534535303947892E-3</v>
+        <v>6.1147410988196147E-3</v>
       </c>
       <c r="N28">
         <f t="shared" si="16"/>
-        <v>6.8251948970053808E-2</v>
+        <v>6.9005596450404855E-2</v>
       </c>
       <c r="O28">
         <f t="shared" si="16"/>
-        <v>0.44878220402568836</v>
+        <v>0.4511330787360065</v>
       </c>
       <c r="P28">
         <f t="shared" si="16"/>
-        <v>0.82520932297079408</v>
+        <v>0.82566146735806312</v>
       </c>
       <c r="Q28">
         <f t="shared" si="16"/>
-        <v>0.88919278071828123</v>
+        <v>0.88785335247716479</v>
       </c>
       <c r="R28">
         <f t="shared" si="16"/>
-        <v>0.89699593671804057</v>
+        <v>0.89466226346612021</v>
       </c>
       <c r="S28">
         <f t="shared" si="16"/>
-        <v>0.89893242240135895</v>
+        <v>0.89600848442826697</v>
       </c>
       <c r="T28">
         <f t="shared" si="16"/>
-        <v>0.89986842054044047</v>
+        <v>0.89658706272043098</v>
       </c>
       <c r="U28">
         <f t="shared" si="16"/>
-        <v>0.90040908341103976</v>
+        <v>0.89691077140982134</v>
       </c>
       <c r="V28">
         <f t="shared" si="16"/>
-        <v>0.90072706597160146</v>
+        <v>0.89709711040980367</v>
       </c>
       <c r="W28">
         <f t="shared" si="16"/>
-        <v>0.90091128162617939</v>
+        <v>0.89720150412175925</v>
       </c>
       <c r="X28">
         <f t="shared" si="16"/>
-        <v>0.90101443024329764</v>
+        <v>0.89725629386994277</v>
       </c>
       <c r="Y28">
         <f t="shared" si="16"/>
-        <v>0.90106840059187354</v>
+        <v>0.89728100041670389</v>
       </c>
       <c r="Z28">
         <f t="shared" si="16"/>
-        <v>0.90109253727645255</v>
+        <v>0.89728745927682085</v>
       </c>
       <c r="AA28">
         <f t="shared" si="16"/>
-        <v>0.90109857696314799</v>
+        <v>0.89728284987999873</v>
       </c>
       <c r="AB28">
         <f t="shared" si="16"/>
-        <v>0.90109363975518164</v>
+        <v>0.89727152724103609</v>
       </c>
       <c r="AC28">
         <f t="shared" si="16"/>
-        <v>0.90108204472528941</v>
+        <v>0.89725613297526041</v>
       </c>
       <c r="AD28">
         <f t="shared" si="16"/>
-        <v>0.90106641168848289</v>
+        <v>0.8972382693505403</v>
       </c>
       <c r="AE28">
         <f t="shared" si="16"/>
-        <v>0.90104832968869231</v>
+        <v>0.89721890819981143</v>
       </c>
       <c r="AF28">
         <f t="shared" si="16"/>
-        <v>0.90102876253753994</v>
+        <v>0.8971986389670924</v>
       </c>
       <c r="AG28">
         <f t="shared" si="16"/>
-        <v>0.90100829481365896</v>
+        <v>0.89717781916399519</v>
       </c>
       <c r="AH28">
         <f t="shared" si="16"/>
-        <v>0.90098728107758164</v>
+        <v>0.89715666562866692</v>
       </c>
       <c r="AI28">
         <f t="shared" si="16"/>
-        <v>0.90096593637751587</v>
+        <v>0.89713530987753232</v>
       </c>
     </row>
     <row r="29" spans="1:35">
@@ -3337,7 +3354,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="28">
-        <v>3.0787694006063286E-2</v>
+        <v>3.5209950754932245E-2</v>
       </c>
       <c r="C29">
         <v>3.0717558531607573E-2</v>
@@ -3362,11 +3379,11 @@
       <c r="C31" s="12"/>
       <c r="G31">
         <f>SUMPRODUCT(dlz1_,wa,ma)</f>
-        <v>-49.079690806817631</v>
+        <v>-47.817938969923659</v>
       </c>
       <c r="H31">
         <f>Ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-18.951970709822817</v>
+        <v>-18.464549473444112</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>52</v>
@@ -3376,99 +3393,99 @@
       </c>
       <c r="L31">
         <f t="shared" ref="L31:AH31" si="17">K31*sa-K$7*K18*K$10</f>
-        <v>-3.8991718982783872E-5</v>
+        <v>-3.90213379669535E-5</v>
       </c>
       <c r="M31">
         <f t="shared" si="17"/>
-        <v>-4.3503323402386499E-4</v>
+        <v>-4.3814399963989554E-4</v>
       </c>
       <c r="N31">
         <f t="shared" si="17"/>
-        <v>-4.3294720984077481E-3</v>
+        <v>-4.4481666599328644E-3</v>
       </c>
       <c r="O31">
         <f t="shared" si="17"/>
-        <v>-3.9826298607956542E-2</v>
+        <v>-4.1806465450880126E-2</v>
       </c>
       <c r="P31">
         <f t="shared" si="17"/>
-        <v>-0.22381379132458709</v>
+        <v>-0.23738433924166549</v>
       </c>
       <c r="Q31">
         <f t="shared" si="17"/>
-        <v>-0.46050606304316027</v>
+        <v>-0.48862735618965492</v>
       </c>
       <c r="R31">
         <f t="shared" si="17"/>
-        <v>-0.61116899330511409</v>
+        <v>-0.64614545984844829</v>
       </c>
       <c r="S31">
         <f t="shared" si="17"/>
-        <v>-0.68709212209979187</v>
+        <v>-0.72235409500746584</v>
       </c>
       <c r="T31">
         <f t="shared" si="17"/>
-        <v>-0.71139777495034473</v>
+        <v>-0.74287154774701059</v>
       </c>
       <c r="U31">
         <f t="shared" si="17"/>
-        <v>-0.70136468674310593</v>
+        <v>-0.72694990209767929</v>
       </c>
       <c r="V31">
         <f t="shared" si="17"/>
-        <v>-0.66932583464532402</v>
+        <v>-0.68827939038455688</v>
       </c>
       <c r="W31">
         <f t="shared" si="17"/>
-        <v>-0.62405908827158252</v>
+        <v>-0.63649668610989618</v>
       </c>
       <c r="X31">
         <f t="shared" si="17"/>
-        <v>-0.5717646613850732</v>
+        <v>-0.57829676973392075</v>
       </c>
       <c r="Y31">
         <f t="shared" si="17"/>
-        <v>-0.51675437479415809</v>
+        <v>-0.51823591270056701</v>
       </c>
       <c r="Z31">
         <f t="shared" si="17"/>
-        <v>-0.46195375947663692</v>
+        <v>-0.45932052117026717</v>
       </c>
       <c r="AA31">
         <f t="shared" si="17"/>
-        <v>-0.40927505870305525</v>
+        <v>-0.40344269284385242</v>
       </c>
       <c r="AB31">
         <f t="shared" si="17"/>
-        <v>-0.35989659347079322</v>
+        <v>-0.35170297601902495</v>
       </c>
       <c r="AC31">
         <f t="shared" si="17"/>
-        <v>-0.31447218258430565</v>
+        <v>-0.30464889420489322</v>
       </c>
       <c r="AD31">
         <f t="shared" si="17"/>
-        <v>-0.27328756950352651</v>
+        <v>-0.262450201834311</v>
       </c>
       <c r="AE31">
         <f t="shared" si="17"/>
-        <v>-0.23637650698592094</v>
+        <v>-0.22502659895523558</v>
       </c>
       <c r="AF31">
         <f t="shared" si="17"/>
-        <v>-0.20360614707691949</v>
+        <v>-0.19213982162023063</v>
       </c>
       <c r="AG31">
         <f t="shared" si="17"/>
-        <v>-0.17473915918534058</v>
+        <v>-0.16345916420539841</v>
       </c>
       <c r="AH31">
         <f t="shared" si="17"/>
-        <v>-0.14947829749420263</v>
+        <v>-0.13860731019405945</v>
       </c>
       <c r="AI31">
         <f>(AH31*sa-AH$7*AH18*AH$10)/oa-AH$7*AH$10*flt1_*sa/oa^2</f>
-        <v>-0.81383039081007091</v>
+        <v>-0.7155171306819218</v>
       </c>
     </row>
     <row r="32" spans="1:35">
@@ -3481,11 +3498,11 @@
       </c>
       <c r="G32">
         <f>SUMPRODUCT(dlz2_,wa,ma)</f>
-        <v>-16.996357177698648</v>
+        <v>-16.703914278445254</v>
       </c>
       <c r="H32">
         <f>Ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-6.5630907226637794</v>
+        <v>-6.4500950529991918</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>53</v>
@@ -3495,99 +3512,99 @@
       </c>
       <c r="L32">
         <f t="shared" ref="L32:AH32" si="18">K32*sa-K$7*K19*K$10</f>
-        <v>-2.5776562149866865E-2</v>
+        <v>-2.5796142604542417E-2</v>
       </c>
       <c r="M32">
         <f t="shared" si="18"/>
-        <v>-0.17146442745920967</v>
+        <v>-0.17282468684952912</v>
       </c>
       <c r="N32">
         <f t="shared" si="18"/>
-        <v>-0.62840367100529471</v>
+        <v>-0.64601751445363953</v>
       </c>
       <c r="O32">
         <f t="shared" si="18"/>
-        <v>-0.94707058775372066</v>
+        <v>-0.98934192656161901</v>
       </c>
       <c r="P32">
         <f t="shared" si="18"/>
-        <v>-0.98330831761341875</v>
+        <v>-1.0321687475444767</v>
       </c>
       <c r="Q32">
         <f t="shared" si="18"/>
-        <v>-0.89672510916241599</v>
+        <v>-0.9402497837896433</v>
       </c>
       <c r="R32">
         <f t="shared" si="18"/>
-        <v>-0.77363974832562965</v>
+        <v>-0.8077488848542248</v>
       </c>
       <c r="S32">
         <f t="shared" si="18"/>
-        <v>-0.64917285309971251</v>
+        <v>-0.6736835094603385</v>
       </c>
       <c r="T32">
         <f t="shared" si="18"/>
-        <v>-0.53656742305101413</v>
+        <v>-0.55284448724586355</v>
       </c>
       <c r="U32">
         <f t="shared" si="18"/>
-        <v>-0.4397009357944679</v>
+        <v>-0.44950383770841967</v>
       </c>
       <c r="V32">
         <f t="shared" si="18"/>
-        <v>-0.35851919813251165</v>
+        <v>-0.36350733330370294</v>
       </c>
       <c r="W32">
         <f t="shared" si="18"/>
-        <v>-0.29145836261344682</v>
+        <v>-0.29302024812669353</v>
       </c>
       <c r="X32">
         <f t="shared" si="18"/>
-        <v>-0.23652041618298222</v>
+        <v>-0.23574739488476668</v>
       </c>
       <c r="Y32">
         <f t="shared" si="18"/>
-        <v>-0.1917329112366872</v>
+        <v>-0.18944966041831099</v>
       </c>
       <c r="Z32">
         <f t="shared" si="18"/>
-        <v>-0.15532626566567354</v>
+        <v>-0.15213803615102722</v>
       </c>
       <c r="AA32">
         <f t="shared" si="18"/>
-        <v>-0.12578365563440011</v>
+        <v>-0.1221233908325392</v>
       </c>
       <c r="AB32">
         <f t="shared" si="18"/>
-        <v>-0.1018360440290399</v>
+        <v>-9.8005273493822431E-2</v>
       </c>
       <c r="AC32">
         <f t="shared" si="18"/>
-        <v>-8.2436072521177461E-2</v>
+        <v>-7.8638172292992359E-2</v>
       </c>
       <c r="AD32">
         <f t="shared" si="18"/>
-        <v>-6.6726144371860321E-2</v>
+        <v>-6.3092435741744363E-2</v>
       </c>
       <c r="AE32">
         <f t="shared" si="18"/>
-        <v>-5.4007314045288718E-2</v>
+        <v>-5.0617090229985673E-2</v>
       </c>
       <c r="AF32">
         <f t="shared" si="18"/>
-        <v>-4.3711522622709054E-2</v>
+        <v>-4.060717752219991E-2</v>
       </c>
       <c r="AG32">
         <f t="shared" si="18"/>
-        <v>-3.5377859521400747E-2</v>
+        <v>-3.2576175004921382E-2</v>
       </c>
       <c r="AH32">
         <f t="shared" si="18"/>
-        <v>-2.8632728943360622E-2</v>
+        <v>-2.6133201414663666E-2</v>
       </c>
       <c r="AI32">
         <f>(AH32*sa-AH$7*AH19*AH$10)/oa-AH$7*AH$10*flt2_*sa/oa^2</f>
-        <v>-0.12153829418246669</v>
+        <v>-0.10599290457540135</v>
       </c>
     </row>
     <row r="33" spans="1:35">
@@ -3596,15 +3613,15 @@
       </c>
       <c r="B33" s="1">
         <f>SUMPRODUCT(lz,wa,ma)</f>
-        <v>4.8520735804265502</v>
+        <v>4.8520998147135295</v>
       </c>
       <c r="G33">
         <f>SUMPRODUCT(dlz3_,wa,ma)</f>
-        <v>-49.079690885129232</v>
+        <v>-47.8179390471456</v>
       </c>
       <c r="H33">
         <f>Ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-18.951970740062599</v>
+        <v>-18.464549503262802</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>54</v>
@@ -3614,99 +3631,99 @@
       </c>
       <c r="L33">
         <f t="shared" ref="L33:AH33" si="19">K33*sa-K$7*K20*K$10</f>
-        <v>-3.9005925460655596E-5</v>
+        <v>-3.9035555236384412E-5</v>
       </c>
       <c r="M33">
         <f t="shared" si="19"/>
-        <v>-4.3504507509284211E-4</v>
+        <v>-4.3815609484132358E-4</v>
       </c>
       <c r="N33">
         <f t="shared" si="19"/>
-        <v>-4.3294816607812731E-3</v>
+        <v>-4.4481766518580006E-3</v>
       </c>
       <c r="O33">
         <f t="shared" si="19"/>
-        <v>-3.9826306281285272E-2</v>
+        <v>-4.1806473556254872E-2</v>
       </c>
       <c r="P33">
         <f t="shared" si="19"/>
-        <v>-0.22381379741513843</v>
+        <v>-0.2373843456824811</v>
       </c>
       <c r="Q33">
         <f t="shared" si="19"/>
-        <v>-0.4605060679024921</v>
+        <v>-0.48862736131236695</v>
       </c>
       <c r="R33">
         <f t="shared" si="19"/>
-        <v>-0.61116899720306983</v>
+        <v>-0.6461454639355011</v>
       </c>
       <c r="S33">
         <f t="shared" si="19"/>
-        <v>-0.68709212523744978</v>
+        <v>-0.72235409827515906</v>
       </c>
       <c r="T33">
         <f t="shared" si="19"/>
-        <v>-0.71139777748137178</v>
+        <v>-0.7428715503630211</v>
       </c>
       <c r="U33">
         <f t="shared" si="19"/>
-        <v>-0.70136468878742364</v>
+        <v>-0.72694990419363803</v>
       </c>
       <c r="V33">
         <f t="shared" si="19"/>
-        <v>-0.66932583629781939</v>
+        <v>-0.68827939206465871</v>
       </c>
       <c r="W33">
         <f t="shared" si="19"/>
-        <v>-0.62405908960798961</v>
+        <v>-0.63649668745704613</v>
       </c>
       <c r="X33">
         <f t="shared" si="19"/>
-        <v>-0.57176466246616575</v>
+        <v>-0.57829677081429409</v>
       </c>
       <c r="Y33">
         <f t="shared" si="19"/>
-        <v>-0.51675437566886662</v>
+        <v>-0.51823591356708809</v>
       </c>
       <c r="Z33">
         <f t="shared" si="19"/>
-        <v>-0.46195376018443685</v>
+        <v>-0.45932052186531303</v>
       </c>
       <c r="AA33">
         <f t="shared" si="19"/>
-        <v>-0.40927505927583308</v>
+        <v>-0.40344269340137912</v>
       </c>
       <c r="AB33">
         <f t="shared" si="19"/>
-        <v>-0.35989659393432494</v>
+        <v>-0.35170297646625304</v>
       </c>
       <c r="AC33">
         <f t="shared" si="19"/>
-        <v>-0.31447218295943719</v>
+        <v>-0.30464889456364952</v>
       </c>
       <c r="AD33">
         <f t="shared" si="19"/>
-        <v>-0.27328756980712154</v>
+        <v>-0.2624502021221003</v>
       </c>
       <c r="AE33">
         <f t="shared" si="19"/>
-        <v>-0.23637650723162379</v>
+        <v>-0.22502659918609774</v>
       </c>
       <c r="AF33">
         <f t="shared" si="19"/>
-        <v>-0.20360614727577089</v>
+        <v>-0.19213982180542727</v>
       </c>
       <c r="AG33">
         <f t="shared" si="19"/>
-        <v>-0.1747391593462751</v>
+        <v>-0.1634591643539629</v>
       </c>
       <c r="AH33">
         <f t="shared" si="19"/>
-        <v>-0.14947829762445067</v>
+        <v>-0.13860731031323806</v>
       </c>
       <c r="AI33">
         <f>(AH33*sa-AH$7*AH20*AH$10)/oa-AH$7*AH$10*flt3_*sa/oa^2</f>
-        <v>-0.8138303913629138</v>
+        <v>-0.71551713116527316</v>
       </c>
     </row>
     <row r="34" spans="1:35">
@@ -3715,11 +3732,11 @@
       </c>
       <c r="B34" s="1">
         <f>f1_*SUMPRODUCT(lz,ta1_)</f>
-        <v>6.0995221285221717E-2</v>
+        <v>7.2482496807273103E-2</v>
       </c>
       <c r="C34" s="10">
         <f>phi_t1/SUM(phi_t1,phi_t2,phi_t3)</f>
-        <v>0.25841295705322731</v>
+        <v>0.33333013650151561</v>
       </c>
       <c r="G34" t="s">
         <v>57</v>
@@ -3732,126 +3749,126 @@
       </c>
       <c r="B35" s="1">
         <f>f2_*SUMPRODUCT(lz,ta2_)</f>
-        <v>0.11404733796632423</v>
+        <v>7.2482393772525411E-2</v>
       </c>
       <c r="C35" s="10">
         <f>phi_t2/SUM(phi_t1,phi_t2,phi_t3)</f>
-        <v>0.48317407867273576</v>
+        <v>0.33332966266868663</v>
       </c>
       <c r="G35" s="1">
         <f>SUM(dqa11_)</f>
-        <v>137.4084926040556</v>
+        <v>136.71146438911074</v>
       </c>
       <c r="H35" s="1">
         <f>SUM(dqa12_)</f>
-        <v>141.92146068490834</v>
+        <v>141.32829153260764</v>
       </c>
       <c r="I35" s="11">
         <f>SUM(dqa13_)</f>
-        <v>137.40849260405466</v>
+        <v>136.71146438910975</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>62</v>
       </c>
       <c r="K35">
         <f>flt1_*qa1_+lz*wa*flt1_^2/za*(sa-oa/za)</f>
-        <v>7.5991458553258747E-11</v>
+        <v>7.6010214162441637E-11</v>
       </c>
       <c r="L35">
         <f t="shared" ref="L35:AI35" si="20">flt1_*qa1_+lz*wa*flt1_^2/za*(sa-oa/za)</f>
-        <v>7.4066112649766338E-8</v>
+        <v>7.4166314318042136E-8</v>
       </c>
       <c r="M35">
         <f t="shared" si="20"/>
-        <v>2.9428931251104205E-5</v>
+        <v>2.9571650125643609E-5</v>
       </c>
       <c r="N35">
         <f t="shared" si="20"/>
-        <v>7.3201566582624319E-3</v>
+        <v>7.3082888404331532E-3</v>
       </c>
       <c r="O35">
         <f t="shared" si="20"/>
-        <v>0.50412636455546866</v>
+        <v>0.49874737370074251</v>
       </c>
       <c r="P35">
         <f t="shared" si="20"/>
-        <v>2.3960659894751637</v>
+        <v>2.3634477273045404</v>
       </c>
       <c r="Q35">
         <f t="shared" si="20"/>
-        <v>3.5630682569194243</v>
+        <v>3.519221888802369</v>
       </c>
       <c r="R35">
         <f t="shared" si="20"/>
-        <v>4.3637973900479512</v>
+        <v>4.3182727417528275</v>
       </c>
       <c r="S35">
         <f t="shared" si="20"/>
-        <v>5.0491855067432923</v>
+        <v>5.0049734831627459</v>
       </c>
       <c r="T35">
         <f t="shared" si="20"/>
-        <v>5.6454278537903626</v>
+        <v>5.6036701549180599</v>
       </c>
       <c r="U35">
         <f t="shared" si="20"/>
-        <v>6.1565569056829492</v>
+        <v>6.1174931249939553</v>
       </c>
       <c r="V35">
         <f t="shared" si="20"/>
-        <v>6.5884698005544049</v>
+        <v>6.5518547076763616</v>
       </c>
       <c r="W35">
         <f t="shared" si="20"/>
-        <v>6.9492958745598514</v>
+        <v>6.9146657289436346</v>
       </c>
       <c r="X35">
         <f t="shared" si="20"/>
-        <v>7.2480526662468492</v>
+        <v>7.2148884173727144</v>
       </c>
       <c r="Y35">
         <f t="shared" si="20"/>
-        <v>7.4936861067749199</v>
+        <v>7.4615025453800534</v>
       </c>
       <c r="Z35">
         <f t="shared" si="20"/>
-        <v>7.6945234758923098</v>
+        <v>7.6629099322638501</v>
       </c>
       <c r="AA35">
         <f t="shared" si="20"/>
-        <v>7.8580094232575695</v>
+        <v>7.8266415648626619</v>
       </c>
       <c r="AB35">
         <f t="shared" si="20"/>
-        <v>7.9906192237875393</v>
+        <v>7.9592552890548491</v>
       </c>
       <c r="AC35">
         <f t="shared" si="20"/>
-        <v>8.0978759257291291</v>
+        <v>8.0663457653706914</v>
       </c>
       <c r="AD35">
         <f t="shared" si="20"/>
-        <v>8.18442319511378</v>
+        <v>8.1526149976363005</v>
       </c>
       <c r="AE35">
         <f t="shared" si="20"/>
-        <v>8.254123462604646</v>
+        <v>8.2219707707251022</v>
       </c>
       <c r="AF35">
         <f t="shared" si="20"/>
-        <v>8.3101630606320711</v>
+        <v>8.2776333007029823</v>
       </c>
       <c r="AG35">
         <f t="shared" si="20"/>
-        <v>8.3551539683607459</v>
+        <v>8.32223892018723</v>
       </c>
       <c r="AH35">
         <f t="shared" si="20"/>
-        <v>8.3912268209169678</v>
+        <v>8.3579350315992631</v>
       </c>
       <c r="AI35">
         <f t="shared" si="20"/>
-        <v>8.3072916726785966</v>
+        <v>8.2878429879669113</v>
       </c>
     </row>
     <row r="36" spans="1:35">
@@ -3860,126 +3877,126 @@
       </c>
       <c r="B36" s="1">
         <f>f3_*SUMPRODUCT(lz,ta3_)</f>
-        <v>6.0995222989605608E-2</v>
+        <v>7.248468529118951E-2</v>
       </c>
       <c r="C36" s="10">
         <f>phi_t3/SUM(phi_t1,phi_t2,phi_t3)</f>
-        <v>0.25841296427403693</v>
+        <v>0.33334020082979787</v>
       </c>
       <c r="G36" s="1">
         <f>SUM(dqa21_)</f>
-        <v>141.92146068490834</v>
+        <v>141.32829153260764</v>
       </c>
       <c r="H36" s="1">
         <f>SUM(dqa22_)</f>
-        <v>2.9730494024317755</v>
+        <v>2.9569816276083545</v>
       </c>
       <c r="I36" s="11">
         <f>SUM(dqa23_)</f>
-        <v>141.92146068486642</v>
+        <v>141.32829153256534</v>
       </c>
       <c r="J36" s="8" t="s">
         <v>63</v>
       </c>
       <c r="K36">
         <f t="shared" ref="K36:AI36" si="21">flt2_*qa2_+lz*wa*flt2_^2/za*(sa-oa/za)</f>
-        <v>3.3210086412017938E-5</v>
+        <v>3.3218283062188014E-5</v>
       </c>
       <c r="L36">
         <f t="shared" si="21"/>
-        <v>1.031067578412727E-2</v>
+        <v>1.0324624766700524E-2</v>
       </c>
       <c r="M36">
         <f t="shared" si="21"/>
-        <v>0.44666724568426142</v>
+        <v>0.44883340816069484</v>
       </c>
       <c r="N36">
         <f t="shared" si="21"/>
-        <v>1.0869559022189095</v>
+        <v>1.0851936729063125</v>
       </c>
       <c r="O36">
         <f t="shared" si="21"/>
-        <v>0.7323402385867368</v>
+        <v>0.72452622265170485</v>
       </c>
       <c r="P36">
         <f t="shared" si="21"/>
-        <v>0.37950269363964428</v>
+        <v>0.37433642592833344</v>
       </c>
       <c r="Q36">
         <f t="shared" si="21"/>
-        <v>0.17989472351343327</v>
+        <v>0.17768097690496787</v>
       </c>
       <c r="R36">
         <f t="shared" si="21"/>
-        <v>8.0069973139530112E-2</v>
+        <v>7.9234655401247814E-2</v>
       </c>
       <c r="S36">
         <f t="shared" si="21"/>
-        <v>3.4049896676572079E-2</v>
+        <v>3.3751746641726019E-2</v>
       </c>
       <c r="T36">
         <f t="shared" si="21"/>
-        <v>1.4004983896324381E-2</v>
+        <v>1.3901392828401776E-2</v>
       </c>
       <c r="U36">
         <f t="shared" si="21"/>
-        <v>5.6188563835489098E-3</v>
+        <v>5.5832043499768162E-3</v>
       </c>
       <c r="V36">
         <f t="shared" si="21"/>
-        <v>2.2121857167051741E-3</v>
+        <v>2.199891604728851E-3</v>
       </c>
       <c r="W36">
         <f t="shared" si="21"/>
-        <v>8.5843030277643595E-4</v>
+        <v>8.541525217000323E-4</v>
       </c>
       <c r="X36">
         <f t="shared" si="21"/>
-        <v>3.2939181920639478E-4</v>
+        <v>3.2788465131285328E-4</v>
       </c>
       <c r="Y36">
         <f t="shared" si="21"/>
-        <v>1.2528936227013192E-4</v>
+        <v>1.2475127489560214E-4</v>
       </c>
       <c r="Z36">
         <f t="shared" si="21"/>
-        <v>4.7329036448110664E-5</v>
+        <v>4.7134581448612226E-5</v>
       </c>
       <c r="AA36">
         <f t="shared" si="21"/>
-        <v>1.7782209068844278E-5</v>
+        <v>1.7711225466512465E-5</v>
       </c>
       <c r="AB36">
         <f t="shared" si="21"/>
-        <v>6.6524379948985889E-6</v>
+        <v>6.6263265478077122E-6</v>
       </c>
       <c r="AC36">
         <f t="shared" si="21"/>
-        <v>2.4802688028012363E-6</v>
+        <v>2.47061154529302E-6</v>
       </c>
       <c r="AD36">
         <f t="shared" si="21"/>
-        <v>9.2223785082610458E-7</v>
+        <v>9.1865363688934303E-7</v>
       </c>
       <c r="AE36">
         <f t="shared" si="21"/>
-        <v>3.4217876827308521E-7</v>
+        <v>3.408458625376852E-7</v>
       </c>
       <c r="AF36">
         <f t="shared" si="21"/>
-        <v>1.2674150981331357E-7</v>
+        <v>1.2624538586758636E-7</v>
       </c>
       <c r="AG36">
         <f t="shared" si="21"/>
-        <v>4.6880368971055735E-8</v>
+        <v>4.6695684211335232E-8</v>
       </c>
       <c r="AH36">
         <f t="shared" si="21"/>
-        <v>1.7321649920367821E-8</v>
+        <v>1.7252927106399014E-8</v>
       </c>
       <c r="AI36">
         <f t="shared" si="21"/>
-        <v>6.308854163722762E-9</v>
+        <v>6.2940841375389239E-9</v>
       </c>
     </row>
     <row r="37" spans="1:35">
@@ -3988,122 +4005,122 @@
       </c>
       <c r="B37" s="1">
         <f>SUMPRODUCT(lz,qa1_)</f>
-        <v>11.403971758770538</v>
+        <v>11.745740426975647</v>
       </c>
       <c r="G37" s="1">
         <f>SUM(dqa31_)</f>
-        <v>137.40849260405466</v>
+        <v>136.71146438910975</v>
       </c>
       <c r="H37" s="1">
         <f>SUM(dqa32_)</f>
-        <v>141.92146068486642</v>
+        <v>141.32829153256534</v>
       </c>
       <c r="I37" s="1">
         <f>SUM(dqa33_)</f>
-        <v>137.40849260406148</v>
+        <v>136.71146438911657</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K37">
         <f t="shared" ref="K37:AI37" si="22">flt3_*qa3_+lz*wa*flt3_^2/za*(sa-oa/za)</f>
-        <v>7.6046843012894936E-11</v>
+        <v>7.606561229163098E-11</v>
       </c>
       <c r="L37">
         <f t="shared" si="22"/>
-        <v>7.406620958394106E-8</v>
+        <v>7.4166411383356007E-8</v>
       </c>
       <c r="M37">
         <f t="shared" si="22"/>
-        <v>2.9428931498365567E-5</v>
+        <v>2.9571650374104112E-5</v>
       </c>
       <c r="N37">
         <f t="shared" si="22"/>
-        <v>7.3201566593543094E-3</v>
+        <v>7.3082888415232639E-3</v>
       </c>
       <c r="O37">
         <f t="shared" si="22"/>
-        <v>0.50412636455847637</v>
+        <v>0.49874737370371802</v>
       </c>
       <c r="P37">
         <f t="shared" si="22"/>
-        <v>2.3960659894762575</v>
+        <v>2.3634477273056191</v>
       </c>
       <c r="Q37">
         <f t="shared" si="22"/>
-        <v>3.5630682569196335</v>
+        <v>3.5192218888025741</v>
       </c>
       <c r="R37">
         <f t="shared" si="22"/>
-        <v>4.3637973900480027</v>
+        <v>4.3182727417528781</v>
       </c>
       <c r="S37">
         <f t="shared" si="22"/>
-        <v>5.0491855067433082</v>
+        <v>5.0049734831627619</v>
       </c>
       <c r="T37">
         <f t="shared" si="22"/>
-        <v>5.6454278537903679</v>
+        <v>5.603670154918067</v>
       </c>
       <c r="U37">
         <f t="shared" si="22"/>
-        <v>6.1565569056829519</v>
+        <v>6.117493124993957</v>
       </c>
       <c r="V37">
         <f t="shared" si="22"/>
-        <v>6.5884698005544067</v>
+        <v>6.551854707676366</v>
       </c>
       <c r="W37">
         <f t="shared" si="22"/>
-        <v>6.9492958745598514</v>
+        <v>6.9146657289436346</v>
       </c>
       <c r="X37">
         <f t="shared" si="22"/>
-        <v>7.2480526662468492</v>
+        <v>7.2148884173727144</v>
       </c>
       <c r="Y37">
         <f t="shared" si="22"/>
-        <v>7.4936861067749199</v>
+        <v>7.4615025453800534</v>
       </c>
       <c r="Z37">
         <f t="shared" si="22"/>
-        <v>7.6945234758923098</v>
+        <v>7.6629099322638501</v>
       </c>
       <c r="AA37">
         <f t="shared" si="22"/>
-        <v>7.8580094232575695</v>
+        <v>7.8266415648626619</v>
       </c>
       <c r="AB37">
         <f t="shared" si="22"/>
-        <v>7.9906192237875393</v>
+        <v>7.9592552890548491</v>
       </c>
       <c r="AC37">
         <f t="shared" si="22"/>
-        <v>8.0978759257291291</v>
+        <v>8.0663457653706914</v>
       </c>
       <c r="AD37">
         <f t="shared" si="22"/>
-        <v>8.18442319511378</v>
+        <v>8.1526149976363005</v>
       </c>
       <c r="AE37">
         <f t="shared" si="22"/>
-        <v>8.254123462604646</v>
+        <v>8.2219707707251022</v>
       </c>
       <c r="AF37">
         <f t="shared" si="22"/>
-        <v>8.3101630606320711</v>
+        <v>8.2776333007029823</v>
       </c>
       <c r="AG37">
         <f t="shared" si="22"/>
-        <v>8.3551539683607459</v>
+        <v>8.32223892018723</v>
       </c>
       <c r="AH37">
         <f t="shared" si="22"/>
-        <v>8.3912268209169678</v>
+        <v>8.3579350315992631</v>
       </c>
       <c r="AI37">
         <f t="shared" si="22"/>
-        <v>8.3072916726785966</v>
+        <v>8.2878429879669113</v>
       </c>
     </row>
     <row r="38" spans="1:35">
@@ -4112,7 +4129,7 @@
       </c>
       <c r="B38" s="1">
         <f>SUMPRODUCT(lz,qa2_)</f>
-        <v>3.5484911859250294</v>
+        <v>3.7046378693679896</v>
       </c>
       <c r="G38" t="s">
         <v>69</v>
@@ -4122,103 +4139,103 @@
       </c>
       <c r="K38">
         <f t="shared" ref="K38:AI38" si="23">flt1_*qa1_+lz*wa*flt2_*flt1_/za*(sa-oa/za)</f>
-        <v>-4.7606926709027299E-8</v>
+        <v>-4.7630744103785547E-8</v>
       </c>
       <c r="L38">
         <f t="shared" si="23"/>
-        <v>-1.9703841193112173E-5</v>
+        <v>-1.9786800198708514E-5</v>
       </c>
       <c r="M38">
         <f t="shared" si="23"/>
-        <v>-1.9262022199289192E-3</v>
+        <v>-1.9648280948683576E-3</v>
       </c>
       <c r="N38">
         <f t="shared" si="23"/>
-        <v>-2.5561847199012975E-2</v>
+        <v>-2.6973682461303914E-2</v>
       </c>
       <c r="O38">
         <f t="shared" si="23"/>
-        <v>0.47307835373947793</v>
+        <v>0.46589044977590599</v>
       </c>
       <c r="P38">
         <f t="shared" si="23"/>
-        <v>2.7230361087979573</v>
+        <v>2.7110243001172756</v>
       </c>
       <c r="Q38">
         <f t="shared" si="23"/>
-        <v>4.0383310001771173</v>
+        <v>4.0236017421319383</v>
       </c>
       <c r="R38">
         <f t="shared" si="23"/>
-        <v>4.8647696507974993</v>
+        <v>4.8474844141317206</v>
       </c>
       <c r="S38">
         <f t="shared" si="23"/>
-        <v>5.5305286826307247</v>
+        <v>5.5102576572866599</v>
       </c>
       <c r="T38">
         <f t="shared" si="23"/>
-        <v>6.0851584911777588</v>
+        <v>6.0619145383255244</v>
       </c>
       <c r="U38">
         <f t="shared" si="23"/>
-        <v>6.5452963793789767</v>
+        <v>6.519408778197703</v>
       </c>
       <c r="V38">
         <f t="shared" si="23"/>
-        <v>6.9244436727479801</v>
+        <v>6.8963535683228692</v>
       </c>
       <c r="W38">
         <f t="shared" si="23"/>
-        <v>7.2350325928987802</v>
+        <v>7.2051732906077728</v>
       </c>
       <c r="X38">
         <f t="shared" si="23"/>
-        <v>7.4882362397597193</v>
+        <v>7.456982993820449</v>
       </c>
       <c r="Y38">
         <f t="shared" si="23"/>
-        <v>7.6938353507511783</v>
+        <v>7.6614935659304839</v>
       </c>
       <c r="Z38">
         <f t="shared" si="23"/>
-        <v>7.8602271324102384</v>
+        <v>7.8270376285618246</v>
       </c>
       <c r="AA38">
         <f t="shared" si="23"/>
-        <v>7.9945162251867012</v>
+        <v>7.9606660918888119</v>
       </c>
       <c r="AB38">
         <f t="shared" si="23"/>
-        <v>8.102645350179321</v>
+        <v>8.0682791742265394</v>
       </c>
       <c r="AC38">
         <f t="shared" si="23"/>
-        <v>8.1895402597731035</v>
+        <v>8.1547698014151457</v>
       </c>
       <c r="AD38">
         <f t="shared" si="23"/>
-        <v>8.2592539791355222</v>
+        <v>8.2241658843938357</v>
       </c>
       <c r="AE38">
         <f t="shared" si="23"/>
-        <v>8.3151018005728083</v>
+        <v>8.2797635268315481</v>
       </c>
       <c r="AF38">
         <f t="shared" si="23"/>
-        <v>8.3597826867947767</v>
+        <v>8.3242469847252476</v>
       </c>
       <c r="AG38">
         <f t="shared" si="23"/>
-        <v>8.395485440749658</v>
+        <v>8.3597937308155608</v>
       </c>
       <c r="AH38">
         <f t="shared" si="23"/>
-        <v>8.4239796696328746</v>
+        <v>8.3881645923889732</v>
       </c>
       <c r="AI38">
         <f t="shared" si="23"/>
-        <v>8.4466894184832295</v>
+        <v>8.4107771636989721</v>
       </c>
     </row>
     <row r="39" spans="1:35">
@@ -4227,239 +4244,239 @@
       </c>
       <c r="B39" s="1">
         <f>SUMPRODUCT(lz,qa3_)</f>
-        <v>11.403971760118671</v>
+        <v>11.745740428325337</v>
       </c>
       <c r="G39" s="1">
         <f>re*phi_q1+f1_*phi_q1*$H31+f1_*re*G35</f>
-        <v>104.65857013892038</v>
+        <v>110.26056183089537</v>
       </c>
       <c r="H39" s="1">
         <f>re*phi_q1+f1_*phi_q1*$H32+f1_*re*H35</f>
-        <v>109.99756890612824</v>
+        <v>116.38652537399793</v>
       </c>
       <c r="I39" s="1">
         <f>re*phi_q1+f1_*phi_q1*$H33+f1_*re*I35</f>
-        <v>104.65857012830291</v>
+        <v>110.26056181856346</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>66</v>
       </c>
       <c r="K39">
         <f t="shared" ref="K39:AI39" si="24">flt1_*qa1_+lz*wa*flt3_*flt1_/za*(sa-oa/za)</f>
-        <v>7.5965138807048583E-11</v>
+        <v>7.5983881259288646E-11</v>
       </c>
       <c r="L39">
         <f t="shared" si="24"/>
-        <v>7.4066077868985193E-8</v>
+        <v>7.4166279391195771E-8</v>
       </c>
       <c r="M39">
         <f t="shared" si="24"/>
-        <v>2.9428931183872598E-5</v>
+        <v>2.9571650057079199E-5</v>
       </c>
       <c r="N39">
         <f t="shared" si="24"/>
-        <v>7.3201566580431889E-3</v>
+        <v>7.3082888402045774E-3</v>
       </c>
       <c r="O39">
         <f t="shared" si="24"/>
-        <v>0.50412636455501747</v>
+        <v>0.49874737370026512</v>
       </c>
       <c r="P39">
         <f t="shared" si="24"/>
-        <v>2.3960659894750398</v>
+        <v>2.3634477273044086</v>
       </c>
       <c r="Q39">
         <f t="shared" si="24"/>
-        <v>3.5630682569194061</v>
+        <v>3.5192218888023499</v>
       </c>
       <c r="R39">
         <f t="shared" si="24"/>
-        <v>4.3637973900479485</v>
+        <v>4.3182727417528239</v>
       </c>
       <c r="S39">
         <f t="shared" si="24"/>
-        <v>5.0491855067432914</v>
+        <v>5.004973483162745</v>
       </c>
       <c r="T39">
         <f t="shared" si="24"/>
-        <v>5.6454278537903626</v>
+        <v>5.603670154918059</v>
       </c>
       <c r="U39">
         <f t="shared" si="24"/>
-        <v>6.1565569056829492</v>
+        <v>6.1174931249939553</v>
       </c>
       <c r="V39">
         <f t="shared" si="24"/>
-        <v>6.5884698005544049</v>
+        <v>6.5518547076763616</v>
       </c>
       <c r="W39">
         <f t="shared" si="24"/>
-        <v>6.9492958745598514</v>
+        <v>6.9146657289436346</v>
       </c>
       <c r="X39">
         <f t="shared" si="24"/>
-        <v>7.2480526662468492</v>
+        <v>7.2148884173727144</v>
       </c>
       <c r="Y39">
         <f t="shared" si="24"/>
-        <v>7.4936861067749199</v>
+        <v>7.4615025453800534</v>
       </c>
       <c r="Z39">
         <f t="shared" si="24"/>
-        <v>7.6945234758923098</v>
+        <v>7.6629099322638501</v>
       </c>
       <c r="AA39">
         <f t="shared" si="24"/>
-        <v>7.8580094232575695</v>
+        <v>7.8266415648626619</v>
       </c>
       <c r="AB39">
         <f t="shared" si="24"/>
-        <v>7.9906192237875393</v>
+        <v>7.9592552890548491</v>
       </c>
       <c r="AC39">
         <f t="shared" si="24"/>
-        <v>8.0978759257291291</v>
+        <v>8.0663457653706914</v>
       </c>
       <c r="AD39">
         <f t="shared" si="24"/>
-        <v>8.18442319511378</v>
+        <v>8.1526149976363005</v>
       </c>
       <c r="AE39">
         <f t="shared" si="24"/>
-        <v>8.254123462604646</v>
+        <v>8.2219707707251022</v>
       </c>
       <c r="AF39">
         <f t="shared" si="24"/>
-        <v>8.3101630606320711</v>
+        <v>8.2776333007029823</v>
       </c>
       <c r="AG39">
         <f t="shared" si="24"/>
-        <v>8.3551539683607459</v>
+        <v>8.32223892018723</v>
       </c>
       <c r="AH39">
         <f t="shared" si="24"/>
-        <v>8.3912268209169678</v>
+        <v>8.3579350315992631</v>
       </c>
       <c r="AI39">
         <f t="shared" si="24"/>
-        <v>8.3072916726785966</v>
+        <v>8.2878429879669113</v>
       </c>
     </row>
     <row r="40" spans="1:35">
       <c r="G40" s="1">
         <f>re*phi_q1+f1_*phi_q1*$H32+f1_*re*G36</f>
-        <v>109.99756890612824</v>
+        <v>116.38652537399793</v>
       </c>
       <c r="H40" s="1">
         <f>re*phi_q2+f2_*phi_q2*$H32+f2_*re*H36</f>
-        <v>25.124605857598642</v>
+        <v>26.260926189133844</v>
       </c>
       <c r="I40" s="1">
         <f>re*phi_q3+f3_*phi_q3*$H33+f3_*re*I36</f>
-        <v>105.64780902756542</v>
+        <v>111.41873308685707</v>
       </c>
       <c r="J40" s="8" t="s">
         <v>65</v>
       </c>
       <c r="K40">
         <f t="shared" ref="K40:AI40" si="25">flt1_*qa1_+lz*wa*flt1_*flt2_/za*(sa-oa/za)</f>
-        <v>-4.7606926709027292E-8</v>
+        <v>-4.763074410378554E-8</v>
       </c>
       <c r="L40">
         <f t="shared" si="25"/>
-        <v>-1.9703841193112177E-5</v>
+        <v>-1.9786800198708514E-5</v>
       </c>
       <c r="M40">
         <f t="shared" si="25"/>
-        <v>-1.9262022199289187E-3</v>
+        <v>-1.9648280948683576E-3</v>
       </c>
       <c r="N40">
         <f t="shared" si="25"/>
-        <v>-2.5561847199012975E-2</v>
+        <v>-2.6973682461303914E-2</v>
       </c>
       <c r="O40">
         <f t="shared" si="25"/>
-        <v>0.47307835373947793</v>
+        <v>0.46589044977590599</v>
       </c>
       <c r="P40">
         <f t="shared" si="25"/>
-        <v>2.7230361087979573</v>
+        <v>2.7110243001172756</v>
       </c>
       <c r="Q40">
         <f t="shared" si="25"/>
-        <v>4.0383310001771173</v>
+        <v>4.0236017421319383</v>
       </c>
       <c r="R40">
         <f t="shared" si="25"/>
-        <v>4.8647696507974993</v>
+        <v>4.8474844141317206</v>
       </c>
       <c r="S40">
         <f t="shared" si="25"/>
-        <v>5.5305286826307247</v>
+        <v>5.5102576572866599</v>
       </c>
       <c r="T40">
         <f t="shared" si="25"/>
-        <v>6.0851584911777588</v>
+        <v>6.0619145383255244</v>
       </c>
       <c r="U40">
         <f t="shared" si="25"/>
-        <v>6.5452963793789767</v>
+        <v>6.519408778197703</v>
       </c>
       <c r="V40">
         <f t="shared" si="25"/>
-        <v>6.9244436727479801</v>
+        <v>6.8963535683228692</v>
       </c>
       <c r="W40">
         <f t="shared" si="25"/>
-        <v>7.2350325928987802</v>
+        <v>7.2051732906077728</v>
       </c>
       <c r="X40">
         <f t="shared" si="25"/>
-        <v>7.4882362397597193</v>
+        <v>7.456982993820449</v>
       </c>
       <c r="Y40">
         <f t="shared" si="25"/>
-        <v>7.6938353507511783</v>
+        <v>7.6614935659304839</v>
       </c>
       <c r="Z40">
         <f t="shared" si="25"/>
-        <v>7.8602271324102384</v>
+        <v>7.8270376285618246</v>
       </c>
       <c r="AA40">
         <f t="shared" si="25"/>
-        <v>7.9945162251867012</v>
+        <v>7.9606660918888119</v>
       </c>
       <c r="AB40">
         <f t="shared" si="25"/>
-        <v>8.102645350179321</v>
+        <v>8.0682791742265394</v>
       </c>
       <c r="AC40">
         <f t="shared" si="25"/>
-        <v>8.1895402597731035</v>
+        <v>8.1547698014151457</v>
       </c>
       <c r="AD40">
         <f t="shared" si="25"/>
-        <v>8.2592539791355222</v>
+        <v>8.2241658843938357</v>
       </c>
       <c r="AE40">
         <f t="shared" si="25"/>
-        <v>8.3151018005728083</v>
+        <v>8.2797635268315481</v>
       </c>
       <c r="AF40">
         <f t="shared" si="25"/>
-        <v>8.3597826867947767</v>
+        <v>8.3242469847252476</v>
       </c>
       <c r="AG40">
         <f t="shared" si="25"/>
-        <v>8.395485440749658</v>
+        <v>8.3597937308155608</v>
       </c>
       <c r="AH40">
         <f t="shared" si="25"/>
-        <v>8.4239796696328746</v>
+        <v>8.3881645923889732</v>
       </c>
       <c r="AI40">
         <f t="shared" si="25"/>
-        <v>8.4466894184832295</v>
+        <v>8.4107771636989721</v>
       </c>
     </row>
     <row r="41" spans="1:35">
@@ -4470,118 +4487,118 @@
       <c r="C41" s="16"/>
       <c r="G41" s="1">
         <f>re*phi_q1+f1_*phi_q1*$H33+f1_*re*G37</f>
-        <v>104.65857012830291</v>
+        <v>110.26056181856346</v>
       </c>
       <c r="H41" s="1">
         <f>re*phi_q3+f3_*phi_q3*$H33+f3_*re*H37</f>
-        <v>105.64780902756542</v>
+        <v>111.41873308685707</v>
       </c>
       <c r="I41" s="1">
         <f>re*phi_q3+f1_*phi_q3*$H33+f3_*re*I37</f>
-        <v>104.65857074079418</v>
+        <v>110.26159630277692</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>67</v>
       </c>
       <c r="K41">
         <f t="shared" ref="K41:AI41" si="26">flt1_*qa1_+lz*wa*flt3_*flt2_/za*(sa-oa/za)</f>
-        <v>-4.7624326110532381E-8</v>
+        <v>-4.7648152203054232E-8</v>
       </c>
       <c r="L41">
         <f t="shared" si="26"/>
-        <v>-1.9703854170076816E-5</v>
+        <v>-1.9786813230171155E-5</v>
       </c>
       <c r="M41">
         <f t="shared" si="26"/>
-        <v>-1.9262022282117393E-3</v>
+        <v>-1.964828103315378E-3</v>
       </c>
       <c r="N41">
         <f t="shared" si="26"/>
-        <v>-2.5561847201684567E-2</v>
+        <v>-2.6973682464089255E-2</v>
       </c>
       <c r="O41">
         <f t="shared" si="26"/>
-        <v>0.47307835373893414</v>
+        <v>0.46589044977533051</v>
       </c>
       <c r="P41">
         <f t="shared" si="26"/>
-        <v>2.723036108797908</v>
+        <v>2.7110243001172232</v>
       </c>
       <c r="Q41">
         <f t="shared" si="26"/>
-        <v>4.0383310001771138</v>
+        <v>4.0236017421319339</v>
       </c>
       <c r="R41">
         <f t="shared" si="26"/>
-        <v>4.8647696507974985</v>
+        <v>4.8474844141317206</v>
       </c>
       <c r="S41">
         <f t="shared" si="26"/>
-        <v>5.5305286826307247</v>
+        <v>5.5102576572866591</v>
       </c>
       <c r="T41">
         <f t="shared" si="26"/>
-        <v>6.0851584911777588</v>
+        <v>6.0619145383255244</v>
       </c>
       <c r="U41">
         <f t="shared" si="26"/>
-        <v>6.5452963793789767</v>
+        <v>6.519408778197703</v>
       </c>
       <c r="V41">
         <f t="shared" si="26"/>
-        <v>6.9244436727479801</v>
+        <v>6.8963535683228692</v>
       </c>
       <c r="W41">
         <f t="shared" si="26"/>
-        <v>7.2350325928987802</v>
+        <v>7.2051732906077728</v>
       </c>
       <c r="X41">
         <f t="shared" si="26"/>
-        <v>7.4882362397597193</v>
+        <v>7.456982993820449</v>
       </c>
       <c r="Y41">
         <f t="shared" si="26"/>
-        <v>7.6938353507511783</v>
+        <v>7.6614935659304839</v>
       </c>
       <c r="Z41">
         <f t="shared" si="26"/>
-        <v>7.8602271324102384</v>
+        <v>7.8270376285618246</v>
       </c>
       <c r="AA41">
         <f t="shared" si="26"/>
-        <v>7.9945162251867012</v>
+        <v>7.9606660918888119</v>
       </c>
       <c r="AB41">
         <f t="shared" si="26"/>
-        <v>8.102645350179321</v>
+        <v>8.0682791742265394</v>
       </c>
       <c r="AC41">
         <f t="shared" si="26"/>
-        <v>8.1895402597731035</v>
+        <v>8.1547698014151457</v>
       </c>
       <c r="AD41">
         <f t="shared" si="26"/>
-        <v>8.2592539791355222</v>
+        <v>8.2241658843938357</v>
       </c>
       <c r="AE41">
         <f t="shared" si="26"/>
-        <v>8.3151018005728083</v>
+        <v>8.2797635268315481</v>
       </c>
       <c r="AF41">
         <f t="shared" si="26"/>
-        <v>8.3597826867947767</v>
+        <v>8.3242469847252476</v>
       </c>
       <c r="AG41">
         <f t="shared" si="26"/>
-        <v>8.395485440749658</v>
+        <v>8.3597937308155608</v>
       </c>
       <c r="AH41">
         <f t="shared" si="26"/>
-        <v>8.4239796696328746</v>
+        <v>8.3881645923889732</v>
       </c>
       <c r="AI41">
         <f t="shared" si="26"/>
-        <v>8.4466894184832295</v>
+        <v>8.4107771636989721</v>
       </c>
     </row>
     <row r="42" spans="1:35">
@@ -4590,110 +4607,110 @@
       </c>
       <c r="B42" s="1">
         <f>phif/phie</f>
-        <v>0.39999855522103445</v>
+        <v>0.40000071794109937</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>68</v>
       </c>
       <c r="K42">
         <f t="shared" ref="K42:AI42" si="27">flt1_*qa1_+lz*wa*flt1_*flt3_/za*(sa-oa/za)</f>
-        <v>7.5965138807048583E-11</v>
+        <v>7.5983881259288646E-11</v>
       </c>
       <c r="L42">
         <f t="shared" si="27"/>
-        <v>7.4066077868985193E-8</v>
+        <v>7.4166279391195771E-8</v>
       </c>
       <c r="M42">
         <f t="shared" si="27"/>
-        <v>2.9428931183872598E-5</v>
+        <v>2.9571650057079199E-5</v>
       </c>
       <c r="N42">
         <f t="shared" si="27"/>
-        <v>7.3201566580431889E-3</v>
+        <v>7.3082888402045774E-3</v>
       </c>
       <c r="O42">
         <f t="shared" si="27"/>
-        <v>0.50412636455501747</v>
+        <v>0.49874737370026512</v>
       </c>
       <c r="P42">
         <f t="shared" si="27"/>
-        <v>2.3960659894750398</v>
+        <v>2.3634477273044086</v>
       </c>
       <c r="Q42">
         <f t="shared" si="27"/>
-        <v>3.5630682569194061</v>
+        <v>3.5192218888023499</v>
       </c>
       <c r="R42">
         <f t="shared" si="27"/>
-        <v>4.3637973900479485</v>
+        <v>4.3182727417528239</v>
       </c>
       <c r="S42">
         <f t="shared" si="27"/>
-        <v>5.0491855067432914</v>
+        <v>5.004973483162745</v>
       </c>
       <c r="T42">
         <f t="shared" si="27"/>
-        <v>5.6454278537903626</v>
+        <v>5.603670154918059</v>
       </c>
       <c r="U42">
         <f t="shared" si="27"/>
-        <v>6.1565569056829492</v>
+        <v>6.1174931249939553</v>
       </c>
       <c r="V42">
         <f t="shared" si="27"/>
-        <v>6.5884698005544049</v>
+        <v>6.5518547076763616</v>
       </c>
       <c r="W42">
         <f t="shared" si="27"/>
-        <v>6.9492958745598514</v>
+        <v>6.9146657289436346</v>
       </c>
       <c r="X42">
         <f t="shared" si="27"/>
-        <v>7.2480526662468492</v>
+        <v>7.2148884173727144</v>
       </c>
       <c r="Y42">
         <f t="shared" si="27"/>
-        <v>7.4936861067749199</v>
+        <v>7.4615025453800534</v>
       </c>
       <c r="Z42">
         <f t="shared" si="27"/>
-        <v>7.6945234758923098</v>
+        <v>7.6629099322638501</v>
       </c>
       <c r="AA42">
         <f t="shared" si="27"/>
-        <v>7.8580094232575695</v>
+        <v>7.8266415648626619</v>
       </c>
       <c r="AB42">
         <f t="shared" si="27"/>
-        <v>7.9906192237875393</v>
+        <v>7.9592552890548491</v>
       </c>
       <c r="AC42">
         <f t="shared" si="27"/>
-        <v>8.0978759257291291</v>
+        <v>8.0663457653706914</v>
       </c>
       <c r="AD42">
         <f t="shared" si="27"/>
-        <v>8.18442319511378</v>
+        <v>8.1526149976363005</v>
       </c>
       <c r="AE42">
         <f t="shared" si="27"/>
-        <v>8.254123462604646</v>
+        <v>8.2219707707251022</v>
       </c>
       <c r="AF42">
         <f t="shared" si="27"/>
-        <v>8.3101630606320711</v>
+        <v>8.2776333007029823</v>
       </c>
       <c r="AG42">
         <f t="shared" si="27"/>
-        <v>8.3551539683607459</v>
+        <v>8.32223892018723</v>
       </c>
       <c r="AH42">
         <f t="shared" si="27"/>
-        <v>8.3912268209169678</v>
+        <v>8.3579350315992631</v>
       </c>
       <c r="AI42">
         <f t="shared" si="27"/>
-        <v>8.3072916726785966</v>
+        <v>8.2878429879669113</v>
       </c>
     </row>
     <row r="43" spans="1:35">
@@ -4702,110 +4719,110 @@
       </c>
       <c r="B43" s="11">
         <f>MAX(0,Ro*(reck-1/spr)/(reck-1))</f>
-        <v>7.1196976633991707</v>
+        <v>7.1197077936331228</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K43">
         <f t="shared" ref="K43:AI43" si="28">flt1_*qa1_+lz*wa*flt2_*flt3_/za*(sa-oa/za)</f>
-        <v>-4.7624326110532381E-8</v>
+        <v>-4.7648152203054232E-8</v>
       </c>
       <c r="L43">
         <f t="shared" si="28"/>
-        <v>-1.9703854170076816E-5</v>
+        <v>-1.9786813230171155E-5</v>
       </c>
       <c r="M43">
         <f t="shared" si="28"/>
-        <v>-1.9262022282117402E-3</v>
+        <v>-1.964828103315378E-3</v>
       </c>
       <c r="N43">
         <f t="shared" si="28"/>
-        <v>-2.556184720168456E-2</v>
+        <v>-2.6973682464089255E-2</v>
       </c>
       <c r="O43">
         <f t="shared" si="28"/>
-        <v>0.47307835373893414</v>
+        <v>0.46589044977533051</v>
       </c>
       <c r="P43">
         <f t="shared" si="28"/>
-        <v>2.723036108797908</v>
+        <v>2.7110243001172232</v>
       </c>
       <c r="Q43">
         <f t="shared" si="28"/>
-        <v>4.0383310001771138</v>
+        <v>4.0236017421319339</v>
       </c>
       <c r="R43">
         <f t="shared" si="28"/>
-        <v>4.8647696507974985</v>
+        <v>4.8474844141317206</v>
       </c>
       <c r="S43">
         <f t="shared" si="28"/>
-        <v>5.5305286826307247</v>
+        <v>5.5102576572866591</v>
       </c>
       <c r="T43">
         <f t="shared" si="28"/>
-        <v>6.0851584911777588</v>
+        <v>6.0619145383255244</v>
       </c>
       <c r="U43">
         <f t="shared" si="28"/>
-        <v>6.5452963793789767</v>
+        <v>6.519408778197703</v>
       </c>
       <c r="V43">
         <f t="shared" si="28"/>
-        <v>6.9244436727479801</v>
+        <v>6.8963535683228692</v>
       </c>
       <c r="W43">
         <f t="shared" si="28"/>
-        <v>7.2350325928987802</v>
+        <v>7.2051732906077728</v>
       </c>
       <c r="X43">
         <f t="shared" si="28"/>
-        <v>7.4882362397597193</v>
+        <v>7.456982993820449</v>
       </c>
       <c r="Y43">
         <f t="shared" si="28"/>
-        <v>7.6938353507511783</v>
+        <v>7.6614935659304839</v>
       </c>
       <c r="Z43">
         <f t="shared" si="28"/>
-        <v>7.8602271324102384</v>
+        <v>7.8270376285618246</v>
       </c>
       <c r="AA43">
         <f t="shared" si="28"/>
-        <v>7.9945162251867012</v>
+        <v>7.9606660918888119</v>
       </c>
       <c r="AB43">
         <f t="shared" si="28"/>
-        <v>8.102645350179321</v>
+        <v>8.0682791742265394</v>
       </c>
       <c r="AC43">
         <f t="shared" si="28"/>
-        <v>8.1895402597731035</v>
+        <v>8.1547698014151457</v>
       </c>
       <c r="AD43">
         <f t="shared" si="28"/>
-        <v>8.2592539791355222</v>
+        <v>8.2241658843938357</v>
       </c>
       <c r="AE43">
         <f t="shared" si="28"/>
-        <v>8.3151018005728083</v>
+        <v>8.2797635268315481</v>
       </c>
       <c r="AF43">
         <f t="shared" si="28"/>
-        <v>8.3597826867947767</v>
+        <v>8.3242469847252476</v>
       </c>
       <c r="AG43">
         <f t="shared" si="28"/>
-        <v>8.395485440749658</v>
+        <v>8.3597937308155608</v>
       </c>
       <c r="AH43">
         <f t="shared" si="28"/>
-        <v>8.4239796696328746</v>
+        <v>8.3881645923889732</v>
       </c>
       <c r="AI43">
         <f t="shared" si="28"/>
-        <v>8.4466894184832295</v>
+        <v>8.4107771636989721</v>
       </c>
     </row>
     <row r="44" spans="1:35">
@@ -4814,11 +4831,11 @@
       </c>
       <c r="B44" s="1">
         <f>f1_*re*phi_q1</f>
-        <v>2.4997399888109619</v>
+        <v>2.9443869019615287</v>
       </c>
       <c r="C44" s="20">
         <f>ye_1/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.37525792595872431</v>
+        <v>0.4232805123398507</v>
       </c>
     </row>
     <row r="45" spans="1:35">
@@ -4827,14 +4844,14 @@
       </c>
       <c r="B45" s="1">
         <f>f2_*re*phi_q2</f>
-        <v>1.6619115533171394</v>
+        <v>1.0672499097516894</v>
       </c>
       <c r="C45" s="20">
         <f>ye_2/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.24948414051706141</v>
+        <v>0.15342619826674431</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:35" ht="19" thickBot="1">
@@ -4843,11 +4860,11 @@
       </c>
       <c r="B46" s="1">
         <f>f3_*re*phi_q3</f>
-        <v>2.4997400392076532</v>
+        <v>2.9444757805846495</v>
       </c>
       <c r="C46" s="20">
         <f>ye_3/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.37525793352421427</v>
+        <v>0.42329328939340488</v>
       </c>
       <c r="G46" s="32" t="s">
         <v>70</v>
@@ -4859,103 +4876,103 @@
       </c>
       <c r="K46">
         <f t="shared" ref="K46:AI46" si="29">lz*qa1_</f>
-        <v>3.2655808350543217E-6</v>
+        <v>3.2667895782250959E-6</v>
       </c>
       <c r="L46">
         <f t="shared" si="29"/>
-        <v>1.9765385080548794E-4</v>
+        <v>1.9830685531339992E-4</v>
       </c>
       <c r="M46">
         <f t="shared" si="29"/>
-        <v>4.9502396798161152E-3</v>
+        <v>5.0303359246510471E-3</v>
       </c>
       <c r="N46">
         <f t="shared" si="29"/>
-        <v>8.0377517435329546E-2</v>
+        <v>8.3472232294431778E-2</v>
       </c>
       <c r="O46">
         <f t="shared" si="29"/>
-        <v>0.62797573641643889</v>
+        <v>0.66332183097283803</v>
       </c>
       <c r="P46">
         <f t="shared" si="29"/>
-        <v>1.2223234458721</v>
+        <v>1.2991013849339932</v>
       </c>
       <c r="Q46">
         <f t="shared" si="29"/>
-        <v>1.282404127206594</v>
+        <v>1.3617080550460643</v>
       </c>
       <c r="R46">
         <f t="shared" si="29"/>
-        <v>1.203703366173996</v>
+        <v>1.2727438014037058</v>
       </c>
       <c r="S46">
         <f t="shared" si="29"/>
-        <v>1.0881556990873975</v>
+        <v>1.1436126364169148</v>
       </c>
       <c r="T46">
         <f t="shared" si="29"/>
-        <v>0.95991092469231665</v>
+        <v>1.0016351835143371</v>
       </c>
       <c r="U46">
         <f t="shared" si="29"/>
-        <v>0.83128455095021225</v>
+        <v>0.86065931313945654</v>
       </c>
       <c r="V46">
         <f t="shared" si="29"/>
-        <v>0.70967255114358918</v>
+        <v>0.7287323518508827</v>
       </c>
       <c r="W46">
         <f t="shared" si="29"/>
-        <v>0.59912285993210612</v>
+        <v>0.61002643916074317</v>
       </c>
       <c r="X46">
         <f t="shared" si="29"/>
-        <v>0.5013789306139792</v>
+        <v>0.50612462876630904</v>
       </c>
       <c r="Y46">
         <f t="shared" si="29"/>
-        <v>0.41669300985110957</v>
+        <v>0.4169916809889424</v>
       </c>
       <c r="Z46">
         <f t="shared" si="29"/>
-        <v>0.34442619628296045</v>
+        <v>0.34166745780758895</v>
       </c>
       <c r="AA46">
         <f t="shared" si="29"/>
-        <v>0.28346515214127155</v>
+        <v>0.27873349161480548</v>
       </c>
       <c r="AB46">
         <f t="shared" si="29"/>
-        <v>0.23249583222769699</v>
+        <v>0.22660949204669933</v>
       </c>
       <c r="AC46">
         <f t="shared" si="29"/>
-        <v>0.19017314505483437</v>
+        <v>0.18373013222111853</v>
       </c>
       <c r="AD46">
         <f t="shared" si="29"/>
-        <v>0.15521874124846763</v>
+        <v>0.14864165408335045</v>
       </c>
       <c r="AE46">
         <f t="shared" si="29"/>
-        <v>0.12647135210203886</v>
+        <v>0.12004715305378347</v>
       </c>
       <c r="AF46">
         <f t="shared" si="29"/>
-        <v>0.10290716582301095</v>
+        <v>9.6820556029183269E-2</v>
       </c>
       <c r="AG46">
         <f t="shared" si="29"/>
-        <v>8.3642230372726056E-2</v>
+        <v>7.8002620743326909E-2</v>
       </c>
       <c r="AH46">
         <f t="shared" si="29"/>
-        <v>6.792480554352695E-2</v>
+        <v>6.2787514438517655E-2</v>
       </c>
       <c r="AI46">
         <f t="shared" si="29"/>
-        <v>0.28909325948738285</v>
+        <v>0.25533890687910993</v>
       </c>
     </row>
     <row r="47" spans="1:35" ht="19" thickTop="1">
@@ -4964,332 +4981,338 @@
       </c>
       <c r="B47" s="1">
         <f>SUM(B44:B46)</f>
-        <v>6.6613915813357547</v>
+        <v>6.9561125922978686</v>
       </c>
       <c r="F47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G47" s="31">
         <f>G39/G53</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="H47" s="31">
-        <f t="shared" ref="H47:I47" si="30">H39/H53</f>
-        <v>2.1450926732367432</v>
+        <f>H53/H39</f>
+        <v>0.46234100977901238</v>
       </c>
       <c r="I47" s="31">
-        <f t="shared" si="30"/>
-        <v>0.99999999702313569</v>
+        <f>I53/I39</f>
+        <v>1.0000046911339013</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>77</v>
       </c>
       <c r="K47">
-        <f t="shared" ref="K47:AI47" si="31">lz*qa2_</f>
-        <v>2.1588031906815412E-3</v>
+        <f t="shared" ref="K47:AI47" si="30">lz*qa2_</f>
+        <v>2.159602264030384E-3</v>
       </c>
       <c r="L47">
-        <f t="shared" si="31"/>
-        <v>7.3746101987390955E-2</v>
+        <f t="shared" si="30"/>
+        <v>7.3989742760603577E-2</v>
       </c>
       <c r="M47">
-        <f t="shared" si="31"/>
-        <v>0.60986124375423811</v>
+        <f t="shared" si="30"/>
+        <v>0.61972896706756475</v>
       </c>
       <c r="N47">
-        <f t="shared" si="31"/>
-        <v>0.97944569823551419</v>
+        <f t="shared" si="30"/>
+        <v>1.0171565563551617</v>
       </c>
       <c r="O47">
-        <f t="shared" si="31"/>
-        <v>0.75688449243930345</v>
+        <f t="shared" si="30"/>
+        <v>0.79948631490890709</v>
       </c>
       <c r="P47">
-        <f t="shared" si="31"/>
-        <v>0.48645669656270074</v>
+        <f t="shared" si="30"/>
+        <v>0.51701255535038293</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="31"/>
-        <v>0.28815227226670354</v>
+        <f t="shared" si="30"/>
+        <v>0.30597162150444701</v>
       </c>
       <c r="R47">
-        <f t="shared" si="31"/>
-        <v>0.16305045961112605</v>
+        <f t="shared" si="30"/>
+        <v>0.17240249351939474</v>
       </c>
       <c r="S47">
-        <f t="shared" si="31"/>
-        <v>8.9358995199419353E-2</v>
+        <f t="shared" si="30"/>
+        <v>9.3913101014202041E-2</v>
       </c>
       <c r="T47">
-        <f t="shared" si="31"/>
-        <v>4.781055778387059E-2</v>
+        <f t="shared" si="30"/>
+        <v>4.9888729868471884E-2</v>
       </c>
       <c r="U47">
-        <f t="shared" si="31"/>
-        <v>2.5113354447076384E-2</v>
+        <f t="shared" si="30"/>
+        <v>2.6000774782043309E-2</v>
       </c>
       <c r="V47">
-        <f t="shared" si="31"/>
-        <v>1.3003986799805528E-2</v>
+        <f t="shared" si="30"/>
+        <v>1.3353237163801107E-2</v>
       </c>
       <c r="W47">
-        <f t="shared" si="31"/>
-        <v>6.6588312546662096E-3</v>
+        <f t="shared" si="30"/>
+        <v>6.7800169062429234E-3</v>
       </c>
       <c r="X47">
-        <f t="shared" si="31"/>
-        <v>3.3799619709382936E-3</v>
+        <f t="shared" si="30"/>
+        <v>3.4119542990977249E-3</v>
       </c>
       <c r="Y47">
-        <f t="shared" si="31"/>
-        <v>1.7038272729331205E-3</v>
+        <f t="shared" si="30"/>
+        <v>1.7050485173942631E-3</v>
       </c>
       <c r="Z47">
-        <f t="shared" si="31"/>
-        <v>8.5421883370293472E-4</v>
+        <f t="shared" si="30"/>
+        <v>8.4737682694399673E-4</v>
       </c>
       <c r="AA47">
-        <f t="shared" si="31"/>
-        <v>4.264187176396412E-4</v>
+        <f t="shared" si="30"/>
+        <v>4.1930084583508085E-4</v>
       </c>
       <c r="AB47">
-        <f t="shared" si="31"/>
-        <v>2.1213648660941927E-4</v>
+        <f t="shared" si="30"/>
+        <v>2.0676560527782718E-4</v>
       </c>
       <c r="AC47">
-        <f t="shared" si="31"/>
-        <v>1.0524779479389867E-4</v>
+        <f t="shared" si="30"/>
+        <v>1.0168202901565561E-4</v>
       </c>
       <c r="AD47">
-        <f t="shared" si="31"/>
-        <v>5.2104062941527744E-5</v>
+        <f t="shared" si="30"/>
+        <v>4.989625632702485E-5</v>
       </c>
       <c r="AE47">
-        <f t="shared" si="31"/>
-        <v>2.5750354403030386E-5</v>
+        <f t="shared" si="30"/>
+        <v>2.4442347494756654E-5</v>
       </c>
       <c r="AF47">
-        <f t="shared" si="31"/>
-        <v>1.2708675270626672E-5</v>
+        <f t="shared" si="30"/>
+        <v>1.1957000236627482E-5</v>
       </c>
       <c r="AG47">
-        <f t="shared" si="31"/>
-        <v>6.2653290809821656E-6</v>
+        <f t="shared" si="30"/>
+        <v>5.8428868522299395E-6</v>
       </c>
       <c r="AH47">
-        <f t="shared" si="31"/>
-        <v>3.0861021849271816E-6</v>
+        <f t="shared" si="30"/>
+        <v>2.8526940039701282E-6</v>
       </c>
       <c r="AI47">
-        <f t="shared" si="31"/>
-        <v>7.9667920334411347E-6</v>
+        <f t="shared" si="30"/>
+        <v>7.0365942559820988E-6</v>
       </c>
     </row>
     <row r="48" spans="1:35">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="F48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G48" s="31">
         <f>G40/G54</f>
-        <v>2.1450926732367432</v>
+        <v>2.162905688331596</v>
       </c>
       <c r="H48" s="31">
-        <f t="shared" ref="H48:I48" si="32">H40/H54</f>
+        <f t="shared" ref="H48:I48" si="31">H40/H54</f>
         <v>1</v>
       </c>
       <c r="I48" s="31">
-        <f t="shared" si="32"/>
-        <v>2.060266810353844</v>
+        <f>I54/I40</f>
+        <v>0.4829575296756457</v>
       </c>
       <c r="J48" s="8" t="s">
         <v>78</v>
       </c>
       <c r="K48">
-        <f t="shared" ref="K48:AI48" si="33">lz*qa3_</f>
-        <v>3.2667706364552806E-6</v>
+        <f t="shared" ref="K48:AI48" si="32">lz*qa3_</f>
+        <v>3.2679798200268268E-6</v>
       </c>
       <c r="L48">
-        <f t="shared" si="33"/>
-        <v>1.9765398014538413E-4</v>
+        <f t="shared" si="32"/>
+        <v>1.9830698508060648E-4</v>
       </c>
       <c r="M48">
-        <f t="shared" si="33"/>
-        <v>4.9502397006120288E-3</v>
+        <f t="shared" si="32"/>
+        <v>5.030335945783445E-3</v>
       </c>
       <c r="N48">
-        <f t="shared" si="33"/>
-        <v>8.0377517441324112E-2</v>
+        <f t="shared" si="32"/>
+        <v>8.3472232300657173E-2</v>
       </c>
       <c r="O48">
-        <f t="shared" si="33"/>
-        <v>0.62797573641831217</v>
+        <f t="shared" si="32"/>
+        <v>0.66332183097481667</v>
       </c>
       <c r="P48">
-        <f t="shared" si="33"/>
-        <v>1.2223234458723788</v>
+        <f t="shared" si="32"/>
+        <v>1.2991013849342896</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="33"/>
-        <v>1.2824041272066318</v>
+        <f t="shared" si="32"/>
+        <v>1.361708055046104</v>
       </c>
       <c r="R48">
-        <f t="shared" si="33"/>
-        <v>1.2037033661740031</v>
+        <f t="shared" si="32"/>
+        <v>1.2727438014037131</v>
       </c>
       <c r="S48">
-        <f t="shared" si="33"/>
-        <v>1.0881556990873993</v>
+        <f t="shared" si="32"/>
+        <v>1.1436126364169166</v>
       </c>
       <c r="T48">
-        <f t="shared" si="33"/>
-        <v>0.95991092469231709</v>
+        <f t="shared" si="32"/>
+        <v>1.0016351835143378</v>
       </c>
       <c r="U48">
-        <f t="shared" si="33"/>
-        <v>0.83128455095021236</v>
+        <f t="shared" si="32"/>
+        <v>0.86065931313945665</v>
       </c>
       <c r="V48">
-        <f t="shared" si="33"/>
-        <v>0.70967255114358929</v>
+        <f t="shared" si="32"/>
+        <v>0.72873235185088303</v>
       </c>
       <c r="W48">
-        <f t="shared" si="33"/>
-        <v>0.59912285993210612</v>
+        <f t="shared" si="32"/>
+        <v>0.61002643916074317</v>
       </c>
       <c r="X48">
-        <f t="shared" si="33"/>
-        <v>0.5013789306139792</v>
+        <f t="shared" si="32"/>
+        <v>0.50612462876630904</v>
       </c>
       <c r="Y48">
-        <f t="shared" si="33"/>
-        <v>0.41669300985110957</v>
+        <f t="shared" si="32"/>
+        <v>0.4169916809889424</v>
       </c>
       <c r="Z48">
-        <f t="shared" si="33"/>
-        <v>0.34442619628296045</v>
+        <f t="shared" si="32"/>
+        <v>0.34166745780758895</v>
       </c>
       <c r="AA48">
-        <f t="shared" si="33"/>
-        <v>0.28346515214127155</v>
+        <f t="shared" si="32"/>
+        <v>0.27873349161480548</v>
       </c>
       <c r="AB48">
-        <f t="shared" si="33"/>
-        <v>0.23249583222769699</v>
+        <f t="shared" si="32"/>
+        <v>0.22660949204669933</v>
       </c>
       <c r="AC48">
-        <f t="shared" si="33"/>
-        <v>0.19017314505483437</v>
+        <f t="shared" si="32"/>
+        <v>0.18373013222111853</v>
       </c>
       <c r="AD48">
-        <f t="shared" si="33"/>
-        <v>0.15521874124846763</v>
+        <f t="shared" si="32"/>
+        <v>0.14864165408335045</v>
       </c>
       <c r="AE48">
-        <f t="shared" si="33"/>
-        <v>0.12647135210203886</v>
+        <f t="shared" si="32"/>
+        <v>0.12004715305378347</v>
       </c>
       <c r="AF48">
-        <f t="shared" si="33"/>
-        <v>0.10290716582301095</v>
+        <f t="shared" si="32"/>
+        <v>9.6820556029183269E-2</v>
       </c>
       <c r="AG48">
-        <f t="shared" si="33"/>
-        <v>8.3642230372726056E-2</v>
+        <f t="shared" si="32"/>
+        <v>7.8002620743326909E-2</v>
       </c>
       <c r="AH48">
-        <f t="shared" si="33"/>
-        <v>6.792480554352695E-2</v>
+        <f t="shared" si="32"/>
+        <v>6.2787514438517655E-2</v>
       </c>
       <c r="AI48">
-        <f t="shared" si="33"/>
-        <v>0.28909325948738285</v>
+        <f t="shared" si="32"/>
+        <v>0.25533890687910993</v>
       </c>
     </row>
     <row r="49" spans="1:21">
-      <c r="A49" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="1">
-        <f>ye_2</f>
-        <v>1.6619115533171394</v>
+      <c r="A49" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="35">
+        <f>f1_*phi_q1</f>
+        <v>0.41355445859654233</v>
       </c>
       <c r="F49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G49" s="31">
         <f>G41/G55</f>
-        <v>0.99999999702313569</v>
+        <v>0.99999530888810539</v>
       </c>
       <c r="H49" s="31">
-        <f t="shared" ref="H49:I49" si="34">H41/H55</f>
-        <v>2.060266810353844</v>
+        <f t="shared" ref="H49:I49" si="33">H41/H55</f>
+        <v>2.0705754410156936</v>
       </c>
       <c r="I49" s="31">
-        <f t="shared" si="34"/>
-        <v>1</v>
+        <f t="shared" si="33"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="35">
+        <f>f2_*phi_q2</f>
+        <v>0.14990080220793464</v>
       </c>
     </row>
     <row r="51" spans="1:21">
-      <c r="B51">
-        <f>1000000*(C51-B7)^2</f>
-        <v>2.0873862593703405E-6</v>
-      </c>
-      <c r="C51">
-        <f>spr</f>
-        <v>0.39999855522103445</v>
+      <c r="A51" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="35">
+        <f>f3_*phi_q3</f>
+        <v>0.41356694206155192</v>
       </c>
       <c r="G51" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:21">
-      <c r="B52">
-        <f>-(ye_1)</f>
-        <v>-2.4997399888109619</v>
-      </c>
-      <c r="C52">
-        <f>-LN(ye_1)</f>
-        <v>-0.9161867219896993</v>
+      <c r="A52" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="34">
+        <f>phi_t1</f>
+        <v>7.2482496807273103E-2</v>
       </c>
       <c r="G52" s="1">
         <f>G39^0.5</f>
-        <v>10.230277129135866</v>
+        <v>10.500502932283547</v>
       </c>
       <c r="H52" s="1">
         <f>H40^0.5</f>
-        <v>5.0124450977141528</v>
+        <v>5.1245415589234753</v>
       </c>
       <c r="I52" s="11">
         <f>I41^0.5</f>
-        <v>10.230277158552166</v>
+        <v>10.500552190374416</v>
       </c>
     </row>
     <row r="53" spans="1:21">
-      <c r="B53">
-        <f>-(ye_2)</f>
-        <v>-1.6619115533171394</v>
-      </c>
-      <c r="C53">
-        <f>-LN(ye_2)</f>
-        <v>-0.5079684779998157</v>
+      <c r="A53" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="34">
+        <f>phi_t2</f>
+        <v>7.2482393772525411E-2</v>
       </c>
       <c r="G53">
-        <f t="shared" ref="G53:I55" si="35">G$52*$J53</f>
-        <v>104.65857013892037</v>
+        <f t="shared" ref="G53:I55" si="34">G$52*$J53</f>
+        <v>110.26056183089537</v>
       </c>
       <c r="H53">
-        <f t="shared" si="35"/>
-        <v>51.278702444194288</v>
+        <f t="shared" si="34"/>
+        <v>53.81026366608485</v>
       </c>
       <c r="I53">
-        <f t="shared" si="35"/>
-        <v>104.65857043985727</v>
+        <f t="shared" si="34"/>
+        <v>110.26107906562298</v>
       </c>
       <c r="J53">
         <f t="array" ref="J53:J55">TRANSPOSE(G52:I52)</f>
-        <v>10.230277129135866</v>
+        <v>10.500502932283547</v>
       </c>
       <c r="S53">
         <v>0.33</v>
@@ -5304,34 +5327,33 @@
       </c>
     </row>
     <row r="54" spans="1:21">
-      <c r="B54">
-        <f>-(ye_3)</f>
-        <v>-2.4997400392076532</v>
-      </c>
-      <c r="C54">
-        <f>-LN(ye_3)</f>
-        <v>-0.91618674215047247</v>
+      <c r="A54" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="34">
+        <f>phi_t3</f>
+        <v>7.248468529118951E-2</v>
       </c>
       <c r="G54">
-        <f t="shared" si="35"/>
-        <v>51.278702444194288</v>
+        <f t="shared" si="34"/>
+        <v>53.81026366608485</v>
       </c>
       <c r="H54">
-        <f t="shared" si="35"/>
-        <v>25.124605857598642</v>
+        <f t="shared" si="34"/>
+        <v>26.260926189133844</v>
       </c>
       <c r="I54">
-        <f t="shared" si="35"/>
-        <v>51.278702591641881</v>
+        <f t="shared" si="34"/>
+        <v>53.810516091218624</v>
       </c>
       <c r="J54">
-        <v>5.0124450977141528</v>
+        <v>5.1245415589234753</v>
       </c>
       <c r="S54">
         <v>0.32</v>
       </c>
       <c r="T54">
-        <f t="shared" ref="T54:T55" si="36">S54/S$57</f>
+        <f t="shared" ref="T54:T55" si="35">S54/S$57</f>
         <v>0.27826086956521739</v>
       </c>
       <c r="U54">
@@ -5340,35 +5362,27 @@
       </c>
     </row>
     <row r="55" spans="1:21">
-      <c r="B55">
-        <f>SUM(B51:B54)</f>
-        <v>-6.6613894939494953</v>
-      </c>
-      <c r="C55">
-        <f>SUM(C52:C54,B51)</f>
-        <v>-2.340339854753728</v>
-      </c>
       <c r="G55">
-        <f t="shared" si="35"/>
-        <v>104.65857043985727</v>
+        <f t="shared" si="34"/>
+        <v>110.26107906562298</v>
       </c>
       <c r="H55">
-        <f t="shared" si="35"/>
-        <v>51.278702591641881</v>
+        <f t="shared" si="34"/>
+        <v>53.810516091218624</v>
       </c>
       <c r="I55">
-        <f t="shared" si="35"/>
-        <v>104.65857074079418</v>
+        <f t="shared" si="34"/>
+        <v>110.26159630277694</v>
       </c>
       <c r="J55">
-        <v>10.230277158552166</v>
+        <v>10.500552190374416</v>
       </c>
       <c r="S55" s="33">
         <f>0.5</f>
         <v>0.5</v>
       </c>
       <c r="T55">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.43478260869565222</v>
       </c>
       <c r="U55">

</xml_diff>

<commit_message>
Now have analytical soln for fmultipliers in TMA.R
</commit_message>
<xml_diff>
--- a/src/dashboard/data/harvestPolicy/SPRbasedPSC.xlsx
+++ b/src/dashboard/data/harvestPolicy/SPRbasedPSC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="6" r:id="rId1"/>
@@ -2549,13 +2549,13 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>27569.43942245611</c:v>
+                  <c:v>27569.4394224561</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24268.78142553413</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27109.57077646559</c:v>
+                  <c:v>27109.57077646557</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>27568.6269329213</c:v>
@@ -2663,13 +2663,13 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7818.16629015721</c:v>
+                  <c:v>7818.166290157208</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6882.162743206078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7687.756328210182</c:v>
+                  <c:v>7687.756328210178</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7817.935883648219</c:v>
@@ -2809,13 +2809,13 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>27569.43942245611</c:v>
+                  <c:v>27569.4394224561</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24268.78142553413</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27109.57077646559</c:v>
+                  <c:v>27109.57077646557</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>27568.6269329213</c:v>
@@ -2923,13 +2923,13 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7818.16629015721</c:v>
+                  <c:v>7818.166290157208</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6882.162743206078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7687.756328210182</c:v>
+                  <c:v>7687.756328210178</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7817.935883648219</c:v>
@@ -3077,13 +3077,13 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>27569.43942245611</c:v>
+                  <c:v>27569.4394224561</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24268.78142553413</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27109.57077646559</c:v>
+                  <c:v>27109.57077646557</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>27568.6269329213</c:v>
@@ -3227,13 +3227,13 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>7818.16629015721</c:v>
+                  <c:v>7818.166290157208</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6882.162743206078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7687.756328210182</c:v>
+                  <c:v>7687.756328210178</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7817.935883648219</c:v>
@@ -4407,7 +4407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -4465,7 +4465,7 @@
       </c>
       <c r="C5" s="65">
         <f ca="1">'Status Quo'!ye_1</f>
-        <v>27569.439422456111</v>
+        <v>27569.439422456104</v>
       </c>
       <c r="D5" s="79">
         <f ca="1">'Excluders (1)'!ye_1</f>
@@ -4473,7 +4473,7 @@
       </c>
       <c r="E5" s="79">
         <f ca="1">'No Size Limit (1)'!ye_1</f>
-        <v>27109.570776465585</v>
+        <v>27109.570776465567</v>
       </c>
       <c r="F5" s="79">
         <f ca="1">'Reduce DMR (1)'!ye_1</f>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="C6" s="65">
         <f ca="1">'Status Quo'!ye_2</f>
-        <v>10281.832414628601</v>
+        <v>10281.832414628605</v>
       </c>
       <c r="D6" s="79">
         <f ca="1">'Excluders (1)'!ye_2</f>
@@ -4506,7 +4506,7 @@
       </c>
       <c r="E6" s="79">
         <f ca="1">'No Size Limit (1)'!ye_2</f>
-        <v>10110.327572677941</v>
+        <v>10110.327572677936</v>
       </c>
       <c r="F6" s="79">
         <f ca="1">'Reduce DMR (1)'!ye_2</f>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="C7" s="67">
         <f ca="1">'Status Quo'!ye_3</f>
-        <v>7818.1662901572099</v>
+        <v>7818.1662901572081</v>
       </c>
       <c r="D7" s="80">
         <f ca="1">'Excluders (1)'!ye_3</f>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="E7" s="80">
         <f ca="1">'No Size Limit (1)'!ye_3</f>
-        <v>7687.7563282101819</v>
+        <v>7687.7563282101783</v>
       </c>
       <c r="F7" s="80">
         <f ca="1">'Reduce DMR (1)'!ye_3</f>
@@ -4564,7 +4564,7 @@
       </c>
       <c r="C8" s="66">
         <f ca="1">SUM(C5:C7)</f>
-        <v>45669.438127241927</v>
+        <v>45669.438127241912</v>
       </c>
       <c r="D8" s="81">
         <f ca="1">SUM(D5:D7)</f>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="E8" s="81">
         <f ca="1">SUM(E5:E7)</f>
-        <v>44907.654677353712</v>
+        <v>44907.654677353683</v>
       </c>
       <c r="F8" s="81">
         <f ca="1">SUM(F5:F7)</f>
@@ -4644,7 +4644,7 @@
       </c>
       <c r="E11" s="82">
         <f ca="1">'No Size Limit (1)'!$E27</f>
-        <v>2035.3111123523527</v>
+        <v>2035.3111123523515</v>
       </c>
       <c r="F11" s="82">
         <f ca="1">'Reduce DMR (1)'!$E27</f>
@@ -4669,7 +4669,7 @@
       </c>
       <c r="C12" s="70">
         <f ca="1">'Status Quo'!E28</f>
-        <v>818.71296036039837</v>
+        <v>818.71296036039905</v>
       </c>
       <c r="D12" s="82">
         <f ca="1">'Excluders (1)'!E28</f>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="E12" s="82">
         <f ca="1">'No Size Limit (1)'!$E28</f>
-        <v>797.53843008718786</v>
+        <v>797.53843008718741</v>
       </c>
       <c r="F12" s="82">
         <f ca="1">'Reduce DMR (1)'!$E28</f>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="C13" s="71">
         <f ca="1">'Status Quo'!E29</f>
-        <v>635.48251459065784</v>
+        <v>635.48251459065807</v>
       </c>
       <c r="D13" s="83">
         <f ca="1">'Excluders (1)'!E29</f>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="E13" s="83">
         <f ca="1">'No Size Limit (1)'!$E29</f>
-        <v>634.21785061702701</v>
+        <v>634.21785061702678</v>
       </c>
       <c r="F13" s="82">
         <f ca="1">'Reduce DMR (1)'!$E29</f>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="C14" s="74">
         <f ca="1">SUM(C11:C13)</f>
-        <v>3518.5208634487958</v>
+        <v>3518.5208634487963</v>
       </c>
       <c r="D14" s="84">
         <f ca="1">SUM(D11:D13)</f>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="E14" s="84">
         <f ca="1">SUM(E11:E13)</f>
-        <v>3467.0673930565677</v>
+        <v>3467.0673930565654</v>
       </c>
       <c r="F14" s="116">
         <f ca="1">SUM(F11:F13)</f>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="E17" s="85">
         <f ca="1">'No Size Limit (1)'!$C4</f>
-        <v>0.60367371601208453</v>
+        <v>0.60367371601208464</v>
       </c>
       <c r="F17" s="85">
         <f ca="1">'Reduce DMR (1)'!$C4</f>
@@ -4848,7 +4848,7 @@
       </c>
       <c r="E18" s="85">
         <f ca="1">'No Size Limit (1)'!$C5</f>
-        <v>0.22513595166163144</v>
+        <v>0.22513595166163142</v>
       </c>
       <c r="F18" s="85">
         <f ca="1">'Reduce DMR (1)'!$C5</f>
@@ -4881,7 +4881,7 @@
       </c>
       <c r="E19" s="86">
         <f ca="1">'No Size Limit (1)'!$C6</f>
-        <v>0.171190332326284</v>
+        <v>0.17119033232628394</v>
       </c>
       <c r="F19" s="85">
         <f ca="1">'Reduce DMR (1)'!$C6</f>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="C23" s="68">
         <f ca="1">'Status Quo'!C11</f>
-        <v>0.27765604524278537</v>
+        <v>0.27765604524278548</v>
       </c>
       <c r="D23" s="85">
         <f ca="1">'Excluders (1)'!C11</f>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="E23" s="85">
         <f ca="1">'No Size Limit (1)'!$C11</f>
-        <v>0.262677960461282</v>
+        <v>0.26267796046128206</v>
       </c>
       <c r="F23" s="85">
         <f ca="1">'Reduce DMR (1)'!$C11</f>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="E24" s="85">
         <f ca="1">'No Size Limit (1)'!$C12</f>
-        <v>0.55724231251811152</v>
+        <v>0.5572423125181114</v>
       </c>
       <c r="F24" s="85">
         <f ca="1">'Reduce DMR (1)'!$C12</f>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="C25" s="72">
         <f ca="1">'Status Quo'!C13</f>
-        <v>0.18274707963565665</v>
+        <v>0.18274707963565662</v>
       </c>
       <c r="D25" s="86">
         <f ca="1">'Excluders (1)'!C13</f>
@@ -5052,7 +5052,7 @@
       </c>
       <c r="E25" s="85">
         <f ca="1">'No Size Limit (1)'!$C13</f>
-        <v>0.18007972702060657</v>
+        <v>0.18007972702060651</v>
       </c>
       <c r="F25" s="85">
         <f ca="1">'Reduce DMR (1)'!$C13</f>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="C26" s="69">
         <f ca="1">SUM(C23:C25)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="D26" s="87">
         <f ca="1">SUM(D23:D25)</f>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="E29" s="89">
         <f ca="1">'No Size Limit (1)'!avg_wt1</f>
-        <v>32.950103460052752</v>
+        <v>32.950103460052745</v>
       </c>
       <c r="F29" s="89">
         <f ca="1">'Reduce DMR (1)'!avg_wt1</f>
@@ -5182,7 +5182,7 @@
       </c>
       <c r="C30" s="75">
         <f ca="1">avg_wt2</f>
-        <v>6.3000620093714135</v>
+        <v>6.3000620093714117</v>
       </c>
       <c r="D30" s="89">
         <f ca="1">'Excluders (1)'!avg_wt2</f>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="C31" s="76">
         <f ca="1">avg_wt3</f>
-        <v>14.144844814495483</v>
+        <v>14.14484481449548</v>
       </c>
       <c r="D31" s="90">
         <f ca="1">'Excluders (1)'!avg_wt3</f>
@@ -5223,7 +5223,7 @@
       </c>
       <c r="E31" s="89">
         <f ca="1">'No Size Limit (1)'!avg_wt3</f>
-        <v>13.629896640494131</v>
+        <v>13.629896640494129</v>
       </c>
       <c r="F31" s="89">
         <f ca="1">'Reduce DMR (1)'!avg_wt3</f>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="C32" s="77">
         <f ca="1">AVERAGE(C29:C31)</f>
-        <v>17.758142227604278</v>
+        <v>17.758142227604274</v>
       </c>
       <c r="D32" s="91">
         <f ca="1">AVERAGE(D29:D31)</f>
@@ -5308,11 +5308,11 @@
       </c>
       <c r="E42" s="52">
         <f ca="1">'Status Quo'!H47</f>
-        <v>0.49437000276321824</v>
+        <v>0.49437000276321835</v>
       </c>
       <c r="F42" s="52">
         <f ca="1">'Status Quo'!I47</f>
-        <v>0.49000026732177498</v>
+        <v>0.49000026732177521</v>
       </c>
     </row>
     <row r="43" spans="3:9">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="D43" s="52">
         <f ca="1">'Status Quo'!G48</f>
-        <v>2.0227764516670246</v>
+        <v>2.022776451667025</v>
       </c>
       <c r="E43" s="52">
         <f ca="1">'Status Quo'!H48</f>
@@ -5329,7 +5329,7 @@
       </c>
       <c r="F43" s="52">
         <f ca="1">'Status Quo'!I48</f>
-        <v>0.66147781371747894</v>
+        <v>0.66147781371747916</v>
       </c>
     </row>
     <row r="44" spans="3:9">
@@ -5342,11 +5342,11 @@
       </c>
       <c r="E44" s="55">
         <f ca="1">'Status Quo'!H49</f>
-        <v>1.5117665011015862</v>
+        <v>1.5117665011015855</v>
       </c>
       <c r="F44" s="55">
         <f ca="1">'Status Quo'!I49</f>
-        <v>1.0000000000000002</v>
+        <v>0.99999999999999944</v>
       </c>
     </row>
   </sheetData>
@@ -6576,7 +6576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="10" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B63" sqref="B63"/>
     </sheetView>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="F4" s="49">
         <f ca="1">ye_1</f>
-        <v>27569.439422456115</v>
+        <v>27569.439422456111</v>
       </c>
       <c r="J4" t="s">
         <v>78</v>
@@ -6846,7 +6846,7 @@
       </c>
       <c r="F5" s="49">
         <f ca="1">ye_2</f>
-        <v>10281.832414628605</v>
+        <v>10281.832414628601</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -6969,7 +6969,7 @@
       </c>
       <c r="F6" s="49">
         <f ca="1">ye_3</f>
-        <v>7818.1662901572108</v>
+        <v>7818.1662901572099</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
@@ -7123,71 +7123,71 @@
       </c>
       <c r="S7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.25483993958634349</v>
+        <v>0.25483993958634343</v>
       </c>
       <c r="T7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.21108564572102489</v>
+        <v>0.21108564572102484</v>
       </c>
       <c r="U7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.17524127063330219</v>
+        <v>0.17524127063330214</v>
       </c>
       <c r="V7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.14576678542097288</v>
+        <v>0.14576678542097282</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.12126049587651816</v>
+        <v>0.1212604958765181</v>
       </c>
       <c r="X7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.10044442788519788</v>
+        <v>0.10044442788519782</v>
       </c>
       <c r="Y7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>8.2084387601109365E-2</v>
+        <v>8.2084387601109324E-2</v>
       </c>
       <c r="Z7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>6.5126856185556692E-2</v>
+        <v>6.5126856185556664E-2</v>
       </c>
       <c r="AA7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4.9225311135593544E-2</v>
+        <v>4.9225311135593523E-2</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>3.536939008596434E-2</v>
+        <v>3.5369390085964326E-2</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>2.452415604623083E-2</v>
+        <v>2.452415604623082E-2</v>
       </c>
       <c r="AD7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.6689203122081116E-2</v>
+        <v>1.6689203122081109E-2</v>
       </c>
       <c r="AE7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1263078954454142E-2</v>
+        <v>1.1263078954454137E-2</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>7.5750407668483928E-3</v>
+        <v>7.5750407668483894E-3</v>
       </c>
       <c r="AG7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>5.0876406663585881E-3</v>
+        <v>5.0876406663585855E-3</v>
       </c>
       <c r="AH7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>3.4151767680497963E-3</v>
+        <v>3.4151767680497946E-3</v>
       </c>
       <c r="AI7" s="1">
         <f ca="1">AH7*EXP(-AH8)/(1-EXP(-AI8))</f>
-        <v>6.9681775007769684E-3</v>
+        <v>6.9681775007769649E-3</v>
       </c>
     </row>
     <row r="8" spans="1:35">
@@ -7199,7 +7199,7 @@
       </c>
       <c r="F8">
         <f ca="1">SUMXMY2(E4:E6,F4:F6)</f>
-        <v>8195976.5512646884</v>
+        <v>8195976.5512646604</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -7218,7 +7218,7 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.17673189386961455</v>
+        <v>0.17673189386961452</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" ca="1" si="5"/>
@@ -7226,15 +7226,15 @@
       </c>
       <c r="P8" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.17440996916307897</v>
+        <v>0.17440996916307894</v>
       </c>
       <c r="Q8" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.18214667265394868</v>
+        <v>0.18214667265394865</v>
       </c>
       <c r="R8" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.18871523616193234</v>
+        <v>0.18871523616193231</v>
       </c>
       <c r="S8" s="1">
         <f t="shared" ca="1" si="5"/>
@@ -7242,7 +7242,7 @@
       </c>
       <c r="T8" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0.18610024127332164</v>
+        <v>0.18610024127332161</v>
       </c>
       <c r="U8" s="1">
         <f t="shared" ca="1" si="5"/>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="P10" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>0.83995247244924198</v>
+        <v>0.83995247244924209</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" ca="1" si="6"/>
@@ -7433,7 +7433,7 @@
       </c>
       <c r="R10" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>0.82802226392345413</v>
+        <v>0.82802226392345424</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" ca="1" si="6"/>
@@ -7513,7 +7513,7 @@
       </c>
       <c r="C11" s="18">
         <f ca="1">mpr1_/SUM(mpr1_,mpr2_,mpr3_)</f>
-        <v>0.27765604524278537</v>
+        <v>0.27765604524278548</v>
       </c>
       <c r="J11" t="s">
         <v>56</v>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="P11" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.16004752755075802</v>
+        <v>0.16004752755075791</v>
       </c>
       <c r="Q11" s="1">
         <f t="shared" ca="1" si="7"/>
@@ -7548,7 +7548,7 @@
       </c>
       <c r="R11" s="1">
         <f t="shared" ca="1" si="7"/>
-        <v>0.17197773607654587</v>
+        <v>0.17197773607654576</v>
       </c>
       <c r="S11" s="1">
         <f t="shared" ca="1" si="7"/>
@@ -7744,7 +7744,7 @@
       </c>
       <c r="C13" s="18">
         <f ca="1">mpr3_/SUM(mpr1_,mpr2_,mpr3_)</f>
-        <v>0.18274707963565665</v>
+        <v>0.18274707963565662</v>
       </c>
       <c r="J13" t="s">
         <v>101</v>
@@ -8475,7 +8475,7 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>2.8510057588414894E-6</v>
+        <v>2.8510057588414898E-6</v>
       </c>
       <c r="O22" s="1">
         <f t="shared" ca="1" si="18"/>
@@ -8483,15 +8483,15 @@
       </c>
       <c r="P22" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>6.8548652264074141E-5</v>
+        <v>6.85486522640741E-5</v>
       </c>
       <c r="Q22" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>8.8301089149712053E-4</v>
+        <v>8.8301089149712064E-4</v>
       </c>
       <c r="R22" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>3.6786284952239488E-3</v>
+        <v>3.6786284952239471E-3</v>
       </c>
       <c r="S22" s="1">
         <f t="shared" ca="1" si="18"/>
@@ -8499,7 +8499,7 @@
       </c>
       <c r="T22" s="1">
         <f t="shared" ca="1" si="18"/>
-        <v>3.8012326926349364E-2</v>
+        <v>3.8012326926349371E-2</v>
       </c>
       <c r="U22" s="1">
         <f t="shared" ca="1" si="18"/>
@@ -8587,7 +8587,7 @@
       </c>
       <c r="N23" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>1.2187788118918834</v>
+        <v>1.2187788118918836</v>
       </c>
       <c r="O23" s="1">
         <f t="shared" ca="1" si="19"/>
@@ -8595,15 +8595,15 @@
       </c>
       <c r="P23" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>2.829641208551537</v>
+        <v>2.8296412085515357</v>
       </c>
       <c r="Q23" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>3.6505631390637387</v>
+        <v>3.6505631390637392</v>
       </c>
       <c r="R23" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>4.4478953524085592</v>
+        <v>4.4478953524085574</v>
       </c>
       <c r="S23" s="1">
         <f t="shared" ca="1" si="19"/>
@@ -8611,7 +8611,7 @@
       </c>
       <c r="T23" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>5.8881459428694285</v>
+        <v>5.8881459428694294</v>
       </c>
       <c r="U23" s="1">
         <f t="shared" ca="1" si="19"/>
@@ -8699,7 +8699,7 @@
       </c>
       <c r="N24" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>1.5639818023416162E-3</v>
+        <v>1.5639818023416164E-3</v>
       </c>
       <c r="O24" s="1">
         <f t="shared" ca="1" si="20"/>
@@ -8707,15 +8707,15 @@
       </c>
       <c r="P24" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>0.13298365493417877</v>
+        <v>0.13298365493417871</v>
       </c>
       <c r="Q24" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>2.9277792666154108</v>
+        <v>2.9277792666154112</v>
       </c>
       <c r="R24" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>7.0113561452289463</v>
+        <v>7.0113561452289437</v>
       </c>
       <c r="S24" s="1">
         <f t="shared" ca="1" si="20"/>
@@ -8723,7 +8723,7 @@
       </c>
       <c r="T24" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>10.979244998934147</v>
+        <v>10.979244998934149</v>
       </c>
       <c r="U24" s="1">
         <f t="shared" ca="1" si="20"/>
@@ -8829,7 +8829,7 @@
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="21"/>
-        <v>1.7061867360413854E-6</v>
+        <v>1.7061867360413856E-6</v>
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="21"/>
@@ -8837,15 +8837,15 @@
       </c>
       <c r="P26">
         <f t="shared" ca="1" si="21"/>
-        <v>1.5726495811777978E-5</v>
+        <v>1.5726495811777968E-5</v>
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="21"/>
-        <v>1.4357287089019312E-4</v>
+        <v>1.4357287089019315E-4</v>
       </c>
       <c r="R26">
         <f t="shared" ca="1" si="21"/>
-        <v>4.4900772558618789E-4</v>
+        <v>4.4900772558618767E-4</v>
       </c>
       <c r="S26">
         <f t="shared" ca="1" si="21"/>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="T26">
         <f t="shared" ca="1" si="21"/>
-        <v>2.9544916474749782E-3</v>
+        <v>2.9544916474749786E-3</v>
       </c>
       <c r="U26">
         <f t="shared" ca="1" si="21"/>
@@ -8950,7 +8950,7 @@
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="22"/>
-        <v>0.72937918016104031</v>
+        <v>0.72937918016104042</v>
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="22"/>
@@ -8958,7 +8958,7 @@
       </c>
       <c r="P27">
         <f t="shared" ca="1" si="22"/>
-        <v>0.64917892832799617</v>
+        <v>0.64917892832799584</v>
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="22"/>
@@ -8966,7 +8966,7 @@
       </c>
       <c r="R27">
         <f t="shared" ca="1" si="22"/>
-        <v>0.54290325278110485</v>
+        <v>0.54290325278110463</v>
       </c>
       <c r="S27">
         <f t="shared" ca="1" si="22"/>
@@ -8974,7 +8974,7 @@
       </c>
       <c r="T27">
         <f t="shared" ca="1" si="22"/>
-        <v>0.45765359329429856</v>
+        <v>0.45765359329429867</v>
       </c>
       <c r="U27">
         <f t="shared" ca="1" si="22"/>
@@ -9043,15 +9043,15 @@
       </c>
       <c r="B28" s="28">
         <f ca="1">fbar*C28</f>
-        <v>3.3568266353080425E-2</v>
+        <v>3.3568266353080439E-2</v>
       </c>
       <c r="C28" s="36">
         <f ca="1">CHOOSE(C$25,E37,E40,1)</f>
-        <v>0.35923410481843726</v>
+        <v>0.35923410481843715</v>
       </c>
       <c r="E28" s="42">
         <f ca="1">f2_/(F5/(365*re*phib))</f>
-        <v>818.71296036039837</v>
+        <v>818.71296036039905</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>32</v>
@@ -9070,7 +9070,7 @@
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="23"/>
-        <v>9.3596619308467899E-4</v>
+        <v>9.3596619308467909E-4</v>
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="23"/>
@@ -9078,15 +9078,15 @@
       </c>
       <c r="P28">
         <f t="shared" ca="1" si="23"/>
-        <v>3.0509234292464136E-2</v>
+        <v>3.0509234292464122E-2</v>
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="23"/>
-        <v>0.47604132484489226</v>
+        <v>0.47604132484489237</v>
       </c>
       <c r="R28">
         <f t="shared" ca="1" si="23"/>
-        <v>0.85579532701693384</v>
+        <v>0.8557953270169335</v>
       </c>
       <c r="S28">
         <f t="shared" ca="1" si="23"/>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="T28">
         <f t="shared" ca="1" si="23"/>
-        <v>0.85335706250718757</v>
+        <v>0.85335706250718768</v>
       </c>
       <c r="U28">
         <f t="shared" ca="1" si="23"/>
@@ -9163,15 +9163,15 @@
       </c>
       <c r="B29" s="28">
         <f ca="1">fbar*C29</f>
-        <v>1.9812315490241407E-2</v>
+        <v>1.9812315490241414E-2</v>
       </c>
       <c r="C29" s="36">
         <f ca="1">CHOOSE(C$25,E38,E41,1)</f>
-        <v>0.21202344335140819</v>
+        <v>0.2120234433514081</v>
       </c>
       <c r="E29" s="42">
         <f ca="1">f3_/(F6/(365*re*phib))</f>
-        <v>635.48251459065784</v>
+        <v>635.48251459065807</v>
       </c>
     </row>
     <row r="30" spans="1:39">
@@ -9201,7 +9201,7 @@
       </c>
       <c r="B31" s="37">
         <f ca="1">SUM(B27:B29)</f>
-        <v>0.28033195542538797</v>
+        <v>0.28033195542538802</v>
       </c>
       <c r="G31">
         <f ca="1">SUMPRODUCT(dlz1_,wa,ma)</f>
@@ -9255,63 +9255,63 @@
       </c>
       <c r="U31">
         <f t="shared" ca="1" si="24"/>
-        <v>-9.0885828147845298E-4</v>
+        <v>-9.0885828147845276E-4</v>
       </c>
       <c r="V31">
         <f t="shared" ca="1" si="24"/>
-        <v>-1.9567170004328419E-3</v>
+        <v>-1.956717000432841E-3</v>
       </c>
       <c r="W31">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.1420680163607813E-3</v>
+        <v>-4.1420680163607804E-3</v>
       </c>
       <c r="X31">
         <f t="shared" ca="1" si="24"/>
-        <v>-8.5569520795532577E-3</v>
+        <v>-8.556952079553256E-3</v>
       </c>
       <c r="Y31">
         <f t="shared" ca="1" si="24"/>
-        <v>-1.6793368464674566E-2</v>
+        <v>-1.6793368464674562E-2</v>
       </c>
       <c r="Z31">
         <f t="shared" ca="1" si="24"/>
-        <v>-2.9750497530034527E-2</v>
+        <v>-2.9750497530034517E-2</v>
       </c>
       <c r="AA31">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.4792499475577174E-2</v>
+        <v>-4.479249947557716E-2</v>
       </c>
       <c r="AB31">
         <f t="shared" ca="1" si="24"/>
-        <v>-5.5773666396525812E-2</v>
+        <v>-5.5773666396525791E-2</v>
       </c>
       <c r="AC31">
         <f t="shared" ca="1" si="24"/>
-        <v>-5.8942212351595483E-2</v>
+        <v>-5.8942212351595455E-2</v>
       </c>
       <c r="AD31">
         <f t="shared" ca="1" si="24"/>
-        <v>-5.5436347781797637E-2</v>
+        <v>-5.543634778179761E-2</v>
       </c>
       <c r="AE31">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.8264734519488039E-2</v>
+        <v>-4.8264734519488012E-2</v>
       </c>
       <c r="AF31">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.9916092690568172E-2</v>
+        <v>-3.9916092690568152E-2</v>
       </c>
       <c r="AG31">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.1862435402336763E-2</v>
+        <v>-3.1862435402336749E-2</v>
       </c>
       <c r="AH31">
         <f t="shared" ca="1" si="24"/>
-        <v>-2.4793883210148828E-2</v>
+        <v>-2.4793883210148818E-2</v>
       </c>
       <c r="AI31">
         <f ca="1">(AH31*sa-AH$7*AH18*AH$10)/oa-AH$7*AH$10*flt1_*sa/oa^2</f>
-        <v>-7.176221696963539E-2</v>
+        <v>-7.1762216969635362E-2</v>
       </c>
     </row>
     <row r="32" spans="1:39">
@@ -9322,11 +9322,11 @@
       <c r="C32" s="12"/>
       <c r="G32">
         <f ca="1">SUMPRODUCT(dlz2_,wa,ma)</f>
-        <v>-106.63282272358627</v>
+        <v>-106.63282272358626</v>
       </c>
       <c r="H32">
         <f ca="1">Ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-33006.426061680824</v>
+        <v>-33006.426061680817</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>53</v>
@@ -9352,7 +9352,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.94032199296849128</v>
+        <v>-0.94032199296849139</v>
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="25"/>
@@ -9360,27 +9360,27 @@
       </c>
       <c r="R32">
         <f t="shared" ca="1" si="25"/>
-        <v>-1.0650769813015899</v>
+        <v>-1.0650769813015901</v>
       </c>
       <c r="S32">
         <f t="shared" ca="1" si="25"/>
-        <v>-1.0340289603095152</v>
+        <v>-1.0340289603095156</v>
       </c>
       <c r="T32">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.97382559241567845</v>
+        <v>-0.9738255924156789</v>
       </c>
       <c r="U32">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.89792795093719402</v>
+        <v>-0.89792795093719424</v>
       </c>
       <c r="V32">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.81405136921887578</v>
+        <v>-0.814051369218876</v>
       </c>
       <c r="W32">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.72551210826408696</v>
+        <v>-0.72551210826408707</v>
       </c>
       <c r="X32">
         <f t="shared" ca="1" si="25"/>
@@ -9428,7 +9428,7 @@
       </c>
       <c r="AI32">
         <f ca="1">(AH32*sa-AH$7*AH19*AH$10)/oa-AH$7*AH$10*flt2_*sa/oa^2</f>
-        <v>-6.4925479052461904E-2</v>
+        <v>-6.492547905246189E-2</v>
       </c>
     </row>
     <row r="33" spans="1:35">
@@ -9437,7 +9437,7 @@
       </c>
       <c r="B33" s="62">
         <f ca="1">SUMPRODUCT(lz,wa)</f>
-        <v>35.62779878205712</v>
+        <v>35.627798782057113</v>
       </c>
       <c r="C33" s="61"/>
       <c r="D33" s="63"/>
@@ -9478,7 +9478,7 @@
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="26"/>
-        <v>-1.4128418029718929E-2</v>
+        <v>-1.4128418029718932E-2</v>
       </c>
       <c r="R33">
         <f t="shared" ca="1" si="26"/>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="S33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.38174995111985283</v>
+        <v>-0.38174995111985288</v>
       </c>
       <c r="T33">
         <f t="shared" ca="1" si="26"/>
@@ -9502,55 +9502,55 @@
       </c>
       <c r="W33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.61058729758125141</v>
+        <v>-0.6105872975812513</v>
       </c>
       <c r="X33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.56815358142281225</v>
+        <v>-0.56815358142281214</v>
       </c>
       <c r="Y33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.50158723876097722</v>
+        <v>-0.50158723876097711</v>
       </c>
       <c r="Z33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.41534277915133178</v>
+        <v>-0.41534277915133166</v>
       </c>
       <c r="AA33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.32581201646069491</v>
+        <v>-0.32581201646069485</v>
       </c>
       <c r="AB33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.2455819481888647</v>
+        <v>-0.24558194818886467</v>
       </c>
       <c r="AC33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.18076432663580719</v>
+        <v>-0.18076432663580716</v>
       </c>
       <c r="AD33">
         <f t="shared" ca="1" si="26"/>
-        <v>-0.13127556758856823</v>
+        <v>-0.1312755675885682</v>
       </c>
       <c r="AE33">
         <f t="shared" ca="1" si="26"/>
-        <v>-9.4554718466184975E-2</v>
+        <v>-9.4554718466184962E-2</v>
       </c>
       <c r="AF33">
         <f t="shared" ca="1" si="26"/>
-        <v>-6.7719321886847858E-2</v>
+        <v>-6.7719321886847844E-2</v>
       </c>
       <c r="AG33">
         <f t="shared" ca="1" si="26"/>
-        <v>-4.8287710742369115E-2</v>
+        <v>-4.8287710742369108E-2</v>
       </c>
       <c r="AH33">
         <f t="shared" ca="1" si="26"/>
-        <v>-3.4306789750843322E-2</v>
+        <v>-3.4306789750843315E-2</v>
       </c>
       <c r="AI33">
         <f ca="1">(AH33*sa-AH$7*AH20*AH$10)/oa-AH$7*AH$10*flt3_*sa/oa^2</f>
-        <v>-8.1775530586942452E-2</v>
+        <v>-8.1775530586942424E-2</v>
       </c>
     </row>
     <row r="34" spans="1:35">
@@ -9572,7 +9572,7 @@
       </c>
       <c r="B35" s="1">
         <f ca="1">SUMPRODUCT(lz,wa,ma)</f>
-        <v>17.137594381347672</v>
+        <v>17.137594381347661</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="1">
@@ -9604,7 +9604,7 @@
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="27"/>
-        <v>3.6960513795410158E-12</v>
+        <v>3.6960513795410133E-12</v>
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="27"/>
@@ -9612,27 +9612,27 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="27"/>
-        <v>9.2404779709251024E-10</v>
+        <v>9.2404779709251138E-10</v>
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="27"/>
-        <v>1.1384644913775043E-7</v>
+        <v>1.1384644913775041E-7</v>
       </c>
       <c r="R35">
         <f t="shared" ca="1" si="27"/>
-        <v>1.5423388201363734E-6</v>
+        <v>1.542338820136374E-6</v>
       </c>
       <c r="S35">
         <f t="shared" ca="1" si="27"/>
-        <v>1.3429916404115864E-5</v>
+        <v>1.3429916404115865E-5</v>
       </c>
       <c r="T35">
         <f t="shared" ca="1" si="27"/>
-        <v>1.1049357955160824E-4</v>
+        <v>1.1049357955160826E-4</v>
       </c>
       <c r="U35">
         <f t="shared" ca="1" si="27"/>
-        <v>8.7402921769853738E-4</v>
+        <v>8.7402921769853749E-4</v>
       </c>
       <c r="V35">
         <f t="shared" ca="1" si="27"/>
@@ -9697,7 +9697,7 @@
       </c>
       <c r="B36" s="1">
         <f ca="1">SUMPRODUCT(lz,ta1_)</f>
-        <v>0.18356485561267402</v>
+        <v>0.18356485561267399</v>
       </c>
       <c r="C36" s="29">
         <f ca="1">B11/(phi_t1/SUM(B$36:B$38))</f>
@@ -9713,7 +9713,7 @@
       </c>
       <c r="H36" s="1">
         <f ca="1">SUM(dqa22_)</f>
-        <v>60.962622500182263</v>
+        <v>60.962622500182256</v>
       </c>
       <c r="I36" s="11">
         <f ca="1">SUM(dqa23_)</f>
@@ -9736,7 +9736,7 @@
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="28"/>
-        <v>0.67544750493471772</v>
+        <v>0.67544750493471728</v>
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="28"/>
@@ -9744,15 +9744,15 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="28"/>
-        <v>1.5745604480993163</v>
+        <v>1.5745604480993183</v>
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="28"/>
-        <v>1.9458398676571085</v>
+        <v>1.9458398676571083</v>
       </c>
       <c r="R36">
         <f t="shared" ca="1" si="28"/>
-        <v>2.2548468522236105</v>
+        <v>2.2548468522236123</v>
       </c>
       <c r="S36">
         <f t="shared" ca="1" si="28"/>
@@ -9768,7 +9768,7 @@
       </c>
       <c r="V36">
         <f t="shared" ca="1" si="28"/>
-        <v>2.7324195514204606</v>
+        <v>2.732419551420461</v>
       </c>
       <c r="W36">
         <f t="shared" ca="1" si="28"/>
@@ -9868,7 +9868,7 @@
       </c>
       <c r="N37">
         <f t="shared" ca="1" si="29"/>
-        <v>1.1122571385390239E-6</v>
+        <v>1.1122571385390235E-6</v>
       </c>
       <c r="O37">
         <f t="shared" ca="1" si="29"/>
@@ -9876,7 +9876,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="29"/>
-        <v>3.477708084034577E-3</v>
+        <v>3.4777080840345817E-3</v>
       </c>
       <c r="Q37">
         <f t="shared" ca="1" si="29"/>
@@ -9884,7 +9884,7 @@
       </c>
       <c r="R37">
         <f t="shared" ca="1" si="29"/>
-        <v>5.6028885559619637</v>
+        <v>5.6028885559619672</v>
       </c>
       <c r="S37">
         <f t="shared" ca="1" si="29"/>
@@ -9896,7 +9896,7 @@
       </c>
       <c r="U37">
         <f t="shared" ca="1" si="29"/>
-        <v>9.3050168565312674</v>
+        <v>9.3050168565312692</v>
       </c>
       <c r="V37">
         <f t="shared" ca="1" si="29"/>
@@ -9961,15 +9961,15 @@
       </c>
       <c r="B38" s="1">
         <f ca="1">SUMPRODUCT(lz,ta3_)</f>
-        <v>1.3839819609943012</v>
+        <v>1.3839819609943007</v>
       </c>
       <c r="C38" s="29">
         <f ca="1">B13/(phi_t3/SUM(B$36:B$38))</f>
-        <v>0.52546108738733188</v>
+        <v>0.52546108738733199</v>
       </c>
       <c r="E38" s="38">
         <f ca="1">C38/AVERAGE(C$36:C$38)</f>
-        <v>0.21202344335152307</v>
+        <v>0.21202344335152312</v>
       </c>
       <c r="G38" t="s">
         <v>69</v>
@@ -9991,7 +9991,7 @@
       </c>
       <c r="N38">
         <f t="shared" ca="1" si="30"/>
-        <v>-6.8859441078764896E-7</v>
+        <v>-6.8859441078765002E-7</v>
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="30"/>
@@ -9999,15 +9999,15 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="30"/>
-        <v>-1.0348506884546809E-5</v>
+        <v>-1.0348506884546736E-5</v>
       </c>
       <c r="Q38">
         <f t="shared" ca="1" si="30"/>
-        <v>-1.0249845876162189E-4</v>
+        <v>-1.0249845876162204E-4</v>
       </c>
       <c r="R38">
         <f t="shared" ca="1" si="30"/>
-        <v>-3.2482638581975772E-4</v>
+        <v>-3.2482638581975549E-4</v>
       </c>
       <c r="S38">
         <f t="shared" ca="1" si="30"/>
@@ -10015,19 +10015,19 @@
       </c>
       <c r="T38">
         <f t="shared" ca="1" si="30"/>
-        <v>-1.8267587358585342E-3</v>
+        <v>-1.8267587358585362E-3</v>
       </c>
       <c r="U38">
         <f t="shared" ca="1" si="30"/>
-        <v>-3.5773920487195414E-3</v>
+        <v>-3.5773920487195397E-3</v>
       </c>
       <c r="V38">
         <f t="shared" ca="1" si="30"/>
-        <v>-3.0994595721158024E-3</v>
+        <v>-3.0994595721157989E-3</v>
       </c>
       <c r="W38">
         <f t="shared" ca="1" si="30"/>
-        <v>2.7982737353943059E-2</v>
+        <v>2.7982737353943073E-2</v>
       </c>
       <c r="X38">
         <f t="shared" ca="1" si="30"/>
@@ -10035,11 +10035,11 @@
       </c>
       <c r="Y38">
         <f t="shared" ca="1" si="30"/>
-        <v>1.5248589445071332</v>
+        <v>1.5248589445071334</v>
       </c>
       <c r="Z38">
         <f t="shared" ca="1" si="30"/>
-        <v>5.5792987645158867</v>
+        <v>5.5792987645158876</v>
       </c>
       <c r="AA38">
         <f t="shared" ca="1" si="30"/>
@@ -10084,11 +10084,11 @@
       </c>
       <c r="B39" s="1">
         <f ca="1">SUMPRODUCT(lz,qa1_)</f>
-        <v>6.026346072740826</v>
+        <v>6.0263460727408242</v>
       </c>
       <c r="C39" s="23">
         <f ca="1">B4/(phi_q1/SUM(B$39:B$41))</f>
-        <v>4.0867897226044043</v>
+        <v>4.0867897226044052</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="39">
@@ -10124,7 +10124,7 @@
       </c>
       <c r="N39">
         <f t="shared" ca="1" si="31"/>
-        <v>-8.7832964124522824E-10</v>
+        <v>-8.7832964124522958E-10</v>
       </c>
       <c r="O39">
         <f t="shared" ca="1" si="31"/>
@@ -10132,43 +10132,43 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="31"/>
-        <v>-4.8522558597085369E-7</v>
+        <v>-4.852255859708503E-7</v>
       </c>
       <c r="Q39">
         <f t="shared" ca="1" si="31"/>
-        <v>-8.2177083540658274E-5</v>
+        <v>-8.2177083540658409E-5</v>
       </c>
       <c r="R39">
         <f t="shared" ca="1" si="31"/>
-        <v>-5.1307855298240404E-4</v>
+        <v>-5.1307855298240068E-4</v>
       </c>
       <c r="S39">
         <f t="shared" ca="1" si="31"/>
-        <v>-1.4694325056408457E-3</v>
+        <v>-1.4694325056408455E-3</v>
       </c>
       <c r="T39">
         <f t="shared" ca="1" si="31"/>
-        <v>-3.5126592779359525E-3</v>
+        <v>-3.5126592779359572E-3</v>
       </c>
       <c r="U39">
         <f t="shared" ca="1" si="31"/>
-        <v>-7.4152095558181587E-3</v>
+        <v>-7.415209555818157E-3</v>
       </c>
       <c r="V39">
         <f t="shared" ca="1" si="31"/>
-        <v>-1.1421710650004656E-2</v>
+        <v>-1.1421710650004642E-2</v>
       </c>
       <c r="W39">
         <f t="shared" ca="1" si="31"/>
-        <v>1.0756213208681649E-2</v>
+        <v>1.075621320868167E-2</v>
       </c>
       <c r="X39">
         <f t="shared" ca="1" si="31"/>
-        <v>0.23785728378204207</v>
+        <v>0.23785728378204213</v>
       </c>
       <c r="Y39">
         <f t="shared" ca="1" si="31"/>
-        <v>1.4692834842979738</v>
+        <v>1.4692834842979741</v>
       </c>
       <c r="Z39">
         <f t="shared" ca="1" si="31"/>
@@ -10257,7 +10257,7 @@
       </c>
       <c r="N40">
         <f t="shared" ca="1" si="32"/>
-        <v>-6.8859441078764875E-7</v>
+        <v>-6.8859441078764991E-7</v>
       </c>
       <c r="O40">
         <f t="shared" ca="1" si="32"/>
@@ -10265,35 +10265,35 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="32"/>
-        <v>-1.0348506884546809E-5</v>
+        <v>-1.0348506884546736E-5</v>
       </c>
       <c r="Q40">
         <f t="shared" ca="1" si="32"/>
-        <v>-1.0249845876162189E-4</v>
+        <v>-1.0249845876162204E-4</v>
       </c>
       <c r="R40">
         <f t="shared" ca="1" si="32"/>
-        <v>-3.2482638581975772E-4</v>
+        <v>-3.2482638581975549E-4</v>
       </c>
       <c r="S40">
         <f t="shared" ca="1" si="32"/>
-        <v>-7.9948088006860879E-4</v>
+        <v>-7.9948088006860857E-4</v>
       </c>
       <c r="T40">
         <f t="shared" ca="1" si="32"/>
-        <v>-1.8267587358585342E-3</v>
+        <v>-1.8267587358585362E-3</v>
       </c>
       <c r="U40">
         <f t="shared" ca="1" si="32"/>
-        <v>-3.5773920487195414E-3</v>
+        <v>-3.5773920487195397E-3</v>
       </c>
       <c r="V40">
         <f t="shared" ca="1" si="32"/>
-        <v>-3.0994595721158058E-3</v>
+        <v>-3.0994595721157989E-3</v>
       </c>
       <c r="W40">
         <f t="shared" ca="1" si="32"/>
-        <v>2.7982737353943059E-2</v>
+        <v>2.798273735394307E-2</v>
       </c>
       <c r="X40">
         <f t="shared" ca="1" si="32"/>
@@ -10301,11 +10301,11 @@
       </c>
       <c r="Y40">
         <f t="shared" ca="1" si="32"/>
-        <v>1.5248589445071332</v>
+        <v>1.5248589445071334</v>
       </c>
       <c r="Z40">
         <f t="shared" ca="1" si="32"/>
-        <v>5.5792987645158867</v>
+        <v>5.5792987645158876</v>
       </c>
       <c r="AA40">
         <f t="shared" ca="1" si="32"/>
@@ -10350,11 +10350,11 @@
       </c>
       <c r="B41" s="1">
         <f ca="1">SUMPRODUCT(lz,qa3_)</f>
-        <v>19.576210064325529</v>
+        <v>19.576210064325519</v>
       </c>
       <c r="C41" s="23">
         <f ca="1">B6/(phi_q3/SUM(B$39:B$41))</f>
-        <v>0.35676702920344355</v>
+        <v>0.35676702920344361</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="39">
@@ -10367,11 +10367,11 @@
       </c>
       <c r="H41" s="1">
         <f ca="1">re*phi_q3+f3_*phi_q3*$H33+f3_*re*H37</f>
-        <v>495547.56107126549</v>
+        <v>495547.56107126537</v>
       </c>
       <c r="I41" s="1">
         <f ca="1">re*phi_q3+f1_*phi_q3*$H33+f3_*re*I37</f>
-        <v>324901.63724451384</v>
+        <v>324901.63724451372</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>67</v>
@@ -10390,7 +10390,7 @@
       </c>
       <c r="N41">
         <f t="shared" ca="1" si="33"/>
-        <v>-3.7774648788630198E-4</v>
+        <v>-3.7774648788630258E-4</v>
       </c>
       <c r="O41">
         <f t="shared" ca="1" si="33"/>
@@ -10398,43 +10398,43 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="33"/>
-        <v>-2.0078270950240541E-2</v>
+        <v>-2.0078270950240399E-2</v>
       </c>
       <c r="Q41">
         <f t="shared" ca="1" si="33"/>
-        <v>-0.34031147956282298</v>
+        <v>-0.34031147956282348</v>
       </c>
       <c r="R41">
         <f t="shared" ca="1" si="33"/>
-        <v>-0.62256212919383758</v>
+        <v>-0.62256212919383347</v>
       </c>
       <c r="S41">
         <f t="shared" ca="1" si="33"/>
-        <v>-0.63976539031778745</v>
+        <v>-0.63976539031778734</v>
       </c>
       <c r="T41">
         <f t="shared" ca="1" si="33"/>
-        <v>-0.56305661555430819</v>
+        <v>-0.56305661555430897</v>
       </c>
       <c r="U41">
         <f t="shared" ca="1" si="33"/>
-        <v>-0.46671294378547162</v>
+        <v>-0.46671294378547151</v>
       </c>
       <c r="V41">
         <f t="shared" ca="1" si="33"/>
-        <v>-0.36960537436998053</v>
+        <v>-0.36960537436998031</v>
       </c>
       <c r="W41">
         <f t="shared" ca="1" si="33"/>
-        <v>-0.2462073947704051</v>
+        <v>-0.24620739477040493</v>
       </c>
       <c r="X41">
         <f t="shared" ca="1" si="33"/>
-        <v>8.8710107575183994E-2</v>
+        <v>8.8710107575184077E-2</v>
       </c>
       <c r="Y41">
         <f t="shared" ca="1" si="33"/>
-        <v>1.4362969911696901</v>
+        <v>1.4362969911696903</v>
       </c>
       <c r="Z41">
         <f t="shared" ca="1" si="33"/>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="B42" s="1">
         <f ca="1">SUMPRODUCT(lz/SUM(lz),len,ta1_)</f>
-        <v>4.3875162197831665</v>
+        <v>4.3875162197831648</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>68</v>
@@ -10502,7 +10502,7 @@
       </c>
       <c r="N42">
         <f t="shared" ca="1" si="34"/>
-        <v>-8.7832964124522824E-10</v>
+        <v>-8.7832964124522958E-10</v>
       </c>
       <c r="O42">
         <f t="shared" ca="1" si="34"/>
@@ -10510,15 +10510,15 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="34"/>
-        <v>-4.8522558597085369E-7</v>
+        <v>-4.852255859708503E-7</v>
       </c>
       <c r="Q42">
         <f t="shared" ca="1" si="34"/>
-        <v>-8.2177083540658274E-5</v>
+        <v>-8.2177083540658409E-5</v>
       </c>
       <c r="R42">
         <f t="shared" ca="1" si="34"/>
-        <v>-5.1307855298240394E-4</v>
+        <v>-5.1307855298240058E-4</v>
       </c>
       <c r="S42">
         <f t="shared" ca="1" si="34"/>
@@ -10526,27 +10526,27 @@
       </c>
       <c r="T42">
         <f t="shared" ca="1" si="34"/>
-        <v>-3.5126592779359525E-3</v>
+        <v>-3.5126592779359572E-3</v>
       </c>
       <c r="U42">
         <f t="shared" ca="1" si="34"/>
-        <v>-7.4152095558181587E-3</v>
+        <v>-7.415209555818157E-3</v>
       </c>
       <c r="V42">
         <f t="shared" ca="1" si="34"/>
-        <v>-1.1421710650004652E-2</v>
+        <v>-1.1421710650004642E-2</v>
       </c>
       <c r="W42">
         <f t="shared" ca="1" si="34"/>
-        <v>1.0756213208681649E-2</v>
+        <v>1.075621320868167E-2</v>
       </c>
       <c r="X42">
         <f t="shared" ca="1" si="34"/>
-        <v>0.23785728378204207</v>
+        <v>0.23785728378204213</v>
       </c>
       <c r="Y42">
         <f t="shared" ca="1" si="34"/>
-        <v>1.4692834842979738</v>
+        <v>1.4692834842979741</v>
       </c>
       <c r="Z42">
         <f t="shared" ca="1" si="34"/>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="N43">
         <f t="shared" ca="1" si="35"/>
-        <v>-3.7774648788630198E-4</v>
+        <v>-3.7774648788630258E-4</v>
       </c>
       <c r="O43">
         <f t="shared" ca="1" si="35"/>
@@ -10617,43 +10617,43 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="35"/>
-        <v>-2.0078270950240538E-2</v>
+        <v>-2.0078270950240399E-2</v>
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="35"/>
-        <v>-0.34031147956282298</v>
+        <v>-0.34031147956282348</v>
       </c>
       <c r="R43">
         <f t="shared" ca="1" si="35"/>
-        <v>-0.62256212919383758</v>
+        <v>-0.62256212919383347</v>
       </c>
       <c r="S43">
         <f t="shared" ca="1" si="35"/>
-        <v>-0.63976539031778745</v>
+        <v>-0.63976539031778734</v>
       </c>
       <c r="T43">
         <f t="shared" ca="1" si="35"/>
-        <v>-0.56305661555430842</v>
+        <v>-0.56305661555430897</v>
       </c>
       <c r="U43">
         <f t="shared" ca="1" si="35"/>
-        <v>-0.46671294378547162</v>
+        <v>-0.46671294378547151</v>
       </c>
       <c r="V43">
         <f t="shared" ca="1" si="35"/>
-        <v>-0.36960537436998053</v>
+        <v>-0.36960537436998042</v>
       </c>
       <c r="W43">
         <f t="shared" ca="1" si="35"/>
-        <v>-0.2462073947704051</v>
+        <v>-0.24620739477040493</v>
       </c>
       <c r="X43">
         <f t="shared" ca="1" si="35"/>
-        <v>8.8710107575183994E-2</v>
+        <v>8.8710107575184077E-2</v>
       </c>
       <c r="Y43">
         <f t="shared" ca="1" si="35"/>
-        <v>1.4362969911696901</v>
+        <v>1.4362969911696903</v>
       </c>
       <c r="Z43">
         <f t="shared" ca="1" si="35"/>
@@ -10712,7 +10712,7 @@
       </c>
       <c r="B46" s="1">
         <f ca="1">phif/phie</f>
-        <v>0.39999999998752639</v>
+        <v>0.39999999998752617</v>
       </c>
       <c r="G46" s="32" t="s">
         <v>94</v>
@@ -10736,7 +10736,7 @@
       </c>
       <c r="N46">
         <f t="shared" ca="1" si="36"/>
-        <v>1.7832379287948257E-6</v>
+        <v>1.7832379287948259E-6</v>
       </c>
       <c r="O46">
         <f t="shared" ca="1" si="36"/>
@@ -10744,7 +10744,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="36"/>
-        <v>3.013526270101504E-5</v>
+        <v>3.0135262701015023E-5</v>
       </c>
       <c r="Q46">
         <f t="shared" ca="1" si="36"/>
@@ -10752,11 +10752,11 @@
       </c>
       <c r="R46">
         <f t="shared" ca="1" si="36"/>
-        <v>1.1321693924526352E-3</v>
+        <v>1.1321693924526346E-3</v>
       </c>
       <c r="S46">
         <f t="shared" ca="1" si="36"/>
-        <v>3.0777794310950352E-3</v>
+        <v>3.0777794310950343E-3</v>
       </c>
       <c r="T46">
         <f t="shared" ca="1" si="36"/>
@@ -10764,63 +10764,63 @@
       </c>
       <c r="U46">
         <f t="shared" ca="1" si="36"/>
-        <v>2.0321203231374027E-2</v>
+        <v>2.032120323137402E-2</v>
       </c>
       <c r="V46">
         <f t="shared" ca="1" si="36"/>
-        <v>4.9974879861832501E-2</v>
+        <v>4.997487986183248E-2</v>
       </c>
       <c r="W46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.11807829814840104</v>
+        <v>0.11807829814840098</v>
       </c>
       <c r="X46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.26015214242939727</v>
+        <v>0.2601521424293971</v>
       </c>
       <c r="Y46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.50260035243535917</v>
+        <v>0.50260035243535894</v>
       </c>
       <c r="Z46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.78047356322031614</v>
+        <v>0.7804735632203158</v>
       </c>
       <c r="AA46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.92370334544791222</v>
+        <v>0.92370334544791188</v>
       </c>
       <c r="AB46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.86502755787380703</v>
+        <v>0.8650275578738067</v>
       </c>
       <c r="AC46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.70001205098637176</v>
+        <v>0.70001205098637143</v>
       </c>
       <c r="AD46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.5259533045482383</v>
+        <v>0.52595330454823808</v>
       </c>
       <c r="AE46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.38155912998423752</v>
+        <v>0.38155912998423736</v>
       </c>
       <c r="AF46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.27209144906829691</v>
+        <v>0.27209144906829674</v>
       </c>
       <c r="AG46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.19219715413414604</v>
+        <v>0.19219715413414593</v>
       </c>
       <c r="AH46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.13493077945837784</v>
+        <v>0.13493077945837775</v>
       </c>
       <c r="AI46">
         <f t="shared" ca="1" si="36"/>
-        <v>0.28667201535751452</v>
+        <v>0.28667201535751435</v>
       </c>
     </row>
     <row r="47" spans="1:35" ht="19" thickTop="1">
@@ -10840,11 +10840,11 @@
       </c>
       <c r="H47" s="31">
         <f ca="1">H53/H39</f>
-        <v>0.49437000276321824</v>
+        <v>0.49437000276321835</v>
       </c>
       <c r="I47" s="31">
         <f ca="1">I53/I39</f>
-        <v>0.49000026732177498</v>
+        <v>0.49000026732177521</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>76</v>
@@ -10863,7 +10863,7 @@
       </c>
       <c r="N47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.76231785833370391</v>
+        <v>0.76231785833370413</v>
       </c>
       <c r="O47">
         <f t="shared" ca="1" si="37"/>
@@ -10871,7 +10871,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="37"/>
-        <v>1.2439629132432803</v>
+        <v>1.2439629132432797</v>
       </c>
       <c r="Q47">
         <f t="shared" ca="1" si="37"/>
@@ -10879,75 +10879,75 @@
       </c>
       <c r="R47">
         <f t="shared" ca="1" si="37"/>
-        <v>1.3689262140407381</v>
+        <v>1.3689262140407377</v>
       </c>
       <c r="S47">
         <f t="shared" ca="1" si="37"/>
-        <v>1.3262161775778787</v>
+        <v>1.3262161775778782</v>
       </c>
       <c r="T47">
         <f t="shared" ca="1" si="37"/>
-        <v>1.2429030884502263</v>
+        <v>1.2429030884502261</v>
       </c>
       <c r="U47">
         <f t="shared" ca="1" si="37"/>
-        <v>1.1353843130428101</v>
+        <v>1.1353843130428096</v>
       </c>
       <c r="V47">
         <f t="shared" ca="1" si="37"/>
-        <v>1.0149408160376086</v>
+        <v>1.0149408160376083</v>
       </c>
       <c r="W47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.88849362677228749</v>
+        <v>0.88849362677228705</v>
       </c>
       <c r="X47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.75885048235818764</v>
+        <v>0.75885048235818719</v>
       </c>
       <c r="Y47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.62596511246331499</v>
+        <v>0.62596511246331465</v>
       </c>
       <c r="Z47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.53519509062798676</v>
+        <v>0.53519509062798654</v>
       </c>
       <c r="AA47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.43118810915395966</v>
+        <v>0.4311881091539595</v>
       </c>
       <c r="AB47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.32972624592924454</v>
+        <v>0.32972624592924443</v>
       </c>
       <c r="AC47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.24338234053345054</v>
+        <v>0.24338234053345043</v>
       </c>
       <c r="AD47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.17597619149950278</v>
+        <v>0.17597619149950272</v>
       </c>
       <c r="AE47">
         <f t="shared" ca="1" si="37"/>
-        <v>0.12570998427570515</v>
+        <v>0.12570998427570509</v>
       </c>
       <c r="AF47">
         <f t="shared" ca="1" si="37"/>
-        <v>8.9099804029746571E-2</v>
+        <v>8.9099804029746529E-2</v>
       </c>
       <c r="AG47">
         <f t="shared" ca="1" si="37"/>
-        <v>6.2787313739461295E-2</v>
+        <v>6.2787313739461267E-2</v>
       </c>
       <c r="AH47">
         <f t="shared" ca="1" si="37"/>
-        <v>4.4038468873394424E-2</v>
+        <v>4.4038468873394396E-2</v>
       </c>
       <c r="AI47">
         <f t="shared" ca="1" si="37"/>
-        <v>9.3529999406370176E-2</v>
+        <v>9.3529999406370135E-2</v>
       </c>
     </row>
     <row r="48" spans="1:35">
@@ -10956,18 +10956,18 @@
       </c>
       <c r="B48" s="1">
         <f ca="1">f1_*re*phi_q1</f>
-        <v>27569.439422456111</v>
+        <v>27569.439422456104</v>
       </c>
       <c r="C48" s="20">
         <f ca="1">ye_1/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.60367371601208464</v>
+        <v>0.60367371601208453</v>
       </c>
       <c r="F48" t="s">
         <v>85</v>
       </c>
       <c r="G48" s="31">
         <f ca="1">G40/G54</f>
-        <v>2.0227764516670246</v>
+        <v>2.022776451667025</v>
       </c>
       <c r="H48" s="31">
         <f t="shared" ref="H48:I49" ca="1" si="38">H40/H54</f>
@@ -10975,7 +10975,7 @@
       </c>
       <c r="I48" s="31">
         <f ca="1">I54/I40</f>
-        <v>0.66147781371747894</v>
+        <v>0.66147781371747916</v>
       </c>
       <c r="J48" s="8" t="s">
         <v>77</v>
@@ -11002,7 +11002,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="39"/>
-        <v>5.8462088516989162E-2</v>
+        <v>5.8462088516989141E-2</v>
       </c>
       <c r="Q48">
         <f t="shared" ca="1" si="39"/>
@@ -11010,75 +11010,75 @@
       </c>
       <c r="R48">
         <f t="shared" ca="1" si="39"/>
-        <v>2.1578810791899907</v>
+        <v>2.1578810791899898</v>
       </c>
       <c r="S48">
         <f t="shared" ca="1" si="39"/>
-        <v>2.4166663530975065</v>
+        <v>2.4166663530975061</v>
       </c>
       <c r="T48">
         <f t="shared" ca="1" si="39"/>
-        <v>2.3175610201293479</v>
+        <v>2.3175610201293475</v>
       </c>
       <c r="U48">
         <f t="shared" ca="1" si="39"/>
-        <v>2.0967421509626676</v>
+        <v>2.0967421509626667</v>
       </c>
       <c r="V48">
         <f t="shared" ca="1" si="39"/>
-        <v>1.8407857445461613</v>
+        <v>1.8407857445461604</v>
       </c>
       <c r="W48">
         <f t="shared" ca="1" si="39"/>
-        <v>1.5792693680298344</v>
+        <v>1.5792693680298338</v>
       </c>
       <c r="X48">
         <f t="shared" ca="1" si="39"/>
-        <v>1.3211927108012875</v>
+        <v>1.3211927108012866</v>
       </c>
       <c r="Y48">
         <f t="shared" ca="1" si="39"/>
-        <v>1.06735804987266</v>
+        <v>1.0673580498726596</v>
       </c>
       <c r="Z48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.91258246963018663</v>
+        <v>0.9125824696301863</v>
       </c>
       <c r="AA48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.73523602218617612</v>
+        <v>0.73523602218617579</v>
       </c>
       <c r="AB48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.56222935725910284</v>
+        <v>0.56222935725910261</v>
       </c>
       <c r="AC48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.41500092448115755</v>
+        <v>0.41500092448115733</v>
       </c>
       <c r="AD48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.30006401450038472</v>
+        <v>0.30006401450038456</v>
       </c>
       <c r="AE48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.21435310210503614</v>
+        <v>0.21435310210503605</v>
       </c>
       <c r="AF48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.15192762532560464</v>
+        <v>0.15192762532560455</v>
       </c>
       <c r="AG48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.10706114991931252</v>
+        <v>0.10706114991931247</v>
       </c>
       <c r="AH48">
         <f t="shared" ca="1" si="39"/>
-        <v>7.5091747639272566E-2</v>
+        <v>7.5091747639272524E-2</v>
       </c>
       <c r="AI48">
         <f t="shared" ca="1" si="39"/>
-        <v>0.15948172794825674</v>
+        <v>0.15948172794825666</v>
       </c>
     </row>
     <row r="49" spans="1:47">
@@ -11087,11 +11087,11 @@
       </c>
       <c r="B49" s="1">
         <f ca="1">f2_*re*phi_q2</f>
-        <v>10281.832414628601</v>
+        <v>10281.832414628605</v>
       </c>
       <c r="C49" s="20">
         <f ca="1">ye_2/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.22513595166163133</v>
+        <v>0.22513595166163144</v>
       </c>
       <c r="F49" t="s">
         <v>86</v>
@@ -11102,11 +11102,11 @@
       </c>
       <c r="H49" s="31">
         <f t="shared" ca="1" si="38"/>
-        <v>1.5117665011015862</v>
+        <v>1.5117665011015855</v>
       </c>
       <c r="I49" s="31">
         <f t="shared" ca="1" si="38"/>
-        <v>1.0000000000000002</v>
+        <v>0.99999999999999944</v>
       </c>
       <c r="AL49" s="31"/>
       <c r="AM49" s="31"/>
@@ -11122,11 +11122,11 @@
       </c>
       <c r="B50" s="1">
         <f ca="1">f3_*re*phi_q3</f>
-        <v>7818.1662901572099</v>
+        <v>7818.1662901572081</v>
       </c>
       <c r="C50" s="20">
         <f ca="1">ye_3/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.17119033232628397</v>
+        <v>0.171190332326284</v>
       </c>
       <c r="AL50" s="31"/>
       <c r="AM50" s="31"/>
@@ -11142,7 +11142,7 @@
       </c>
       <c r="B51" s="1">
         <f ca="1">SUM(B48:B50)</f>
-        <v>45669.438127241927</v>
+        <v>45669.438127241912</v>
       </c>
       <c r="G51" t="s">
         <v>70</v>
@@ -11168,7 +11168,7 @@
       </c>
       <c r="I52" s="11">
         <f ca="1">I41^0.5</f>
-        <v>570.00143617758886</v>
+        <v>570.00143617758874</v>
       </c>
       <c r="AL52" s="31"/>
       <c r="AM52" s="31"/>
@@ -11184,7 +11184,7 @@
       </c>
       <c r="B53" s="35">
         <f ca="1">f1_*phi_q1</f>
-        <v>1.3676875188894202</v>
+        <v>1.36768751888942</v>
       </c>
       <c r="C53">
         <f ca="1">AVERAGE(B53:B55)/B53</f>
@@ -11192,15 +11192,15 @@
       </c>
       <c r="G53">
         <f ca="1">G$52*$J53</f>
-        <v>1416566.9922551173</v>
+        <v>1416566.992255117</v>
       </c>
       <c r="H53">
         <f t="shared" ref="G53:I55" ca="1" si="40">H$52*$J53</f>
-        <v>684452.374384981</v>
+        <v>684452.37438498088</v>
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="40"/>
-        <v>678413.54279688757</v>
+        <v>678413.54279688722</v>
       </c>
       <c r="J53">
         <f t="array" aca="1" ref="J53:J55" ca="1">TRANSPOSE(G52:I52)</f>
@@ -11218,11 +11218,11 @@
       </c>
       <c r="B54" s="35">
         <f ca="1">f2_*phi_q2</f>
-        <v>0.51006963360111091</v>
+        <v>0.51006963360111102</v>
       </c>
       <c r="C54">
         <f ca="1">AVERAGE(B53:B55)/B54</f>
-        <v>1.4805868670602975</v>
+        <v>1.4805868670602966</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="40"/>
@@ -11234,7 +11234,7 @@
       </c>
       <c r="I54">
         <f ca="1">I$52*$J54</f>
-        <v>327793.71729044965</v>
+        <v>327793.7172904496</v>
       </c>
       <c r="J54">
         <f ca="1"/>
@@ -11253,27 +11253,27 @@
       </c>
       <c r="B55" s="35">
         <f ca="1">f3_*phi_q3</f>
-        <v>0.38785004989765642</v>
+        <v>0.38785004989765637</v>
       </c>
       <c r="C55">
         <f ca="1">AVERAGE(B53:B55)/B55</f>
-        <v>1.9471504541390183</v>
+        <v>1.9471504541390179</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="40"/>
-        <v>678413.54279688746</v>
+        <v>678413.54279688722</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="40"/>
-        <v>327793.71729044965</v>
+        <v>327793.7172904496</v>
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="40"/>
-        <v>324901.6372445139</v>
+        <v>324901.63724451378</v>
       </c>
       <c r="J55">
         <f ca="1"/>
-        <v>570.00143617758886</v>
+        <v>570.00143617758874</v>
       </c>
       <c r="S55" s="33"/>
       <c r="AL55" s="31"/>
@@ -11289,11 +11289,11 @@
       </c>
       <c r="B56" s="34">
         <f ca="1">phi_t1*f1_</f>
-        <v>4.166029612269001E-2</v>
+        <v>4.1660296122690003E-2</v>
       </c>
       <c r="C56">
         <f ca="1">AVERAGE(B56:B58)/B56</f>
-        <v>1.2005261151143429</v>
+        <v>1.2005261151143427</v>
       </c>
       <c r="AL56" s="31"/>
       <c r="AM56" s="31"/>
@@ -11308,23 +11308,23 @@
       </c>
       <c r="B57" s="34">
         <f ca="1">phi_t2*f2_</f>
-        <v>8.0962637009346347E-2</v>
+        <v>8.0962637009346389E-2</v>
       </c>
       <c r="C57">
         <f ca="1">AVERAGE(B56:B58)/B57</f>
-        <v>0.61774511436568558</v>
+        <v>0.61774511436568547</v>
       </c>
       <c r="G57">
         <f t="array" aca="1" ref="G57:I59" ca="1">MMULT($G$52:$I$52,TRANSPOSE($G$52:$I$52))</f>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="H57">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="I57">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="AL57" s="31"/>
       <c r="AM57" s="31"/>
@@ -11339,23 +11339,23 @@
       </c>
       <c r="B58" s="34">
         <f ca="1">phi_t3*f3_</f>
-        <v>2.741988724402207E-2</v>
+        <v>2.7419887244022074E-2</v>
       </c>
       <c r="C58">
         <f ca="1">AVERAGE(B56:B58)/B58</f>
-        <v>1.8240145560624059</v>
+        <v>1.8240145560624064</v>
       </c>
       <c r="G58">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="H58">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="I58">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="AL58" s="31"/>
       <c r="AM58" s="31"/>
@@ -11366,15 +11366,15 @@
     <row r="59" spans="1:47">
       <c r="G59">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="H59">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="I59">
         <f ca="1"/>
-        <v>2072180.1704027865</v>
+        <v>2072180.1704027862</v>
       </c>
       <c r="AL59" s="31"/>
       <c r="AM59" s="31"/>
@@ -11402,7 +11402,7 @@
       </c>
       <c r="B61">
         <f ca="1">ypr2/mpr2_</f>
-        <v>6.3000620093714135</v>
+        <v>6.3000620093714117</v>
       </c>
       <c r="AL61" s="31"/>
       <c r="AM61" s="31"/>
@@ -11416,7 +11416,7 @@
       </c>
       <c r="B62">
         <f ca="1">ypr3/mpr3_</f>
-        <v>14.144844814495483</v>
+        <v>14.14484481449548</v>
       </c>
       <c r="AL62" s="31"/>
       <c r="AM62" s="31"/>
@@ -21629,14 +21629,14 @@
       </c>
       <c r="C4" s="22">
         <f ca="1">ypr1/SUM(ypr1,ypr2,ypr3)</f>
-        <v>0.60367371601208453</v>
+        <v>0.60367371601208464</v>
       </c>
       <c r="E4" s="49">
         <v>24977</v>
       </c>
       <c r="F4" s="49">
         <f ca="1">ye_1</f>
-        <v>27109.570776465567</v>
+        <v>27109.570776465585</v>
       </c>
       <c r="J4" t="s">
         <v>78</v>
@@ -21752,14 +21752,14 @@
       </c>
       <c r="C5" s="22">
         <f ca="1">ypr2/SUM(ypr1,ypr2,ypr3)</f>
-        <v>0.22513595166163144</v>
+        <v>0.22513595166163142</v>
       </c>
       <c r="E5" s="49">
         <v>9315</v>
       </c>
       <c r="F5" s="49">
         <f ca="1">ye_2</f>
-        <v>10110.327572677939</v>
+        <v>10110.327572677941</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
@@ -21875,14 +21875,14 @@
       </c>
       <c r="C6" s="22">
         <f ca="1">ypr3/SUM(ypr1,ypr2,ypr3)</f>
-        <v>0.171190332326284</v>
+        <v>0.17119033232628394</v>
       </c>
       <c r="E6" s="49">
         <v>7083</v>
       </c>
       <c r="F6" s="49">
         <f ca="1">ye_3</f>
-        <v>7687.756328210181</v>
+        <v>7687.7563282101819</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
@@ -21997,7 +21997,7 @@
       </c>
       <c r="C7" s="23">
         <f ca="1">spr</f>
-        <v>0.40000000000004887</v>
+        <v>0.40000000000004898</v>
       </c>
       <c r="J7" t="s">
         <v>7</v>
@@ -22048,59 +22048,59 @@
       </c>
       <c r="V7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.14428208091818298</v>
+        <v>0.14428208091818295</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>0.12014832604251621</v>
+        <v>0.12014832604251618</v>
       </c>
       <c r="X7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>9.9638536360132909E-2</v>
+        <v>9.9638536360132882E-2</v>
       </c>
       <c r="Y7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>8.1554130946726214E-2</v>
+        <v>8.1554130946726186E-2</v>
       </c>
       <c r="Z7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>6.4866782507165224E-2</v>
+        <v>6.4866782507165197E-2</v>
       </c>
       <c r="AA7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>4.9223245589603767E-2</v>
+        <v>4.9223245589603747E-2</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5563097092698698E-2</v>
+        <v>3.5563097092698677E-2</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>2.482151206164971E-2</v>
+        <v>2.4821512061649696E-2</v>
       </c>
       <c r="AD7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.7012954562218952E-2</v>
+        <v>1.7012954562218942E-2</v>
       </c>
       <c r="AE7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1567024685752244E-2</v>
+        <v>1.1567024685752235E-2</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>7.8381840927252838E-3</v>
+        <v>7.8381840927252786E-3</v>
       </c>
       <c r="AG7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>5.3043363685660715E-3</v>
+        <v>5.3043363685660681E-3</v>
       </c>
       <c r="AH7" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>3.5877247293795607E-3</v>
+        <v>3.5877247293795581E-3</v>
       </c>
       <c r="AI7" s="1">
         <f ca="1">AH7*EXP(-AH8)/(1-EXP(-AI8))</f>
-        <v>7.4923929050578235E-3</v>
+        <v>7.4923929050578182E-3</v>
       </c>
     </row>
     <row r="8" spans="1:35">
@@ -22112,7 +22112,7 @@
       </c>
       <c r="F8">
         <f ca="1">SUMXMY2(E4:E6,F4:F6)</f>
-        <v>5546134.2810069956</v>
+        <v>5546134.2810070775</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -22426,7 +22426,7 @@
       </c>
       <c r="C11" s="18">
         <f ca="1">mpr1_/SUM(mpr1_,mpr2_,mpr3_)</f>
-        <v>0.262677960461282</v>
+        <v>0.26267796046128206</v>
       </c>
       <c r="J11" t="s">
         <v>56</v>
@@ -22541,7 +22541,7 @@
       </c>
       <c r="C12" s="18">
         <f ca="1">mpr2_/SUM(mpr1_,mpr2_,mpr3_)</f>
-        <v>0.55724231251811152</v>
+        <v>0.5572423125181114</v>
       </c>
       <c r="J12" t="s">
         <v>100</v>
@@ -22657,7 +22657,7 @@
       </c>
       <c r="C13" s="18">
         <f ca="1">mpr3_/SUM(mpr1_,mpr2_,mpr3_)</f>
-        <v>0.18007972702060657</v>
+        <v>0.18007972702060651</v>
       </c>
       <c r="J13" t="s">
         <v>101</v>
@@ -22772,7 +22772,7 @@
       </c>
       <c r="C14" s="29">
         <f ca="1">spr</f>
-        <v>0.40000000000004887</v>
+        <v>0.40000000000004898</v>
       </c>
       <c r="J14" t="s">
         <v>102</v>
@@ -22885,7 +22885,7 @@
       </c>
       <c r="C15" s="26">
         <f ca="1">CHOOSE(C25,SUMXMY2(B14,C14),SUMXMY2(B7,C7))</f>
-        <v>2.3863042382935607E-27</v>
+        <v>2.3971634016919937E-27</v>
       </c>
     </row>
     <row r="17" spans="1:39">
@@ -23844,7 +23844,7 @@
       </c>
       <c r="E27" s="42">
         <f ca="1">f1_/(F4/(365*re*phib))</f>
-        <v>2035.3111123523527</v>
+        <v>2035.3111123523515</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>31</v>
@@ -23956,15 +23956,15 @@
       </c>
       <c r="B28" s="28">
         <f ca="1">fbar*C28</f>
-        <v>3.2154634114065231E-2</v>
+        <v>3.2154634114065217E-2</v>
       </c>
       <c r="C28" s="36">
         <f ca="1">CHOOSE(C$25,E37,E40,1)</f>
-        <v>0.355133929093567</v>
+        <v>0.35513392909356717</v>
       </c>
       <c r="E28" s="42">
         <f ca="1">f2_/(F5/(365*re*phib))</f>
-        <v>797.53843008718786</v>
+        <v>797.53843008718741</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>32</v>
@@ -24076,15 +24076,15 @@
       </c>
       <c r="B29" s="28">
         <f ca="1">fbar*C29</f>
-        <v>1.9443068089278967E-2</v>
+        <v>1.9443068089278964E-2</v>
       </c>
       <c r="C29" s="36">
         <f ca="1">CHOOSE(C$25,E38,E41,1)</f>
-        <v>0.21474021877173291</v>
+        <v>0.21474021877173294</v>
       </c>
       <c r="E29" s="42">
         <f ca="1">f3_/(F6/(365*re*phib))</f>
-        <v>634.21785061702701</v>
+        <v>634.21785061702678</v>
       </c>
     </row>
     <row r="30" spans="1:39">
@@ -24096,7 +24096,7 @@
       </c>
       <c r="C30" s="36">
         <f ca="1">AVERAGE(C27:C29)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G30" t="s">
         <v>58</v>
@@ -24118,7 +24118,7 @@
       </c>
       <c r="G31">
         <f ca="1">SUMPRODUCT(dlz1_,wa,ma)</f>
-        <v>-19.509994924445799</v>
+        <v>-19.509994924445813</v>
       </c>
       <c r="H31">
         <f ca="1">Ro/(reck-1)*phie/phif^2*dphif</f>
@@ -24176,55 +24176,55 @@
       </c>
       <c r="W31">
         <f t="shared" ca="1" si="23"/>
-        <v>-4.1211687571712317E-3</v>
+        <v>-4.1211687571712308E-3</v>
       </c>
       <c r="X31">
         <f t="shared" ca="1" si="23"/>
-        <v>-8.5036844626700733E-3</v>
+        <v>-8.5036844626700716E-3</v>
       </c>
       <c r="Y31">
         <f t="shared" ca="1" si="23"/>
-        <v>-1.6703229250975213E-2</v>
+        <v>-1.6703229250975209E-2</v>
       </c>
       <c r="Z31">
         <f t="shared" ca="1" si="23"/>
-        <v>-2.9664336652874483E-2</v>
+        <v>-2.9664336652874473E-2</v>
       </c>
       <c r="AA31">
         <f t="shared" ca="1" si="23"/>
-        <v>-4.484724029710864E-2</v>
+        <v>-4.4847240297108626E-2</v>
       </c>
       <c r="AB31">
         <f t="shared" ca="1" si="23"/>
-        <v>-5.6152592385630848E-2</v>
+        <v>-5.6152592385630834E-2</v>
       </c>
       <c r="AC31">
         <f t="shared" ca="1" si="23"/>
-        <v>-5.9729173259787605E-2</v>
+        <v>-5.9729173259787584E-2</v>
       </c>
       <c r="AD31">
         <f t="shared" ca="1" si="23"/>
-        <v>-5.6571206411371915E-2</v>
+        <v>-5.6571206411371894E-2</v>
       </c>
       <c r="AE31">
         <f t="shared" ca="1" si="23"/>
-        <v>-4.9611514728469114E-2</v>
+        <v>-4.9611514728469086E-2</v>
       </c>
       <c r="AF31">
         <f t="shared" ca="1" si="23"/>
-        <v>-4.133409489072816E-2</v>
+        <v>-4.1334094890728139E-2</v>
       </c>
       <c r="AG31">
         <f t="shared" ca="1" si="23"/>
-        <v>-3.3241229546014217E-2</v>
+        <v>-3.3241229546014196E-2</v>
       </c>
       <c r="AH31">
         <f t="shared" ca="1" si="23"/>
-        <v>-2.6061378984821082E-2</v>
+        <v>-2.6061378984821068E-2</v>
       </c>
       <c r="AI31">
         <f ca="1">(AH31*sa-AH$7*AH18*AH$10)/oa-AH$7*AH$10*flt1_*sa/oa^2</f>
-        <v>-7.7551409132707916E-2</v>
+        <v>-7.7551409132707874E-2</v>
       </c>
     </row>
     <row r="32" spans="1:39">
@@ -24235,11 +24235,11 @@
       <c r="C32" s="12"/>
       <c r="G32">
         <f ca="1">SUMPRODUCT(dlz2_,wa,ma)</f>
-        <v>-115.71746211086332</v>
+        <v>-115.71746211086329</v>
       </c>
       <c r="H32">
         <f ca="1">Ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-35818.425878766473</v>
+        <v>-35818.425878766437</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>53</v>
@@ -24337,11 +24337,11 @@
       </c>
       <c r="AH32">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.1585182095093416E-2</v>
+        <v>-3.1585182095093409E-2</v>
       </c>
       <c r="AI32">
         <f ca="1">(AH32*sa-AH$7*AH19*AH$10)/oa-AH$7*AH$10*flt2_*sa/oa^2</f>
-        <v>-7.3502948802619594E-2</v>
+        <v>-7.350294880261958E-2</v>
       </c>
     </row>
     <row r="33" spans="1:35">
@@ -24361,7 +24361,7 @@
       </c>
       <c r="H33">
         <f ca="1">Ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-31639.596220242136</v>
+        <v>-31639.596220242114</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>54</v>
@@ -24415,11 +24415,11 @@
       </c>
       <c r="W33">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.62106048891564858</v>
+        <v>-0.62106048891564847</v>
       </c>
       <c r="X33">
         <f t="shared" ca="1" si="25"/>
-        <v>-0.57695727798005425</v>
+        <v>-0.57695727798005414</v>
       </c>
       <c r="Y33">
         <f t="shared" ca="1" si="25"/>
@@ -24447,23 +24447,23 @@
       </c>
       <c r="AE33">
         <f t="shared" ca="1" si="25"/>
-        <v>-9.8783707215243627E-2</v>
+        <v>-9.8783707215243613E-2</v>
       </c>
       <c r="AF33">
         <f t="shared" ca="1" si="25"/>
-        <v>-7.120962388105323E-2</v>
+        <v>-7.1209623881053216E-2</v>
       </c>
       <c r="AG33">
         <f t="shared" ca="1" si="25"/>
-        <v>-5.1114806826933208E-2</v>
+        <v>-5.1114806826933201E-2</v>
       </c>
       <c r="AH33">
         <f t="shared" ca="1" si="25"/>
-        <v>-3.6561292832894235E-2</v>
+        <v>-3.6561292832894228E-2</v>
       </c>
       <c r="AI33">
         <f ca="1">(AH33*sa-AH$7*AH20*AH$10)/oa-AH$7*AH$10*flt3_*sa/oa^2</f>
-        <v>-8.9215997868592509E-2</v>
+        <v>-8.9215997868592495E-2</v>
       </c>
     </row>
     <row r="34" spans="1:35">
@@ -24485,7 +24485,7 @@
       </c>
       <c r="B35" s="1">
         <f ca="1">SUMPRODUCT(lz,wa,ma)</f>
-        <v>17.137594381884188</v>
+        <v>17.137594381884185</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="1">
@@ -24610,15 +24610,15 @@
       </c>
       <c r="B36" s="1">
         <f ca="1">SUMPRODUCT(lz,ta1_)</f>
-        <v>0.18550030825567762</v>
+        <v>0.18550030825567754</v>
       </c>
       <c r="C36" s="29">
         <f ca="1">B11/(phi_t1/SUM(B$36:B$38))</f>
-        <v>6.4622941018092517</v>
+        <v>6.4622941018092552</v>
       </c>
       <c r="E36" s="38">
         <f ca="1">C36/AVERAGE(C$36:C$38)</f>
-        <v>2.461611056739371</v>
+        <v>2.4616110567393714</v>
       </c>
       <c r="G36" s="1">
         <f ca="1">SUM(dqa21_)</f>
@@ -24626,7 +24626,7 @@
       </c>
       <c r="H36" s="1">
         <f ca="1">SUM(dqa22_)</f>
-        <v>62.21831984735487</v>
+        <v>62.218319847354877</v>
       </c>
       <c r="I36" s="11">
         <f ca="1">SUM(dqa23_)</f>
@@ -24750,7 +24750,7 @@
       </c>
       <c r="E37" s="38">
         <f ca="1">C37/AVERAGE(C$36:C$38)</f>
-        <v>0.32955255026974611</v>
+        <v>0.329552550269746</v>
       </c>
       <c r="G37" s="1">
         <f ca="1">SUM(dqa31_)</f>
@@ -24882,7 +24882,7 @@
       </c>
       <c r="E38" s="38">
         <f ca="1">C38/AVERAGE(C$36:C$38)</f>
-        <v>0.20883639299088319</v>
+        <v>0.20883639299088311</v>
       </c>
       <c r="G38" t="s">
         <v>69</v>
@@ -24936,7 +24936,7 @@
       </c>
       <c r="V38">
         <f t="shared" ca="1" si="29"/>
-        <v>-2.9985501473822479E-3</v>
+        <v>-2.9985501473822444E-3</v>
       </c>
       <c r="W38">
         <f t="shared" ca="1" si="29"/>
@@ -24997,11 +24997,11 @@
       </c>
       <c r="B39" s="1">
         <f ca="1">SUMPRODUCT(lz,qa1_)</f>
-        <v>6.1122543488962551</v>
+        <v>6.1122543488962506</v>
       </c>
       <c r="C39" s="23">
         <f ca="1">B4/(phi_q1/SUM(B$39:B$41))</f>
-        <v>4.0815336481522424</v>
+        <v>4.0815336481522451</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="39">
@@ -25010,7 +25010,7 @@
       </c>
       <c r="G39" s="1">
         <f ca="1">re*phi_q1+f1_*phi_q1*$H31+f1_*re*G35</f>
-        <v>1382554.0938899997</v>
+        <v>1382554.0938899994</v>
       </c>
       <c r="H39" s="1">
         <f ca="1">re*phi_q1+f1_*phi_q1*$H32+f1_*re*H35</f>
@@ -25018,7 +25018,7 @@
       </c>
       <c r="I39" s="1">
         <f ca="1">re*phi_q1+f1_*phi_q1*$H33+f1_*re*I35</f>
-        <v>1350166.8690472962</v>
+        <v>1350166.869047296</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>66</v>
@@ -25069,23 +25069,23 @@
       </c>
       <c r="V39">
         <f t="shared" ca="1" si="30"/>
-        <v>-1.1241572316004596E-2</v>
+        <v>-1.1241572316004592E-2</v>
       </c>
       <c r="W39">
         <f t="shared" ca="1" si="30"/>
-        <v>1.1115902069305267E-2</v>
+        <v>1.1115902069305274E-2</v>
       </c>
       <c r="X39">
         <f t="shared" ca="1" si="30"/>
-        <v>0.23864215142978726</v>
+        <v>0.23864215142978729</v>
       </c>
       <c r="Y39">
         <f t="shared" ca="1" si="30"/>
-        <v>1.4718481462026332</v>
+        <v>1.4718481462026334</v>
       </c>
       <c r="Z39">
         <f t="shared" ca="1" si="30"/>
-        <v>5.504788736800335</v>
+        <v>5.5047887368003359</v>
       </c>
       <c r="AA39">
         <f t="shared" ca="1" si="30"/>
@@ -25139,7 +25139,7 @@
       <c r="D40" s="21"/>
       <c r="E40" s="39">
         <f ca="1">C40/AVERAGE(C$39:C$41)</f>
-        <v>0.35513392909356717</v>
+        <v>0.355133929093567</v>
       </c>
       <c r="G40" s="1">
         <f ca="1">re*phi_q1+f1_*phi_q1*$H32+f1_*re*G36</f>
@@ -25202,11 +25202,11 @@
       </c>
       <c r="V40">
         <f t="shared" ca="1" si="31"/>
-        <v>-2.9985501473822479E-3</v>
+        <v>-2.9985501473822444E-3</v>
       </c>
       <c r="W40">
         <f t="shared" ca="1" si="31"/>
-        <v>2.8197407261281577E-2</v>
+        <v>2.8197407261281584E-2</v>
       </c>
       <c r="X40">
         <f t="shared" ca="1" si="31"/>
@@ -25263,24 +25263,24 @@
       </c>
       <c r="B41" s="1">
         <f ca="1">SUMPRODUCT(lz,qa3_)</f>
-        <v>19.615246063682058</v>
+        <v>19.615246063682054</v>
       </c>
       <c r="C41" s="23">
         <f ca="1">B6/(phi_q3/SUM(B$39:B$41))</f>
-        <v>0.36066832825077072</v>
+        <v>0.36066832825077083</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="39">
         <f ca="1">C41/AVERAGE(C$39:C$41)</f>
-        <v>0.21474021877173294</v>
+        <v>0.21474021877173291</v>
       </c>
       <c r="G41" s="1">
         <f ca="1">re*phi_q1+f1_*phi_q1*$H33+f1_*re*G37</f>
-        <v>1350166.8690472962</v>
+        <v>1350166.869047296</v>
       </c>
       <c r="H41" s="1">
         <f ca="1">re*phi_q3+f3_*phi_q3*$H33+f3_*re*H37</f>
-        <v>494457.85510086227</v>
+        <v>494457.85510086216</v>
       </c>
       <c r="I41" s="1">
         <f ca="1">re*phi_q3+f1_*phi_q3*$H33+f3_*re*I37</f>
@@ -25343,7 +25343,7 @@
       </c>
       <c r="X41">
         <f t="shared" ca="1" si="32"/>
-        <v>9.0538854692959303E-2</v>
+        <v>9.0538854692959442E-2</v>
       </c>
       <c r="Y41">
         <f t="shared" ca="1" si="32"/>
@@ -25396,7 +25396,7 @@
       </c>
       <c r="B42" s="1">
         <f ca="1">SUMPRODUCT(lz/SUM(lz),len,ta1_)</f>
-        <v>4.4644369117528306</v>
+        <v>4.4644369117528289</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>68</v>
@@ -25447,11 +25447,11 @@
       </c>
       <c r="V42">
         <f t="shared" ca="1" si="33"/>
-        <v>-1.1241572316004599E-2</v>
+        <v>-1.1241572316004592E-2</v>
       </c>
       <c r="W42">
         <f t="shared" ca="1" si="33"/>
-        <v>1.1115902069305267E-2</v>
+        <v>1.1115902069305281E-2</v>
       </c>
       <c r="X42">
         <f t="shared" ca="1" si="33"/>
@@ -25459,7 +25459,7 @@
       </c>
       <c r="Y42">
         <f t="shared" ca="1" si="33"/>
-        <v>1.4718481462026332</v>
+        <v>1.4718481462026334</v>
       </c>
       <c r="Z42">
         <f t="shared" ca="1" si="33"/>
@@ -25625,7 +25625,7 @@
       </c>
       <c r="B46" s="1">
         <f ca="1">phif/phie</f>
-        <v>0.40000000000004898</v>
+        <v>0.40000000000004887</v>
       </c>
       <c r="G46" s="32" t="s">
         <v>94</v>
@@ -25681,59 +25681,59 @@
       </c>
       <c r="V46">
         <f t="shared" ca="1" si="35"/>
-        <v>4.9490416670800348E-2</v>
+        <v>4.9490416670800341E-2</v>
       </c>
       <c r="W46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.11706098107776555</v>
+        <v>0.11706098107776552</v>
       </c>
       <c r="X46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.25826134078620833</v>
+        <v>0.25826134078620822</v>
       </c>
       <c r="Y46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.49994931120139474</v>
+        <v>0.49994931120139458</v>
       </c>
       <c r="Z46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.7788259774114149</v>
+        <v>0.77882597741141457</v>
       </c>
       <c r="AA46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.9260708810324525</v>
+        <v>0.92607088103245216</v>
       </c>
       <c r="AB46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.8724622842384343</v>
+        <v>0.87246228423843375</v>
       </c>
       <c r="AC46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.71087965315840496</v>
+        <v>0.71087965315840451</v>
       </c>
       <c r="AD46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.53801855561325784</v>
+        <v>0.53801855561325751</v>
       </c>
       <c r="AE46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.39323548198378855</v>
+        <v>0.39323548198378822</v>
       </c>
       <c r="AF46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.28253992555367591</v>
+        <v>0.28253992555367574</v>
       </c>
       <c r="AG46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.20109405287416454</v>
+        <v>0.2010940528741644</v>
       </c>
       <c r="AH46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.14225117141697999</v>
+        <v>0.14225117141697988</v>
       </c>
       <c r="AI46">
         <f t="shared" ca="1" si="35"/>
-        <v>0.30933283031448044</v>
+        <v>0.30933283031448022</v>
       </c>
     </row>
     <row r="47" spans="1:35" ht="19" thickTop="1">
@@ -25749,7 +25749,7 @@
       </c>
       <c r="G47" s="31">
         <f ca="1">G39/G53</f>
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="H47" s="31">
         <f ca="1">H53/H39</f>
@@ -25757,7 +25757,7 @@
       </c>
       <c r="I47" s="31">
         <f ca="1">I53/I39</f>
-        <v>0.49624956723582808</v>
+        <v>0.49624956723582819</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>76</v>
@@ -25808,59 +25808,59 @@
       </c>
       <c r="V47">
         <f t="shared" ca="1" si="36"/>
-        <v>1.0051017391512047</v>
+        <v>1.0051017391512045</v>
       </c>
       <c r="W47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.88083869933397863</v>
+        <v>0.8808386993339784</v>
       </c>
       <c r="X47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.75333510984092755</v>
+        <v>0.75333510984092733</v>
       </c>
       <c r="Y47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.62266336512349596</v>
+        <v>0.62266336512349574</v>
       </c>
       <c r="Z47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.53406528958272947</v>
+        <v>0.53406528958272925</v>
       </c>
       <c r="AA47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.43229328344515217</v>
+        <v>0.432293283445152</v>
       </c>
       <c r="AB47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.33256017230662865</v>
+        <v>0.33256017230662843</v>
       </c>
       <c r="AC47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.24716082184508928</v>
+        <v>0.24716082184508914</v>
       </c>
       <c r="AD47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.18001304593798786</v>
+        <v>0.18001304593798775</v>
       </c>
       <c r="AE47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.12955692151534318</v>
+        <v>0.12955692151534309</v>
       </c>
       <c r="AF47">
         <f t="shared" ca="1" si="36"/>
-        <v>9.2521290483820573E-2</v>
+        <v>9.2521290483820504E-2</v>
       </c>
       <c r="AG47">
         <f t="shared" ca="1" si="36"/>
-        <v>6.569376870240963E-2</v>
+        <v>6.5693768702409588E-2</v>
       </c>
       <c r="AH47">
         <f t="shared" ca="1" si="36"/>
-        <v>4.6427685438391646E-2</v>
+        <v>4.6427685438391611E-2</v>
       </c>
       <c r="AI47">
         <f t="shared" ca="1" si="36"/>
-        <v>0.10092334753918199</v>
+        <v>0.10092334753918192</v>
       </c>
     </row>
     <row r="48" spans="1:35">
@@ -25869,11 +25869,11 @@
       </c>
       <c r="B48" s="1">
         <f ca="1">f1_*re*phi_q1</f>
-        <v>27109.570776465585</v>
+        <v>27109.570776465567</v>
       </c>
       <c r="C48" s="20">
         <f ca="1">ye_1/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.60367371601208464</v>
+        <v>0.60367371601208442</v>
       </c>
       <c r="F48" t="s">
         <v>85</v>
@@ -25939,59 +25939,59 @@
       </c>
       <c r="V48">
         <f t="shared" ca="1" si="38"/>
-        <v>1.8229407311367145</v>
+        <v>1.8229407311367141</v>
       </c>
       <c r="W48">
         <f t="shared" ca="1" si="38"/>
-        <v>1.5656629762071608</v>
+        <v>1.5656629762071603</v>
       </c>
       <c r="X48">
         <f t="shared" ca="1" si="38"/>
-        <v>1.3115901999818793</v>
+        <v>1.3115901999818789</v>
       </c>
       <c r="Y48">
         <f t="shared" ca="1" si="38"/>
-        <v>1.0617281089516186</v>
+        <v>1.0617281089516184</v>
       </c>
       <c r="Z48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.91065600085996334</v>
+        <v>0.91065600085996301</v>
       </c>
       <c r="AA48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.73712049889698594</v>
+        <v>0.73712049889698561</v>
       </c>
       <c r="AB48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.56706159802048328</v>
+        <v>0.56706159802048295</v>
       </c>
       <c r="AC48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.42144376348922985</v>
+        <v>0.42144376348922963</v>
       </c>
       <c r="AD48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.30694741581986912</v>
+        <v>0.30694741581986895</v>
       </c>
       <c r="AE48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.22091266804302315</v>
+        <v>0.22091266804302298</v>
       </c>
       <c r="AF48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.15776173818041672</v>
+        <v>0.15776173818041664</v>
       </c>
       <c r="AG48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.11201706206126445</v>
+        <v>0.11201706206126438</v>
       </c>
       <c r="AH48">
         <f t="shared" ca="1" si="38"/>
-        <v>7.9165695983619527E-2</v>
+        <v>7.9165695983619472E-2</v>
       </c>
       <c r="AI48">
         <f t="shared" ca="1" si="38"/>
-        <v>0.17208842037878763</v>
+        <v>0.17208842037878749</v>
       </c>
     </row>
     <row r="49" spans="1:47">
@@ -26000,22 +26000,22 @@
       </c>
       <c r="B49" s="1">
         <f ca="1">f2_*re*phi_q2</f>
-        <v>10110.327572677941</v>
+        <v>10110.327572677936</v>
       </c>
       <c r="C49" s="20">
         <f ca="1">ye_2/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.22513595166163142</v>
+        <v>0.22513595166163139</v>
       </c>
       <c r="F49" t="s">
         <v>86</v>
       </c>
       <c r="G49" s="31">
         <f ca="1">G41/G55</f>
-        <v>2.0151151074450797</v>
+        <v>2.0151151074450793</v>
       </c>
       <c r="H49" s="31">
         <f t="shared" ca="1" si="37"/>
-        <v>1.4952115134815014</v>
+        <v>1.4952115134815009</v>
       </c>
       <c r="I49" s="31">
         <f t="shared" ca="1" si="37"/>
@@ -26035,11 +26035,11 @@
       </c>
       <c r="B50" s="1">
         <f ca="1">f3_*re*phi_q3</f>
-        <v>7687.7563282101819</v>
+        <v>7687.7563282101783</v>
       </c>
       <c r="C50" s="20">
         <f ca="1">ye_3/SUM(ye_1,ye_2,ye_3)</f>
-        <v>0.17119033232628394</v>
+        <v>0.17119033232628397</v>
       </c>
       <c r="AL50" s="31"/>
       <c r="AM50" s="31"/>
@@ -26055,7 +26055,7 @@
       </c>
       <c r="B51" s="1">
         <f ca="1">SUM(B48:B50)</f>
-        <v>44907.654677353712</v>
+        <v>44907.654677353683</v>
       </c>
       <c r="G51" t="s">
         <v>70</v>
@@ -26097,11 +26097,11 @@
       </c>
       <c r="B53" s="35">
         <f ca="1">f1_*phi_q1</f>
-        <v>1.3448739753088796</v>
+        <v>1.3448739753088788</v>
       </c>
       <c r="C53">
         <f ca="1">AVERAGE(B53:B55)/B53</f>
-        <v>0.55217466736063836</v>
+        <v>0.55217466736063847</v>
       </c>
       <c r="G53">
         <f ca="1">G$52*$J53</f>
@@ -26131,7 +26131,7 @@
       </c>
       <c r="B54" s="35">
         <f ca="1">f2_*phi_q2</f>
-        <v>0.50156147976146903</v>
+        <v>0.50156147976146881</v>
       </c>
       <c r="C54">
         <f ca="1">AVERAGE(B53:B55)/B54</f>
@@ -26166,11 +26166,11 @@
       </c>
       <c r="B55" s="35">
         <f ca="1">f3_*phi_q3</f>
-        <v>0.38138056480413146</v>
+        <v>0.38138056480413135</v>
       </c>
       <c r="C55">
         <f ca="1">AVERAGE(B53:B55)/B55</f>
-        <v>1.9471504541390188</v>
+        <v>1.9471504541390183</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="40"/>
@@ -26202,11 +26202,11 @@
       </c>
       <c r="B56" s="34">
         <f ca="1">phi_t1*f1_</f>
-        <v>4.0815470486742035E-2</v>
+        <v>4.0815470486742014E-2</v>
       </c>
       <c r="C56">
         <f ca="1">AVERAGE(B56:B58)/B56</f>
-        <v>1.2689809710261766</v>
+        <v>1.2689809710261768</v>
       </c>
       <c r="AL56" s="31"/>
       <c r="AM56" s="31"/>
@@ -26221,11 +26221,11 @@
       </c>
       <c r="B57" s="34">
         <f ca="1">phi_t2*f2_</f>
-        <v>8.6585517569142498E-2</v>
+        <v>8.6585517569142456E-2</v>
       </c>
       <c r="C57">
         <f ca="1">AVERAGE(B56:B58)/B57</f>
-        <v>0.59818381670810294</v>
+        <v>0.59818381670810283</v>
       </c>
       <c r="G57">
         <f t="array" aca="1" ref="G57:I59" ca="1">MMULT($G$52:$I$52,TRANSPOSE($G$52:$I$52))</f>
@@ -26252,11 +26252,11 @@
       </c>
       <c r="B58" s="34">
         <f ca="1">phi_t3*f3_</f>
-        <v>2.798117805758394E-2</v>
+        <v>2.7981178057583937E-2</v>
       </c>
       <c r="C58">
         <f ca="1">AVERAGE(B56:B58)/B58</f>
-        <v>1.8510319781592628</v>
+        <v>1.8510319781592621</v>
       </c>
       <c r="G58">
         <f ca="1"/>
@@ -26301,7 +26301,7 @@
       </c>
       <c r="B60">
         <f ca="1">ypr1/mpr1_</f>
-        <v>32.950103460052752</v>
+        <v>32.950103460052745</v>
       </c>
       <c r="AL60" s="31"/>
       <c r="AM60" s="31"/>
@@ -26329,7 +26329,7 @@
       </c>
       <c r="B62">
         <f ca="1">ypr3/mpr3_</f>
-        <v>13.629896640494131</v>
+        <v>13.629896640494129</v>
       </c>
       <c r="AL62" s="31"/>
       <c r="AM62" s="31"/>

</xml_diff>